<commit_message>
M3 Cord Production System #972 - Implements Wet Pick up #13
</commit_message>
<xml_diff>
--- a/05.Controls/M3.Cord.Controls/Resources/Excels/FMCS11_S8.xlsx
+++ b/05.Controls/M3.Cord.Controls/Resources/Excels/FMCS11_S8.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="72" windowWidth="11712" windowHeight="6456"/>
+    <workbookView xWindow="120" yWindow="72" windowWidth="11712" windowHeight="6456" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FM-CS-11" sheetId="4" r:id="rId1"/>
@@ -1852,7 +1852,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="307">
+  <cellXfs count="310">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1884,9 +1884,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1920,9 +1917,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2004,9 +1998,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2067,9 +2058,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2079,18 +2067,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2109,9 +2091,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2162,18 +2141,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2346,309 +2313,381 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2675,12 +2714,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2690,76 +2723,52 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3175,7 +3184,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AU48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
@@ -3203,1149 +3212,1149 @@
   <sheetData>
     <row r="1" spans="1:47" ht="6" customHeight="1" thickBot="1"/>
     <row r="2" spans="1:47" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A2" s="230" t="s">
+      <c r="A2" s="228" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="230"/>
-      <c r="C2" s="230"/>
-      <c r="D2" s="230"/>
-      <c r="E2" s="230"/>
-      <c r="F2" s="230"/>
-      <c r="G2" s="230"/>
-      <c r="H2" s="230"/>
-      <c r="I2" s="230"/>
-      <c r="J2" s="230"/>
-      <c r="K2" s="230"/>
-      <c r="L2" s="230"/>
-      <c r="M2" s="230"/>
-      <c r="N2" s="230"/>
-      <c r="O2" s="230"/>
-      <c r="P2" s="230"/>
-      <c r="Q2" s="230"/>
-      <c r="R2" s="231"/>
-      <c r="S2" s="218" t="s">
+      <c r="B2" s="228"/>
+      <c r="C2" s="228"/>
+      <c r="D2" s="228"/>
+      <c r="E2" s="228"/>
+      <c r="F2" s="228"/>
+      <c r="G2" s="228"/>
+      <c r="H2" s="228"/>
+      <c r="I2" s="228"/>
+      <c r="J2" s="228"/>
+      <c r="K2" s="228"/>
+      <c r="L2" s="228"/>
+      <c r="M2" s="228"/>
+      <c r="N2" s="228"/>
+      <c r="O2" s="228"/>
+      <c r="P2" s="228"/>
+      <c r="Q2" s="228"/>
+      <c r="R2" s="229"/>
+      <c r="S2" s="216" t="s">
         <v>155</v>
       </c>
-      <c r="T2" s="219"/>
-      <c r="U2" s="220"/>
-      <c r="V2" s="218" t="s">
+      <c r="T2" s="217"/>
+      <c r="U2" s="218"/>
+      <c r="V2" s="216" t="s">
         <v>156</v>
       </c>
-      <c r="W2" s="219"/>
-      <c r="X2" s="220"/>
-      <c r="Z2" s="221"/>
-      <c r="AA2" s="221"/>
-      <c r="AB2" s="221"/>
-      <c r="AC2" s="221"/>
-      <c r="AD2" s="221"/>
-      <c r="AE2" s="221"/>
-      <c r="AF2" s="221"/>
-      <c r="AG2" s="221"/>
-      <c r="AH2" s="221"/>
-      <c r="AI2" s="221"/>
-      <c r="AJ2" s="221"/>
-      <c r="AK2" s="221"/>
-      <c r="AL2" s="221"/>
-      <c r="AM2" s="221"/>
-      <c r="AN2" s="221"/>
-      <c r="AO2" s="221"/>
-      <c r="AP2" s="221"/>
-      <c r="AQ2" s="221"/>
-      <c r="AR2" s="221"/>
-      <c r="AS2" s="221"/>
-      <c r="AT2" s="221"/>
-      <c r="AU2" s="221"/>
+      <c r="W2" s="217"/>
+      <c r="X2" s="218"/>
+      <c r="Z2" s="219"/>
+      <c r="AA2" s="219"/>
+      <c r="AB2" s="219"/>
+      <c r="AC2" s="219"/>
+      <c r="AD2" s="219"/>
+      <c r="AE2" s="219"/>
+      <c r="AF2" s="219"/>
+      <c r="AG2" s="219"/>
+      <c r="AH2" s="219"/>
+      <c r="AI2" s="219"/>
+      <c r="AJ2" s="219"/>
+      <c r="AK2" s="219"/>
+      <c r="AL2" s="219"/>
+      <c r="AM2" s="219"/>
+      <c r="AN2" s="219"/>
+      <c r="AO2" s="219"/>
+      <c r="AP2" s="219"/>
+      <c r="AQ2" s="219"/>
+      <c r="AR2" s="219"/>
+      <c r="AS2" s="219"/>
+      <c r="AT2" s="219"/>
+      <c r="AU2" s="219"/>
     </row>
     <row r="3" spans="1:47" ht="39.75" customHeight="1" thickBot="1">
-      <c r="A3" s="232"/>
-      <c r="B3" s="232"/>
-      <c r="C3" s="232"/>
-      <c r="D3" s="232"/>
-      <c r="E3" s="232"/>
-      <c r="F3" s="232"/>
-      <c r="G3" s="232"/>
-      <c r="H3" s="232"/>
-      <c r="I3" s="232"/>
-      <c r="J3" s="232"/>
-      <c r="K3" s="232"/>
-      <c r="L3" s="232"/>
-      <c r="M3" s="232"/>
-      <c r="N3" s="232"/>
-      <c r="O3" s="232"/>
-      <c r="P3" s="232"/>
-      <c r="Q3" s="232"/>
-      <c r="R3" s="233"/>
-      <c r="S3" s="119"/>
-      <c r="T3" s="120"/>
-      <c r="U3" s="118"/>
-      <c r="V3" s="119"/>
-      <c r="W3" s="121"/>
-      <c r="X3" s="47"/>
+      <c r="A3" s="230"/>
+      <c r="B3" s="230"/>
+      <c r="C3" s="230"/>
+      <c r="D3" s="230"/>
+      <c r="E3" s="230"/>
+      <c r="F3" s="230"/>
+      <c r="G3" s="230"/>
+      <c r="H3" s="230"/>
+      <c r="I3" s="230"/>
+      <c r="J3" s="230"/>
+      <c r="K3" s="230"/>
+      <c r="L3" s="230"/>
+      <c r="M3" s="230"/>
+      <c r="N3" s="230"/>
+      <c r="O3" s="230"/>
+      <c r="P3" s="230"/>
+      <c r="Q3" s="230"/>
+      <c r="R3" s="231"/>
+      <c r="S3" s="108"/>
+      <c r="T3" s="109"/>
+      <c r="U3" s="107"/>
+      <c r="V3" s="108"/>
+      <c r="W3" s="110"/>
+      <c r="X3" s="45"/>
     </row>
     <row r="4" spans="1:47" s="2" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A4" s="222" t="s">
+      <c r="A4" s="220" t="s">
         <v>163</v>
       </c>
-      <c r="B4" s="223"/>
-      <c r="C4" s="224" t="s">
+      <c r="B4" s="221"/>
+      <c r="C4" s="222" t="s">
         <v>164</v>
       </c>
-      <c r="D4" s="225"/>
-      <c r="E4" s="223"/>
-      <c r="F4" s="224" t="s">
+      <c r="D4" s="223"/>
+      <c r="E4" s="221"/>
+      <c r="F4" s="222" t="s">
         <v>165</v>
       </c>
-      <c r="G4" s="225"/>
-      <c r="H4" s="225"/>
-      <c r="I4" s="223"/>
-      <c r="J4" s="225" t="s">
+      <c r="G4" s="223"/>
+      <c r="H4" s="223"/>
+      <c r="I4" s="221"/>
+      <c r="J4" s="223" t="s">
         <v>166</v>
       </c>
-      <c r="K4" s="225"/>
-      <c r="L4" s="225"/>
-      <c r="M4" s="223"/>
-      <c r="N4" s="225" t="s">
+      <c r="K4" s="223"/>
+      <c r="L4" s="223"/>
+      <c r="M4" s="221"/>
+      <c r="N4" s="223" t="s">
         <v>167</v>
       </c>
-      <c r="O4" s="225"/>
-      <c r="P4" s="225"/>
-      <c r="Q4" s="223"/>
-      <c r="R4" s="226" t="s">
+      <c r="O4" s="223"/>
+      <c r="P4" s="223"/>
+      <c r="Q4" s="221"/>
+      <c r="R4" s="224" t="s">
         <v>168</v>
       </c>
-      <c r="S4" s="227"/>
-      <c r="T4" s="226" t="s">
+      <c r="S4" s="225"/>
+      <c r="T4" s="224" t="s">
         <v>169</v>
       </c>
-      <c r="U4" s="228"/>
-      <c r="V4" s="228"/>
-      <c r="W4" s="228"/>
-      <c r="X4" s="229"/>
+      <c r="U4" s="226"/>
+      <c r="V4" s="226"/>
+      <c r="W4" s="226"/>
+      <c r="X4" s="227"/>
     </row>
     <row r="5" spans="1:47" s="3" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A5" s="254"/>
-      <c r="B5" s="236"/>
-      <c r="C5" s="234"/>
-      <c r="D5" s="235"/>
-      <c r="E5" s="236"/>
-      <c r="F5" s="240"/>
-      <c r="G5" s="241"/>
-      <c r="H5" s="241"/>
-      <c r="I5" s="242"/>
-      <c r="J5" s="167" t="s">
+      <c r="A5" s="158"/>
+      <c r="B5" s="159"/>
+      <c r="C5" s="185"/>
+      <c r="D5" s="186"/>
+      <c r="E5" s="159"/>
+      <c r="F5" s="190"/>
+      <c r="G5" s="191"/>
+      <c r="H5" s="191"/>
+      <c r="I5" s="192"/>
+      <c r="J5" s="205" t="s">
         <v>140</v>
       </c>
-      <c r="K5" s="252"/>
-      <c r="L5" s="252"/>
-      <c r="M5" s="253"/>
-      <c r="N5" s="167" t="s">
+      <c r="K5" s="206"/>
+      <c r="L5" s="206"/>
+      <c r="M5" s="207"/>
+      <c r="N5" s="205" t="s">
         <v>140</v>
       </c>
-      <c r="O5" s="252"/>
-      <c r="P5" s="252"/>
-      <c r="Q5" s="253"/>
-      <c r="R5" s="44" t="s">
+      <c r="O5" s="206"/>
+      <c r="P5" s="206"/>
+      <c r="Q5" s="207"/>
+      <c r="R5" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="S5" s="17" t="s">
+      <c r="S5" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="T5" s="250" t="s">
+      <c r="T5" s="199" t="s">
         <v>0</v>
       </c>
-      <c r="U5" s="251"/>
-      <c r="V5" s="167" t="s">
+      <c r="U5" s="200"/>
+      <c r="V5" s="205" t="s">
         <v>2</v>
       </c>
-      <c r="W5" s="168"/>
-      <c r="X5" s="169"/>
+      <c r="W5" s="266"/>
+      <c r="X5" s="267"/>
     </row>
     <row r="6" spans="1:47" s="3" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A6" s="255"/>
-      <c r="B6" s="239"/>
-      <c r="C6" s="237"/>
-      <c r="D6" s="238"/>
-      <c r="E6" s="239"/>
-      <c r="F6" s="243"/>
-      <c r="G6" s="244"/>
-      <c r="H6" s="244"/>
-      <c r="I6" s="245"/>
-      <c r="J6" s="261"/>
-      <c r="K6" s="262"/>
-      <c r="L6" s="262"/>
-      <c r="M6" s="263"/>
-      <c r="N6" s="249"/>
-      <c r="O6" s="296"/>
-      <c r="P6" s="296"/>
-      <c r="Q6" s="297"/>
-      <c r="R6" s="303"/>
-      <c r="S6" s="303"/>
-      <c r="T6" s="216" t="s">
+      <c r="A6" s="160"/>
+      <c r="B6" s="161"/>
+      <c r="C6" s="187"/>
+      <c r="D6" s="188"/>
+      <c r="E6" s="161"/>
+      <c r="F6" s="193"/>
+      <c r="G6" s="194"/>
+      <c r="H6" s="194"/>
+      <c r="I6" s="195"/>
+      <c r="J6" s="175"/>
+      <c r="K6" s="176"/>
+      <c r="L6" s="176"/>
+      <c r="M6" s="177"/>
+      <c r="N6" s="210"/>
+      <c r="O6" s="211"/>
+      <c r="P6" s="211"/>
+      <c r="Q6" s="212"/>
+      <c r="R6" s="208"/>
+      <c r="S6" s="208"/>
+      <c r="T6" s="201" t="s">
         <v>1</v>
       </c>
-      <c r="U6" s="217"/>
-      <c r="V6" s="170" t="s">
+      <c r="U6" s="202"/>
+      <c r="V6" s="168" t="s">
         <v>67</v>
       </c>
-      <c r="W6" s="171"/>
-      <c r="X6" s="172"/>
+      <c r="W6" s="189"/>
+      <c r="X6" s="268"/>
     </row>
     <row r="7" spans="1:47" s="3" customFormat="1" ht="21" customHeight="1">
-      <c r="A7" s="197"/>
-      <c r="B7" s="198"/>
-      <c r="C7" s="170"/>
-      <c r="D7" s="171"/>
-      <c r="E7" s="198"/>
-      <c r="F7" s="246"/>
-      <c r="G7" s="247"/>
-      <c r="H7" s="247"/>
-      <c r="I7" s="248"/>
-      <c r="J7" s="264"/>
-      <c r="K7" s="265"/>
-      <c r="L7" s="265"/>
-      <c r="M7" s="266"/>
-      <c r="N7" s="298"/>
-      <c r="O7" s="299"/>
-      <c r="P7" s="299"/>
-      <c r="Q7" s="300"/>
-      <c r="R7" s="304"/>
-      <c r="S7" s="304"/>
-      <c r="T7" s="213" t="s">
+      <c r="A7" s="162"/>
+      <c r="B7" s="163"/>
+      <c r="C7" s="168"/>
+      <c r="D7" s="189"/>
+      <c r="E7" s="163"/>
+      <c r="F7" s="196"/>
+      <c r="G7" s="197"/>
+      <c r="H7" s="197"/>
+      <c r="I7" s="198"/>
+      <c r="J7" s="178"/>
+      <c r="K7" s="179"/>
+      <c r="L7" s="179"/>
+      <c r="M7" s="180"/>
+      <c r="N7" s="213"/>
+      <c r="O7" s="214"/>
+      <c r="P7" s="214"/>
+      <c r="Q7" s="215"/>
+      <c r="R7" s="209"/>
+      <c r="S7" s="209"/>
+      <c r="T7" s="203" t="s">
         <v>3</v>
       </c>
-      <c r="U7" s="214"/>
+      <c r="U7" s="204"/>
       <c r="V7" s="173"/>
       <c r="W7" s="174"/>
-      <c r="X7" s="175"/>
+      <c r="X7" s="269"/>
     </row>
     <row r="8" spans="1:47" s="3" customFormat="1" ht="19.8">
-      <c r="A8" s="260" t="s">
+      <c r="A8" s="171" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="215"/>
+      <c r="B8" s="172"/>
       <c r="C8" s="173" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="174"/>
-      <c r="E8" s="215"/>
+      <c r="E8" s="172"/>
       <c r="F8" s="173" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="215"/>
+      <c r="G8" s="172"/>
       <c r="H8" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="215"/>
+      <c r="I8" s="172"/>
       <c r="J8" s="174" t="s">
         <v>19</v>
       </c>
       <c r="K8" s="174"/>
       <c r="L8" s="174"/>
-      <c r="M8" s="215"/>
+      <c r="M8" s="172"/>
       <c r="N8" s="174" t="s">
         <v>19</v>
       </c>
       <c r="O8" s="174"/>
       <c r="P8" s="174"/>
-      <c r="Q8" s="215"/>
-      <c r="R8" s="268" t="s">
+      <c r="Q8" s="172"/>
+      <c r="R8" s="232" t="s">
         <v>7</v>
       </c>
-      <c r="S8" s="269"/>
-      <c r="T8" s="213" t="s">
+      <c r="S8" s="233"/>
+      <c r="T8" s="203" t="s">
         <v>4</v>
       </c>
-      <c r="U8" s="214"/>
+      <c r="U8" s="204"/>
       <c r="V8" s="173"/>
       <c r="W8" s="174"/>
-      <c r="X8" s="175"/>
+      <c r="X8" s="269"/>
     </row>
     <row r="9" spans="1:47" s="3" customFormat="1" ht="21" customHeight="1">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="257"/>
-      <c r="D9" s="210"/>
-      <c r="E9" s="196"/>
-      <c r="F9" s="206"/>
-      <c r="G9" s="207"/>
-      <c r="H9" s="210"/>
-      <c r="I9" s="196"/>
+      <c r="C9" s="166"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="167"/>
+      <c r="F9" s="245"/>
+      <c r="G9" s="246"/>
+      <c r="H9" s="181"/>
+      <c r="I9" s="167"/>
       <c r="J9" s="173" t="s">
         <v>17</v>
       </c>
-      <c r="K9" s="215"/>
+      <c r="K9" s="172"/>
       <c r="L9" s="174" t="s">
         <v>18</v>
       </c>
-      <c r="M9" s="215"/>
+      <c r="M9" s="172"/>
       <c r="N9" s="173" t="s">
         <v>17</v>
       </c>
-      <c r="O9" s="215"/>
+      <c r="O9" s="172"/>
       <c r="P9" s="174" t="s">
         <v>18</v>
       </c>
-      <c r="Q9" s="215"/>
-      <c r="R9" s="216" t="s">
+      <c r="Q9" s="172"/>
+      <c r="R9" s="201" t="s">
         <v>8</v>
       </c>
-      <c r="S9" s="217"/>
-      <c r="T9" s="213" t="s">
+      <c r="S9" s="202"/>
+      <c r="T9" s="203" t="s">
         <v>5</v>
       </c>
-      <c r="U9" s="214"/>
+      <c r="U9" s="204"/>
       <c r="V9" s="173"/>
       <c r="W9" s="174"/>
-      <c r="X9" s="175"/>
+      <c r="X9" s="269"/>
     </row>
     <row r="10" spans="1:47" s="3" customFormat="1" ht="29.25" customHeight="1" thickBot="1">
-      <c r="A10" s="301"/>
-      <c r="B10" s="302"/>
-      <c r="C10" s="267"/>
-      <c r="D10" s="211"/>
-      <c r="E10" s="212"/>
-      <c r="F10" s="208"/>
-      <c r="G10" s="209"/>
-      <c r="H10" s="211"/>
-      <c r="I10" s="212"/>
-      <c r="J10" s="176"/>
-      <c r="K10" s="256"/>
-      <c r="L10" s="176"/>
-      <c r="M10" s="256"/>
-      <c r="N10" s="176"/>
-      <c r="O10" s="256"/>
-      <c r="P10" s="176"/>
-      <c r="Q10" s="256"/>
-      <c r="R10" s="305"/>
-      <c r="S10" s="306"/>
-      <c r="T10" s="200" t="s">
+      <c r="A10" s="156"/>
+      <c r="B10" s="157"/>
+      <c r="C10" s="182"/>
+      <c r="D10" s="183"/>
+      <c r="E10" s="184"/>
+      <c r="F10" s="247"/>
+      <c r="G10" s="248"/>
+      <c r="H10" s="183"/>
+      <c r="I10" s="184"/>
+      <c r="J10" s="164"/>
+      <c r="K10" s="165"/>
+      <c r="L10" s="164"/>
+      <c r="M10" s="165"/>
+      <c r="N10" s="164"/>
+      <c r="O10" s="165"/>
+      <c r="P10" s="164"/>
+      <c r="Q10" s="165"/>
+      <c r="R10" s="249"/>
+      <c r="S10" s="250"/>
+      <c r="T10" s="237" t="s">
         <v>20</v>
       </c>
-      <c r="U10" s="201"/>
-      <c r="V10" s="176"/>
-      <c r="W10" s="177"/>
-      <c r="X10" s="178"/>
+      <c r="U10" s="238"/>
+      <c r="V10" s="164"/>
+      <c r="W10" s="251"/>
+      <c r="X10" s="252"/>
     </row>
     <row r="11" spans="1:47" s="3" customFormat="1" ht="9.75" customHeight="1" thickBot="1"/>
     <row r="12" spans="1:47" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A12" s="146" t="s">
+      <c r="A12" s="135" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="148" t="s">
+      <c r="B12" s="137" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="187" t="s">
+      <c r="C12" s="239" t="s">
         <v>72</v>
       </c>
-      <c r="D12" s="202"/>
-      <c r="E12" s="188"/>
-      <c r="F12" s="187" t="s">
+      <c r="D12" s="240"/>
+      <c r="E12" s="241"/>
+      <c r="F12" s="239" t="s">
         <v>71</v>
       </c>
-      <c r="G12" s="188"/>
-      <c r="H12" s="153" t="s">
+      <c r="G12" s="241"/>
+      <c r="H12" s="142" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="153" t="s">
+      <c r="I12" s="142" t="s">
         <v>55</v>
       </c>
-      <c r="J12" s="153" t="s">
+      <c r="J12" s="142" t="s">
         <v>50</v>
       </c>
-      <c r="K12" s="153" t="s">
+      <c r="K12" s="142" t="s">
         <v>57</v>
       </c>
-      <c r="L12" s="148" t="s">
+      <c r="L12" s="137" t="s">
         <v>23</v>
       </c>
-      <c r="M12" s="187" t="s">
+      <c r="M12" s="239" t="s">
         <v>70</v>
       </c>
-      <c r="N12" s="202"/>
-      <c r="O12" s="188"/>
-      <c r="P12" s="187" t="s">
+      <c r="N12" s="240"/>
+      <c r="O12" s="241"/>
+      <c r="P12" s="239" t="s">
         <v>69</v>
       </c>
-      <c r="Q12" s="202"/>
-      <c r="R12" s="202"/>
-      <c r="S12" s="188"/>
-      <c r="T12" s="203" t="s">
+      <c r="Q12" s="240"/>
+      <c r="R12" s="240"/>
+      <c r="S12" s="241"/>
+      <c r="T12" s="242" t="s">
         <v>60</v>
       </c>
-      <c r="U12" s="204"/>
-      <c r="V12" s="205"/>
-      <c r="W12" s="151" t="s">
+      <c r="U12" s="243"/>
+      <c r="V12" s="244"/>
+      <c r="W12" s="140" t="s">
         <v>32</v>
       </c>
-      <c r="X12" s="152" t="s">
+      <c r="X12" s="141" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:47" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A13" s="147"/>
-      <c r="B13" s="149" t="s">
+      <c r="A13" s="136"/>
+      <c r="B13" s="138" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="28" t="s">
+      <c r="E13" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="28" t="s">
+      <c r="F13" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="G13" s="28" t="s">
+      <c r="G13" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="30" t="s">
+      <c r="H13" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="I13" s="30" t="s">
+      <c r="I13" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="J13" s="30" t="s">
+      <c r="J13" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="K13" s="30" t="s">
+      <c r="K13" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="L13" s="30" t="s">
+      <c r="L13" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="M13" s="30" t="s">
+      <c r="M13" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="N13" s="30" t="s">
+      <c r="N13" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="O13" s="30" t="s">
+      <c r="O13" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="P13" s="28" t="s">
+      <c r="P13" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="Q13" s="28" t="s">
+      <c r="Q13" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="R13" s="28" t="s">
+      <c r="R13" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="S13" s="30" t="s">
+      <c r="S13" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="T13" s="30" t="s">
+      <c r="T13" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="U13" s="30" t="s">
+      <c r="U13" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="V13" s="30" t="s">
+      <c r="V13" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="W13" s="30" t="s">
+      <c r="W13" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="X13" s="26" t="s">
+      <c r="X13" s="24" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:47" s="3" customFormat="1" ht="24.75" customHeight="1" thickBot="1">
-      <c r="A14" s="137" t="s">
+      <c r="A14" s="126" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="150" t="s">
+      <c r="B14" s="139" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="100" t="s">
+      <c r="C14" s="93" t="s">
         <v>135</v>
       </c>
-      <c r="D14" s="100" t="s">
+      <c r="D14" s="93" t="s">
         <v>136</v>
       </c>
-      <c r="E14" s="100" t="s">
+      <c r="E14" s="93" t="s">
         <v>137</v>
       </c>
-      <c r="F14" s="100" t="s">
+      <c r="F14" s="93" t="s">
         <v>135</v>
       </c>
-      <c r="G14" s="33" t="s">
+      <c r="G14" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="H14" s="31" t="s">
+      <c r="H14" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="I14" s="31" t="s">
+      <c r="I14" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="J14" s="31" t="s">
+      <c r="J14" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="K14" s="31" t="s">
+      <c r="K14" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="L14" s="31" t="s">
+      <c r="L14" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="M14" s="31" t="s">
+      <c r="M14" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="N14" s="31" t="s">
+      <c r="N14" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="O14" s="32" t="s">
+      <c r="O14" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="P14" s="31" t="s">
+      <c r="P14" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="Q14" s="31" t="s">
+      <c r="Q14" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="R14" s="33" t="s">
+      <c r="R14" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="S14" s="33" t="s">
+      <c r="S14" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="T14" s="31" t="s">
+      <c r="T14" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="U14" s="31" t="s">
+      <c r="U14" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="V14" s="31" t="s">
+      <c r="V14" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="W14" s="16"/>
+      <c r="W14" s="15"/>
       <c r="X14" s="6"/>
     </row>
     <row r="15" spans="1:47" s="3" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A15" s="147"/>
-      <c r="B15" s="149"/>
-      <c r="C15" s="157"/>
-      <c r="D15" s="157"/>
-      <c r="E15" s="157"/>
-      <c r="F15" s="157"/>
-      <c r="G15" s="157"/>
-      <c r="H15" s="157"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="30"/>
-      <c r="O15" s="155"/>
-      <c r="P15" s="30"/>
-      <c r="Q15" s="30"/>
-      <c r="R15" s="154"/>
-      <c r="S15" s="154"/>
-      <c r="T15" s="30"/>
-      <c r="U15" s="30"/>
-      <c r="V15" s="30"/>
-      <c r="W15" s="156"/>
-      <c r="X15" s="74"/>
+      <c r="A15" s="136"/>
+      <c r="B15" s="138"/>
+      <c r="C15" s="146"/>
+      <c r="D15" s="146"/>
+      <c r="E15" s="146"/>
+      <c r="F15" s="146"/>
+      <c r="G15" s="146"/>
+      <c r="H15" s="146"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="144"/>
+      <c r="P15" s="28"/>
+      <c r="Q15" s="28"/>
+      <c r="R15" s="143"/>
+      <c r="S15" s="143"/>
+      <c r="T15" s="28"/>
+      <c r="U15" s="28"/>
+      <c r="V15" s="28"/>
+      <c r="W15" s="145"/>
+      <c r="X15" s="70"/>
     </row>
     <row r="16" spans="1:47" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A16" s="161"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="165"/>
-      <c r="D16" s="165"/>
-      <c r="E16" s="165"/>
-      <c r="F16" s="165"/>
-      <c r="G16" s="165"/>
-      <c r="H16" s="166"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="15"/>
-      <c r="S16" s="15"/>
-      <c r="T16" s="15"/>
-      <c r="U16" s="15"/>
-      <c r="V16" s="15"/>
-      <c r="W16" s="15"/>
-      <c r="X16" s="139"/>
+      <c r="A16" s="150"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="154"/>
+      <c r="D16" s="154"/>
+      <c r="E16" s="154"/>
+      <c r="F16" s="154"/>
+      <c r="G16" s="154"/>
+      <c r="H16" s="155"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="14"/>
+      <c r="U16" s="14"/>
+      <c r="V16" s="14"/>
+      <c r="W16" s="14"/>
+      <c r="X16" s="128"/>
     </row>
     <row r="17" spans="1:24" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A17" s="164" t="s">
+      <c r="A17" s="153" t="s">
         <v>134</v>
       </c>
-      <c r="B17" s="162"/>
-      <c r="C17" s="162"/>
-      <c r="D17" s="162"/>
-      <c r="E17" s="162"/>
-      <c r="F17" s="162"/>
-      <c r="G17" s="162"/>
-      <c r="H17" s="162"/>
-      <c r="I17" s="162"/>
-      <c r="J17" s="162"/>
-      <c r="K17" s="162"/>
-      <c r="L17" s="162"/>
-      <c r="M17" s="162"/>
-      <c r="N17" s="162"/>
-      <c r="O17" s="162"/>
-      <c r="P17" s="162"/>
-      <c r="Q17" s="162"/>
-      <c r="R17" s="162"/>
-      <c r="S17" s="162"/>
-      <c r="T17" s="162"/>
-      <c r="U17" s="162"/>
-      <c r="V17" s="162"/>
-      <c r="W17" s="162"/>
-      <c r="X17" s="163"/>
+      <c r="B17" s="151"/>
+      <c r="C17" s="151"/>
+      <c r="D17" s="151"/>
+      <c r="E17" s="151"/>
+      <c r="F17" s="151"/>
+      <c r="G17" s="151"/>
+      <c r="H17" s="151"/>
+      <c r="I17" s="151"/>
+      <c r="J17" s="151"/>
+      <c r="K17" s="151"/>
+      <c r="L17" s="151"/>
+      <c r="M17" s="151"/>
+      <c r="N17" s="151"/>
+      <c r="O17" s="151"/>
+      <c r="P17" s="151"/>
+      <c r="Q17" s="151"/>
+      <c r="R17" s="151"/>
+      <c r="S17" s="151"/>
+      <c r="T17" s="151"/>
+      <c r="U17" s="151"/>
+      <c r="V17" s="151"/>
+      <c r="W17" s="151"/>
+      <c r="X17" s="152"/>
     </row>
     <row r="18" spans="1:24" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A18" s="158"/>
-      <c r="B18" s="159"/>
-      <c r="C18" s="159"/>
-      <c r="D18" s="159"/>
-      <c r="E18" s="159"/>
-      <c r="F18" s="159"/>
-      <c r="G18" s="159"/>
-      <c r="H18" s="159"/>
-      <c r="I18" s="159"/>
-      <c r="J18" s="159"/>
-      <c r="K18" s="159"/>
-      <c r="L18" s="159"/>
-      <c r="M18" s="159"/>
-      <c r="N18" s="159"/>
-      <c r="O18" s="159"/>
-      <c r="P18" s="159"/>
-      <c r="Q18" s="159"/>
-      <c r="R18" s="159"/>
-      <c r="S18" s="159"/>
-      <c r="T18" s="159"/>
-      <c r="U18" s="159"/>
-      <c r="V18" s="159"/>
-      <c r="W18" s="159"/>
-      <c r="X18" s="160"/>
+      <c r="A18" s="147"/>
+      <c r="B18" s="148"/>
+      <c r="C18" s="148"/>
+      <c r="D18" s="148"/>
+      <c r="E18" s="148"/>
+      <c r="F18" s="148"/>
+      <c r="G18" s="148"/>
+      <c r="H18" s="148"/>
+      <c r="I18" s="148"/>
+      <c r="J18" s="148"/>
+      <c r="K18" s="148"/>
+      <c r="L18" s="148"/>
+      <c r="M18" s="148"/>
+      <c r="N18" s="148"/>
+      <c r="O18" s="148"/>
+      <c r="P18" s="148"/>
+      <c r="Q18" s="148"/>
+      <c r="R18" s="148"/>
+      <c r="S18" s="148"/>
+      <c r="T18" s="148"/>
+      <c r="U18" s="148"/>
+      <c r="V18" s="148"/>
+      <c r="W18" s="148"/>
+      <c r="X18" s="149"/>
     </row>
     <row r="19" spans="1:24" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A19" s="90"/>
-      <c r="B19" s="91"/>
-      <c r="C19" s="91"/>
-      <c r="D19" s="91"/>
-      <c r="E19" s="91"/>
-      <c r="F19" s="91"/>
-      <c r="G19" s="91"/>
-      <c r="H19" s="91"/>
-      <c r="I19" s="91"/>
-      <c r="J19" s="91"/>
-      <c r="K19" s="91"/>
-      <c r="L19" s="91"/>
-      <c r="M19" s="91"/>
-      <c r="N19" s="91"/>
-      <c r="O19" s="91"/>
-      <c r="P19" s="91"/>
-      <c r="Q19" s="91"/>
-      <c r="R19" s="91"/>
-      <c r="S19" s="91"/>
-      <c r="T19" s="91"/>
-      <c r="U19" s="91"/>
-      <c r="V19" s="91"/>
-      <c r="W19" s="91"/>
-      <c r="X19" s="92"/>
+      <c r="A19" s="83"/>
+      <c r="B19" s="84"/>
+      <c r="C19" s="84"/>
+      <c r="D19" s="84"/>
+      <c r="E19" s="84"/>
+      <c r="F19" s="84"/>
+      <c r="G19" s="84"/>
+      <c r="H19" s="84"/>
+      <c r="I19" s="84"/>
+      <c r="J19" s="84"/>
+      <c r="K19" s="84"/>
+      <c r="L19" s="84"/>
+      <c r="M19" s="84"/>
+      <c r="N19" s="84"/>
+      <c r="O19" s="84"/>
+      <c r="P19" s="84"/>
+      <c r="Q19" s="84"/>
+      <c r="R19" s="84"/>
+      <c r="S19" s="84"/>
+      <c r="T19" s="84"/>
+      <c r="U19" s="84"/>
+      <c r="V19" s="84"/>
+      <c r="W19" s="84"/>
+      <c r="X19" s="85"/>
     </row>
     <row r="20" spans="1:24" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A20" s="90"/>
-      <c r="B20" s="91"/>
-      <c r="C20" s="91"/>
-      <c r="D20" s="91"/>
-      <c r="E20" s="91"/>
-      <c r="F20" s="91"/>
-      <c r="G20" s="91"/>
-      <c r="H20" s="91"/>
-      <c r="I20" s="91"/>
-      <c r="J20" s="91"/>
-      <c r="K20" s="91"/>
-      <c r="L20" s="91"/>
-      <c r="M20" s="91"/>
-      <c r="N20" s="91"/>
-      <c r="O20" s="91"/>
-      <c r="P20" s="91"/>
-      <c r="Q20" s="91"/>
-      <c r="R20" s="91"/>
-      <c r="S20" s="91"/>
-      <c r="T20" s="91"/>
-      <c r="U20" s="91"/>
-      <c r="V20" s="91"/>
-      <c r="W20" s="91"/>
-      <c r="X20" s="92"/>
+      <c r="A20" s="83"/>
+      <c r="B20" s="84"/>
+      <c r="C20" s="84"/>
+      <c r="D20" s="84"/>
+      <c r="E20" s="84"/>
+      <c r="F20" s="84"/>
+      <c r="G20" s="84"/>
+      <c r="H20" s="84"/>
+      <c r="I20" s="84"/>
+      <c r="J20" s="84"/>
+      <c r="K20" s="84"/>
+      <c r="L20" s="84"/>
+      <c r="M20" s="84"/>
+      <c r="N20" s="84"/>
+      <c r="O20" s="84"/>
+      <c r="P20" s="84"/>
+      <c r="Q20" s="84"/>
+      <c r="R20" s="84"/>
+      <c r="S20" s="84"/>
+      <c r="T20" s="84"/>
+      <c r="U20" s="84"/>
+      <c r="V20" s="84"/>
+      <c r="W20" s="84"/>
+      <c r="X20" s="85"/>
     </row>
     <row r="21" spans="1:24" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A21" s="90"/>
-      <c r="B21" s="91"/>
-      <c r="C21" s="91"/>
-      <c r="D21" s="91"/>
-      <c r="E21" s="91"/>
-      <c r="F21" s="91"/>
-      <c r="G21" s="91"/>
-      <c r="H21" s="91"/>
-      <c r="I21" s="91"/>
-      <c r="J21" s="91"/>
-      <c r="K21" s="91"/>
-      <c r="L21" s="91"/>
-      <c r="M21" s="91"/>
-      <c r="N21" s="91"/>
-      <c r="O21" s="91"/>
-      <c r="P21" s="91"/>
-      <c r="Q21" s="91"/>
-      <c r="R21" s="91"/>
-      <c r="S21" s="91"/>
-      <c r="T21" s="91"/>
-      <c r="U21" s="91"/>
-      <c r="V21" s="91"/>
-      <c r="W21" s="91"/>
-      <c r="X21" s="92"/>
+      <c r="A21" s="83"/>
+      <c r="B21" s="84"/>
+      <c r="C21" s="84"/>
+      <c r="D21" s="84"/>
+      <c r="E21" s="84"/>
+      <c r="F21" s="84"/>
+      <c r="G21" s="84"/>
+      <c r="H21" s="84"/>
+      <c r="I21" s="84"/>
+      <c r="J21" s="84"/>
+      <c r="K21" s="84"/>
+      <c r="L21" s="84"/>
+      <c r="M21" s="84"/>
+      <c r="N21" s="84"/>
+      <c r="O21" s="84"/>
+      <c r="P21" s="84"/>
+      <c r="Q21" s="84"/>
+      <c r="R21" s="84"/>
+      <c r="S21" s="84"/>
+      <c r="T21" s="84"/>
+      <c r="U21" s="84"/>
+      <c r="V21" s="84"/>
+      <c r="W21" s="84"/>
+      <c r="X21" s="85"/>
     </row>
     <row r="22" spans="1:24" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A22" s="90"/>
-      <c r="B22" s="91"/>
-      <c r="C22" s="91"/>
-      <c r="D22" s="91"/>
-      <c r="E22" s="91"/>
-      <c r="F22" s="91"/>
-      <c r="G22" s="91"/>
-      <c r="H22" s="91"/>
-      <c r="I22" s="91"/>
-      <c r="J22" s="91"/>
-      <c r="K22" s="91"/>
-      <c r="L22" s="91"/>
-      <c r="M22" s="91"/>
-      <c r="N22" s="91"/>
-      <c r="O22" s="91"/>
-      <c r="P22" s="91"/>
-      <c r="Q22" s="91"/>
-      <c r="R22" s="91"/>
-      <c r="S22" s="91"/>
-      <c r="T22" s="91"/>
-      <c r="U22" s="91"/>
-      <c r="V22" s="91"/>
-      <c r="W22" s="91"/>
-      <c r="X22" s="92"/>
+      <c r="A22" s="83"/>
+      <c r="B22" s="84"/>
+      <c r="C22" s="84"/>
+      <c r="D22" s="84"/>
+      <c r="E22" s="84"/>
+      <c r="F22" s="84"/>
+      <c r="G22" s="84"/>
+      <c r="H22" s="84"/>
+      <c r="I22" s="84"/>
+      <c r="J22" s="84"/>
+      <c r="K22" s="84"/>
+      <c r="L22" s="84"/>
+      <c r="M22" s="84"/>
+      <c r="N22" s="84"/>
+      <c r="O22" s="84"/>
+      <c r="P22" s="84"/>
+      <c r="Q22" s="84"/>
+      <c r="R22" s="84"/>
+      <c r="S22" s="84"/>
+      <c r="T22" s="84"/>
+      <c r="U22" s="84"/>
+      <c r="V22" s="84"/>
+      <c r="W22" s="84"/>
+      <c r="X22" s="85"/>
     </row>
     <row r="23" spans="1:24" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A23" s="90"/>
-      <c r="B23" s="91"/>
-      <c r="C23" s="91"/>
-      <c r="D23" s="91"/>
-      <c r="E23" s="91"/>
-      <c r="F23" s="91"/>
-      <c r="G23" s="91"/>
-      <c r="H23" s="91"/>
-      <c r="I23" s="91"/>
-      <c r="J23" s="91"/>
-      <c r="K23" s="91"/>
-      <c r="L23" s="91"/>
-      <c r="M23" s="91"/>
-      <c r="N23" s="91"/>
-      <c r="O23" s="91"/>
-      <c r="P23" s="91"/>
-      <c r="Q23" s="91"/>
-      <c r="R23" s="91"/>
-      <c r="S23" s="91"/>
-      <c r="T23" s="91"/>
-      <c r="U23" s="91"/>
-      <c r="V23" s="91"/>
-      <c r="W23" s="91"/>
-      <c r="X23" s="92"/>
+      <c r="A23" s="83"/>
+      <c r="B23" s="84"/>
+      <c r="C23" s="84"/>
+      <c r="D23" s="84"/>
+      <c r="E23" s="84"/>
+      <c r="F23" s="84"/>
+      <c r="G23" s="84"/>
+      <c r="H23" s="84"/>
+      <c r="I23" s="84"/>
+      <c r="J23" s="84"/>
+      <c r="K23" s="84"/>
+      <c r="L23" s="84"/>
+      <c r="M23" s="84"/>
+      <c r="N23" s="84"/>
+      <c r="O23" s="84"/>
+      <c r="P23" s="84"/>
+      <c r="Q23" s="84"/>
+      <c r="R23" s="84"/>
+      <c r="S23" s="84"/>
+      <c r="T23" s="84"/>
+      <c r="U23" s="84"/>
+      <c r="V23" s="84"/>
+      <c r="W23" s="84"/>
+      <c r="X23" s="85"/>
     </row>
     <row r="24" spans="1:24" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A24" s="90"/>
-      <c r="B24" s="91"/>
-      <c r="C24" s="91"/>
-      <c r="D24" s="91"/>
-      <c r="E24" s="91"/>
-      <c r="F24" s="91"/>
-      <c r="G24" s="91"/>
-      <c r="H24" s="91"/>
-      <c r="I24" s="91"/>
-      <c r="J24" s="91"/>
-      <c r="K24" s="91"/>
-      <c r="L24" s="91"/>
-      <c r="M24" s="91"/>
-      <c r="N24" s="91"/>
-      <c r="O24" s="91"/>
-      <c r="P24" s="91"/>
-      <c r="Q24" s="91"/>
-      <c r="R24" s="91"/>
-      <c r="S24" s="91"/>
-      <c r="T24" s="91"/>
-      <c r="U24" s="91"/>
-      <c r="V24" s="91"/>
-      <c r="W24" s="91"/>
-      <c r="X24" s="92"/>
+      <c r="A24" s="83"/>
+      <c r="B24" s="84"/>
+      <c r="C24" s="84"/>
+      <c r="D24" s="84"/>
+      <c r="E24" s="84"/>
+      <c r="F24" s="84"/>
+      <c r="G24" s="84"/>
+      <c r="H24" s="84"/>
+      <c r="I24" s="84"/>
+      <c r="J24" s="84"/>
+      <c r="K24" s="84"/>
+      <c r="L24" s="84"/>
+      <c r="M24" s="84"/>
+      <c r="N24" s="84"/>
+      <c r="O24" s="84"/>
+      <c r="P24" s="84"/>
+      <c r="Q24" s="84"/>
+      <c r="R24" s="84"/>
+      <c r="S24" s="84"/>
+      <c r="T24" s="84"/>
+      <c r="U24" s="84"/>
+      <c r="V24" s="84"/>
+      <c r="W24" s="84"/>
+      <c r="X24" s="85"/>
     </row>
     <row r="25" spans="1:24" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A25" s="90"/>
-      <c r="B25" s="91"/>
-      <c r="C25" s="91"/>
-      <c r="D25" s="91"/>
-      <c r="E25" s="91"/>
-      <c r="F25" s="91"/>
-      <c r="G25" s="91"/>
-      <c r="H25" s="91"/>
-      <c r="I25" s="91"/>
-      <c r="J25" s="91"/>
-      <c r="K25" s="91"/>
-      <c r="L25" s="91"/>
-      <c r="M25" s="91"/>
-      <c r="N25" s="91"/>
-      <c r="O25" s="91"/>
-      <c r="P25" s="91"/>
-      <c r="Q25" s="91"/>
-      <c r="R25" s="91"/>
-      <c r="S25" s="91"/>
-      <c r="T25" s="91"/>
-      <c r="U25" s="91"/>
-      <c r="V25" s="91"/>
-      <c r="W25" s="91"/>
-      <c r="X25" s="92"/>
+      <c r="A25" s="83"/>
+      <c r="B25" s="84"/>
+      <c r="C25" s="84"/>
+      <c r="D25" s="84"/>
+      <c r="E25" s="84"/>
+      <c r="F25" s="84"/>
+      <c r="G25" s="84"/>
+      <c r="H25" s="84"/>
+      <c r="I25" s="84"/>
+      <c r="J25" s="84"/>
+      <c r="K25" s="84"/>
+      <c r="L25" s="84"/>
+      <c r="M25" s="84"/>
+      <c r="N25" s="84"/>
+      <c r="O25" s="84"/>
+      <c r="P25" s="84"/>
+      <c r="Q25" s="84"/>
+      <c r="R25" s="84"/>
+      <c r="S25" s="84"/>
+      <c r="T25" s="84"/>
+      <c r="U25" s="84"/>
+      <c r="V25" s="84"/>
+      <c r="W25" s="84"/>
+      <c r="X25" s="85"/>
     </row>
     <row r="26" spans="1:24" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A26" s="90"/>
-      <c r="B26" s="91"/>
-      <c r="C26" s="91"/>
-      <c r="D26" s="91"/>
-      <c r="E26" s="91"/>
-      <c r="F26" s="91"/>
-      <c r="G26" s="91"/>
-      <c r="H26" s="91"/>
-      <c r="I26" s="91"/>
-      <c r="J26" s="91"/>
-      <c r="K26" s="91"/>
-      <c r="L26" s="91"/>
-      <c r="M26" s="91"/>
-      <c r="N26" s="91"/>
-      <c r="O26" s="91"/>
-      <c r="P26" s="91"/>
-      <c r="Q26" s="91"/>
-      <c r="R26" s="91"/>
-      <c r="S26" s="91"/>
-      <c r="T26" s="91"/>
-      <c r="U26" s="91"/>
-      <c r="V26" s="91"/>
-      <c r="W26" s="91"/>
-      <c r="X26" s="92"/>
+      <c r="A26" s="83"/>
+      <c r="B26" s="84"/>
+      <c r="C26" s="84"/>
+      <c r="D26" s="84"/>
+      <c r="E26" s="84"/>
+      <c r="F26" s="84"/>
+      <c r="G26" s="84"/>
+      <c r="H26" s="84"/>
+      <c r="I26" s="84"/>
+      <c r="J26" s="84"/>
+      <c r="K26" s="84"/>
+      <c r="L26" s="84"/>
+      <c r="M26" s="84"/>
+      <c r="N26" s="84"/>
+      <c r="O26" s="84"/>
+      <c r="P26" s="84"/>
+      <c r="Q26" s="84"/>
+      <c r="R26" s="84"/>
+      <c r="S26" s="84"/>
+      <c r="T26" s="84"/>
+      <c r="U26" s="84"/>
+      <c r="V26" s="84"/>
+      <c r="W26" s="84"/>
+      <c r="X26" s="85"/>
     </row>
     <row r="27" spans="1:24" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A27" s="90"/>
-      <c r="B27" s="91"/>
-      <c r="C27" s="91"/>
-      <c r="D27" s="91"/>
-      <c r="E27" s="91"/>
-      <c r="F27" s="91"/>
-      <c r="G27" s="91"/>
-      <c r="H27" s="91"/>
-      <c r="I27" s="91"/>
-      <c r="J27" s="91"/>
-      <c r="K27" s="91"/>
-      <c r="L27" s="91"/>
-      <c r="M27" s="91"/>
-      <c r="N27" s="91"/>
-      <c r="O27" s="91"/>
-      <c r="P27" s="91"/>
-      <c r="Q27" s="91"/>
-      <c r="R27" s="91"/>
-      <c r="S27" s="91"/>
-      <c r="T27" s="91"/>
-      <c r="U27" s="91"/>
-      <c r="V27" s="91"/>
-      <c r="W27" s="91"/>
-      <c r="X27" s="92"/>
+      <c r="A27" s="83"/>
+      <c r="B27" s="84"/>
+      <c r="C27" s="84"/>
+      <c r="D27" s="84"/>
+      <c r="E27" s="84"/>
+      <c r="F27" s="84"/>
+      <c r="G27" s="84"/>
+      <c r="H27" s="84"/>
+      <c r="I27" s="84"/>
+      <c r="J27" s="84"/>
+      <c r="K27" s="84"/>
+      <c r="L27" s="84"/>
+      <c r="M27" s="84"/>
+      <c r="N27" s="84"/>
+      <c r="O27" s="84"/>
+      <c r="P27" s="84"/>
+      <c r="Q27" s="84"/>
+      <c r="R27" s="84"/>
+      <c r="S27" s="84"/>
+      <c r="T27" s="84"/>
+      <c r="U27" s="84"/>
+      <c r="V27" s="84"/>
+      <c r="W27" s="84"/>
+      <c r="X27" s="85"/>
     </row>
     <row r="28" spans="1:24" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A28" s="90"/>
-      <c r="B28" s="91"/>
-      <c r="C28" s="91"/>
-      <c r="D28" s="91"/>
-      <c r="E28" s="91"/>
-      <c r="F28" s="91"/>
-      <c r="G28" s="91"/>
-      <c r="H28" s="91"/>
-      <c r="I28" s="91"/>
-      <c r="J28" s="91"/>
-      <c r="K28" s="91"/>
-      <c r="L28" s="91"/>
-      <c r="M28" s="91"/>
-      <c r="N28" s="91"/>
-      <c r="O28" s="91"/>
-      <c r="P28" s="91"/>
-      <c r="Q28" s="91"/>
-      <c r="R28" s="91"/>
-      <c r="S28" s="91"/>
-      <c r="T28" s="91"/>
-      <c r="U28" s="91"/>
-      <c r="V28" s="91"/>
-      <c r="W28" s="91"/>
-      <c r="X28" s="92"/>
+      <c r="A28" s="83"/>
+      <c r="B28" s="84"/>
+      <c r="C28" s="84"/>
+      <c r="D28" s="84"/>
+      <c r="E28" s="84"/>
+      <c r="F28" s="84"/>
+      <c r="G28" s="84"/>
+      <c r="H28" s="84"/>
+      <c r="I28" s="84"/>
+      <c r="J28" s="84"/>
+      <c r="K28" s="84"/>
+      <c r="L28" s="84"/>
+      <c r="M28" s="84"/>
+      <c r="N28" s="84"/>
+      <c r="O28" s="84"/>
+      <c r="P28" s="84"/>
+      <c r="Q28" s="84"/>
+      <c r="R28" s="84"/>
+      <c r="S28" s="84"/>
+      <c r="T28" s="84"/>
+      <c r="U28" s="84"/>
+      <c r="V28" s="84"/>
+      <c r="W28" s="84"/>
+      <c r="X28" s="85"/>
     </row>
     <row r="29" spans="1:24" s="3" customFormat="1" ht="20.25" customHeight="1" thickBot="1">
-      <c r="A29" s="22"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="16"/>
-      <c r="L29" s="16"/>
-      <c r="M29" s="16"/>
-      <c r="N29" s="16"/>
-      <c r="O29" s="16"/>
-      <c r="P29" s="16"/>
-      <c r="Q29" s="16"/>
-      <c r="R29" s="16"/>
-      <c r="S29" s="16"/>
-      <c r="T29" s="16"/>
-      <c r="U29" s="16"/>
-      <c r="V29" s="16"/>
-      <c r="W29" s="16"/>
+      <c r="A29" s="21"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="15"/>
+      <c r="O29" s="15"/>
+      <c r="P29" s="15"/>
+      <c r="Q29" s="15"/>
+      <c r="R29" s="15"/>
+      <c r="S29" s="15"/>
+      <c r="T29" s="15"/>
+      <c r="U29" s="15"/>
+      <c r="V29" s="15"/>
+      <c r="W29" s="15"/>
       <c r="X29" s="6"/>
     </row>
     <row r="30" spans="1:24" s="3" customFormat="1" ht="12" customHeight="1" thickBot="1"/>
     <row r="31" spans="1:24" s="3" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A31" s="37"/>
-      <c r="B31" s="39"/>
-      <c r="C31" s="187" t="s">
+      <c r="A31" s="35"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="239" t="s">
         <v>161</v>
       </c>
-      <c r="D31" s="188"/>
-      <c r="E31" s="187" t="s">
+      <c r="D31" s="241"/>
+      <c r="E31" s="239" t="s">
         <v>162</v>
       </c>
-      <c r="F31" s="188"/>
-      <c r="G31" s="138" t="s">
+      <c r="F31" s="241"/>
+      <c r="G31" s="127" t="s">
         <v>73</v>
       </c>
-      <c r="H31" s="141" t="s">
+      <c r="H31" s="130" t="s">
         <v>74</v>
       </c>
-      <c r="I31" s="44" t="s">
+      <c r="I31" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="J31" s="38"/>
-      <c r="K31" s="40" t="s">
+      <c r="J31" s="36"/>
+      <c r="K31" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="L31" s="34" t="s">
+      <c r="L31" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="M31" s="36"/>
-      <c r="N31" s="25" t="s">
+      <c r="M31" s="34"/>
+      <c r="N31" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="O31" s="189" t="s">
+      <c r="O31" s="259" t="s">
         <v>78</v>
       </c>
-      <c r="P31" s="190"/>
-      <c r="Q31" s="190"/>
-      <c r="R31" s="190"/>
-      <c r="S31" s="190"/>
-      <c r="T31" s="190"/>
-      <c r="U31" s="190"/>
-      <c r="V31" s="190"/>
-      <c r="W31" s="190"/>
-      <c r="X31" s="191"/>
+      <c r="P31" s="260"/>
+      <c r="Q31" s="260"/>
+      <c r="R31" s="260"/>
+      <c r="S31" s="260"/>
+      <c r="T31" s="260"/>
+      <c r="U31" s="260"/>
+      <c r="V31" s="260"/>
+      <c r="W31" s="260"/>
+      <c r="X31" s="261"/>
     </row>
     <row r="32" spans="1:24" s="3" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A32" s="195" t="s">
+      <c r="A32" s="265" t="s">
         <v>158</v>
       </c>
-      <c r="B32" s="196"/>
-      <c r="C32" s="257"/>
-      <c r="D32" s="196"/>
-      <c r="E32" s="257"/>
-      <c r="F32" s="196"/>
-      <c r="G32" s="258"/>
-      <c r="H32" s="35">
+      <c r="B32" s="167"/>
+      <c r="C32" s="166"/>
+      <c r="D32" s="167"/>
+      <c r="E32" s="166"/>
+      <c r="F32" s="167"/>
+      <c r="G32" s="169"/>
+      <c r="H32" s="33">
         <v>1</v>
       </c>
-      <c r="I32" s="45" t="s">
+      <c r="I32" s="43" t="s">
         <v>76</v>
       </c>
       <c r="J32" s="8"/>
-      <c r="K32" s="41" t="s">
+      <c r="K32" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="L32" s="46" t="s">
+      <c r="L32" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="M32" s="18"/>
-      <c r="N32" s="142"/>
-      <c r="O32" s="192" t="s">
+      <c r="M32" s="17"/>
+      <c r="N32" s="131"/>
+      <c r="O32" s="262" t="s">
         <v>139</v>
       </c>
-      <c r="P32" s="193"/>
-      <c r="Q32" s="193"/>
-      <c r="R32" s="182"/>
-      <c r="S32" s="181" t="s">
+      <c r="P32" s="263"/>
+      <c r="Q32" s="263"/>
+      <c r="R32" s="236"/>
+      <c r="S32" s="235" t="s">
         <v>79</v>
       </c>
-      <c r="T32" s="193"/>
-      <c r="U32" s="193"/>
-      <c r="V32" s="193"/>
-      <c r="W32" s="193"/>
-      <c r="X32" s="194"/>
+      <c r="T32" s="263"/>
+      <c r="U32" s="263"/>
+      <c r="V32" s="263"/>
+      <c r="W32" s="263"/>
+      <c r="X32" s="264"/>
     </row>
     <row r="33" spans="1:28" s="3" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A33" s="197"/>
-      <c r="B33" s="198"/>
-      <c r="C33" s="170"/>
-      <c r="D33" s="198"/>
-      <c r="E33" s="170"/>
-      <c r="F33" s="198"/>
-      <c r="G33" s="259"/>
-      <c r="H33" s="143" t="s">
+      <c r="A33" s="162"/>
+      <c r="B33" s="163"/>
+      <c r="C33" s="168"/>
+      <c r="D33" s="163"/>
+      <c r="E33" s="168"/>
+      <c r="F33" s="163"/>
+      <c r="G33" s="170"/>
+      <c r="H33" s="132" t="s">
         <v>74</v>
       </c>
-      <c r="I33" s="43" t="s">
+      <c r="I33" s="41" t="s">
         <v>75</v>
       </c>
       <c r="J33" s="8"/>
-      <c r="K33" s="41" t="s">
+      <c r="K33" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="L33" s="28" t="s">
+      <c r="L33" s="26" t="s">
         <v>58</v>
       </c>
       <c r="M33" s="4"/>
-      <c r="N33" s="144" t="s">
+      <c r="N33" s="133" t="s">
         <v>59</v>
       </c>
-      <c r="O33" s="136">
+      <c r="O33" s="125">
         <v>1</v>
       </c>
-      <c r="P33" s="125"/>
-      <c r="Q33" s="125">
+      <c r="P33" s="114"/>
+      <c r="Q33" s="114">
         <v>4</v>
       </c>
-      <c r="R33" s="126"/>
-      <c r="S33" s="127">
+      <c r="R33" s="115"/>
+      <c r="S33" s="116">
         <v>1</v>
       </c>
-      <c r="T33" s="128"/>
-      <c r="U33" s="129"/>
-      <c r="V33" s="181">
+      <c r="T33" s="117"/>
+      <c r="U33" s="118"/>
+      <c r="V33" s="235">
         <v>4</v>
       </c>
-      <c r="W33" s="182"/>
-      <c r="X33" s="130"/>
+      <c r="W33" s="236"/>
+      <c r="X33" s="119"/>
     </row>
     <row r="34" spans="1:28" s="3" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A34" s="179" t="s">
+      <c r="A34" s="253" t="s">
         <v>159</v>
       </c>
-      <c r="B34" s="180"/>
+      <c r="B34" s="254"/>
       <c r="C34" s="173"/>
-      <c r="D34" s="215"/>
+      <c r="D34" s="172"/>
       <c r="E34" s="173"/>
-      <c r="F34" s="215"/>
-      <c r="G34" s="139"/>
-      <c r="H34" s="145">
+      <c r="F34" s="172"/>
+      <c r="G34" s="128"/>
+      <c r="H34" s="134">
         <v>2</v>
       </c>
-      <c r="I34" s="43" t="s">
+      <c r="I34" s="41" t="s">
         <v>76</v>
       </c>
       <c r="J34" s="8"/>
-      <c r="K34" s="41" t="s">
+      <c r="K34" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="L34" s="46" t="s">
+      <c r="L34" s="44" t="s">
         <v>77</v>
       </c>
       <c r="M34" s="7"/>
-      <c r="N34" s="142"/>
-      <c r="O34" s="136">
+      <c r="N34" s="131"/>
+      <c r="O34" s="125">
         <v>2</v>
       </c>
-      <c r="P34" s="125"/>
-      <c r="Q34" s="125">
+      <c r="P34" s="114"/>
+      <c r="Q34" s="114">
         <v>5</v>
       </c>
-      <c r="R34" s="126"/>
-      <c r="S34" s="125">
+      <c r="R34" s="115"/>
+      <c r="S34" s="114">
         <v>2</v>
       </c>
-      <c r="T34" s="123"/>
-      <c r="U34" s="124"/>
-      <c r="V34" s="181">
+      <c r="T34" s="112"/>
+      <c r="U34" s="113"/>
+      <c r="V34" s="235">
         <v>5</v>
       </c>
-      <c r="W34" s="182"/>
-      <c r="X34" s="130"/>
+      <c r="W34" s="236"/>
+      <c r="X34" s="119"/>
       <c r="AB34" s="4"/>
     </row>
     <row r="35" spans="1:28" s="3" customFormat="1" ht="28.5" customHeight="1" thickBot="1">
-      <c r="A35" s="183" t="s">
+      <c r="A35" s="255" t="s">
         <v>160</v>
       </c>
-      <c r="B35" s="184"/>
-      <c r="C35" s="176"/>
-      <c r="D35" s="256"/>
-      <c r="E35" s="176"/>
-      <c r="F35" s="256"/>
-      <c r="G35" s="140"/>
-      <c r="H35" s="62"/>
+      <c r="B35" s="256"/>
+      <c r="C35" s="164"/>
+      <c r="D35" s="165"/>
+      <c r="E35" s="164"/>
+      <c r="F35" s="165"/>
+      <c r="G35" s="129"/>
+      <c r="H35" s="59"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
       <c r="M35" s="5"/>
       <c r="N35" s="6"/>
-      <c r="O35" s="137">
+      <c r="O35" s="126">
         <v>3</v>
       </c>
-      <c r="P35" s="131"/>
-      <c r="Q35" s="131">
+      <c r="P35" s="120"/>
+      <c r="Q35" s="120">
         <v>6</v>
       </c>
-      <c r="R35" s="132"/>
-      <c r="S35" s="131">
+      <c r="R35" s="121"/>
+      <c r="S35" s="120">
         <v>3</v>
       </c>
-      <c r="T35" s="133"/>
-      <c r="U35" s="134"/>
-      <c r="V35" s="185">
+      <c r="T35" s="122"/>
+      <c r="U35" s="123"/>
+      <c r="V35" s="257">
         <v>6</v>
       </c>
-      <c r="W35" s="186"/>
-      <c r="X35" s="135"/>
+      <c r="W35" s="258"/>
+      <c r="X35" s="124"/>
     </row>
     <row r="36" spans="1:28" s="3" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A36" s="113" t="s">
+      <c r="A36" s="102" t="s">
         <v>173</v>
       </c>
-      <c r="B36" s="114"/>
-      <c r="C36" s="114"/>
-      <c r="D36" s="114"/>
-      <c r="E36" s="114"/>
-      <c r="F36" s="114"/>
-      <c r="G36" s="115"/>
-      <c r="T36" s="199" t="s">
+      <c r="B36" s="103"/>
+      <c r="C36" s="103"/>
+      <c r="D36" s="103"/>
+      <c r="E36" s="103"/>
+      <c r="F36" s="103"/>
+      <c r="G36" s="104"/>
+      <c r="T36" s="234" t="s">
         <v>153</v>
       </c>
-      <c r="U36" s="199"/>
-      <c r="V36" s="199"/>
-      <c r="W36" s="199"/>
-      <c r="X36" s="122" t="s">
+      <c r="U36" s="234"/>
+      <c r="V36" s="234"/>
+      <c r="W36" s="234"/>
+      <c r="X36" s="111" t="s">
         <v>132</v>
       </c>
     </row>
@@ -4368,49 +4377,23 @@
     <row r="48" spans="1:28" s="3" customFormat="1" ht="17.399999999999999"/>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="A5:B7"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="C32:D33"/>
-    <mergeCell ref="E32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:M8"/>
-    <mergeCell ref="J6:M7"/>
-    <mergeCell ref="C9:E10"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C5:E7"/>
-    <mergeCell ref="F5:I7"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="T7:U7"/>
-    <mergeCell ref="J5:M5"/>
-    <mergeCell ref="N5:Q5"/>
-    <mergeCell ref="R6:R7"/>
-    <mergeCell ref="S6:S7"/>
-    <mergeCell ref="N6:Q7"/>
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="Z2:AU2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="N4:Q4"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="T4:X4"/>
-    <mergeCell ref="A2:R3"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="T8:U8"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="T9:U9"/>
-    <mergeCell ref="R8:S8"/>
-    <mergeCell ref="N8:Q8"/>
+    <mergeCell ref="V5:X5"/>
+    <mergeCell ref="V6:X6"/>
+    <mergeCell ref="V7:X7"/>
+    <mergeCell ref="V8:X8"/>
+    <mergeCell ref="V9:X9"/>
+    <mergeCell ref="V10:X10"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="V34:W34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="V35:W35"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="O31:X31"/>
+    <mergeCell ref="O32:R32"/>
+    <mergeCell ref="S32:X32"/>
+    <mergeCell ref="A32:B33"/>
+    <mergeCell ref="E35:F35"/>
     <mergeCell ref="T36:W36"/>
     <mergeCell ref="V33:W33"/>
     <mergeCell ref="T10:U10"/>
@@ -4427,23 +4410,49 @@
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="C35:D35"/>
-    <mergeCell ref="V10:X10"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="V34:W34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="V35:W35"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="O31:X31"/>
-    <mergeCell ref="O32:R32"/>
-    <mergeCell ref="S32:X32"/>
-    <mergeCell ref="A32:B33"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="V5:X5"/>
-    <mergeCell ref="V6:X6"/>
-    <mergeCell ref="V7:X7"/>
-    <mergeCell ref="V8:X8"/>
-    <mergeCell ref="V9:X9"/>
+    <mergeCell ref="T8:U8"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="T9:U9"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="N8:Q8"/>
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="Z2:AU2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="N4:Q4"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="T4:X4"/>
+    <mergeCell ref="A2:R3"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="T7:U7"/>
+    <mergeCell ref="J5:M5"/>
+    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="R6:R7"/>
+    <mergeCell ref="S6:S7"/>
+    <mergeCell ref="N6:Q7"/>
+    <mergeCell ref="A5:B7"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="C32:D33"/>
+    <mergeCell ref="E32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:M8"/>
+    <mergeCell ref="J6:M7"/>
+    <mergeCell ref="C9:E10"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C5:E7"/>
+    <mergeCell ref="F5:I7"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -4461,208 +4470,208 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23:P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="19.8"/>
   <cols>
-    <col min="1" max="1" width="12.875" style="49" customWidth="1"/>
-    <col min="2" max="2" width="10.75" style="49" customWidth="1"/>
-    <col min="3" max="3" width="12.875" style="49" customWidth="1"/>
-    <col min="4" max="4" width="12.125" style="49" customWidth="1"/>
-    <col min="5" max="7" width="11" style="49" customWidth="1"/>
-    <col min="8" max="9" width="10.75" style="49" customWidth="1"/>
-    <col min="10" max="10" width="4" style="49" customWidth="1"/>
-    <col min="11" max="13" width="11.125" style="49" customWidth="1"/>
-    <col min="14" max="14" width="11.375" style="49" customWidth="1"/>
-    <col min="15" max="18" width="11.125" style="49" customWidth="1"/>
-    <col min="19" max="16384" width="9.125" style="49"/>
+    <col min="1" max="1" width="12.875" style="47" customWidth="1"/>
+    <col min="2" max="2" width="10.75" style="47" customWidth="1"/>
+    <col min="3" max="3" width="12.875" style="47" customWidth="1"/>
+    <col min="4" max="4" width="12.125" style="47" customWidth="1"/>
+    <col min="5" max="7" width="11" style="47" customWidth="1"/>
+    <col min="8" max="9" width="10.75" style="47" customWidth="1"/>
+    <col min="10" max="10" width="4" style="47" customWidth="1"/>
+    <col min="11" max="13" width="11.125" style="47" customWidth="1"/>
+    <col min="14" max="14" width="11.375" style="47" customWidth="1"/>
+    <col min="15" max="18" width="11.125" style="47" customWidth="1"/>
+    <col min="19" max="16384" width="9.125" style="47"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="8.25" customHeight="1" thickBot="1"/>
     <row r="2" spans="1:18" s="1" customFormat="1" ht="23.4">
-      <c r="A2" s="109" t="s">
+      <c r="A2" s="98" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="110"/>
-      <c r="C2" s="110"/>
-      <c r="D2" s="110"/>
-      <c r="E2" s="110"/>
-      <c r="F2" s="110"/>
-      <c r="G2" s="110"/>
-      <c r="H2" s="110"/>
-      <c r="I2" s="110"/>
-      <c r="J2" s="110"/>
-      <c r="K2" s="110" t="s">
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99" t="s">
         <v>92</v>
       </c>
-      <c r="L2" s="110"/>
-      <c r="M2" s="110"/>
-      <c r="N2" s="110"/>
-      <c r="O2" s="110"/>
-      <c r="P2" s="110"/>
-      <c r="Q2" s="110"/>
-      <c r="R2" s="111"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
+      <c r="O2" s="99"/>
+      <c r="P2" s="99"/>
+      <c r="Q2" s="99"/>
+      <c r="R2" s="100"/>
     </row>
     <row r="3" spans="1:18" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A3" s="87"/>
-      <c r="B3" s="88"/>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="88"/>
-      <c r="K3" s="88"/>
-      <c r="L3" s="88"/>
-      <c r="M3" s="88"/>
-      <c r="N3" s="88"/>
-      <c r="O3" s="88"/>
-      <c r="P3" s="88"/>
-      <c r="Q3" s="88"/>
-      <c r="R3" s="89"/>
+      <c r="A3" s="80"/>
+      <c r="B3" s="81"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
+      <c r="O3" s="81"/>
+      <c r="P3" s="81"/>
+      <c r="Q3" s="81"/>
+      <c r="R3" s="82"/>
     </row>
     <row r="4" spans="1:18" s="3" customFormat="1" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A4" s="218" t="s">
+      <c r="A4" s="216" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="283"/>
-      <c r="C4" s="286" t="s">
+      <c r="B4" s="275"/>
+      <c r="C4" s="276" t="s">
         <v>89</v>
       </c>
-      <c r="D4" s="283"/>
-      <c r="E4" s="286" t="s">
+      <c r="D4" s="275"/>
+      <c r="E4" s="276" t="s">
         <v>88</v>
       </c>
-      <c r="F4" s="283"/>
-      <c r="G4" s="219" t="s">
+      <c r="F4" s="275"/>
+      <c r="G4" s="217" t="s">
         <v>152</v>
       </c>
-      <c r="H4" s="219"/>
-      <c r="I4" s="220"/>
+      <c r="H4" s="217"/>
+      <c r="I4" s="218"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="289" t="s">
+      <c r="K4" s="277" t="s">
         <v>94</v>
       </c>
-      <c r="L4" s="290"/>
-      <c r="M4" s="290"/>
-      <c r="N4" s="290"/>
-      <c r="O4" s="290"/>
-      <c r="P4" s="290"/>
-      <c r="Q4" s="290"/>
-      <c r="R4" s="291"/>
+      <c r="L4" s="278"/>
+      <c r="M4" s="278"/>
+      <c r="N4" s="278"/>
+      <c r="O4" s="278"/>
+      <c r="P4" s="278"/>
+      <c r="Q4" s="278"/>
+      <c r="R4" s="279"/>
     </row>
     <row r="5" spans="1:18" ht="21.75" customHeight="1">
-      <c r="A5" s="50"/>
-      <c r="B5" s="51"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="88"/>
-      <c r="K5" s="292" t="s">
+      <c r="A5" s="296"/>
+      <c r="B5" s="200"/>
+      <c r="C5" s="199"/>
+      <c r="D5" s="200"/>
+      <c r="E5" s="199"/>
+      <c r="F5" s="200"/>
+      <c r="G5" s="199"/>
+      <c r="H5" s="234"/>
+      <c r="I5" s="298"/>
+      <c r="J5" s="81"/>
+      <c r="K5" s="270" t="s">
         <v>170</v>
       </c>
-      <c r="L5" s="293"/>
-      <c r="M5" s="279"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="278" t="s">
+      <c r="L5" s="271"/>
+      <c r="M5" s="272"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="280" t="s">
         <v>141</v>
       </c>
-      <c r="P5" s="279"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="9"/>
+      <c r="P5" s="272"/>
+      <c r="Q5" s="280"/>
+      <c r="R5" s="305"/>
     </row>
     <row r="6" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A6" s="54"/>
-      <c r="B6" s="55"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="88"/>
-      <c r="K6" s="260" t="s">
+      <c r="A6" s="285"/>
+      <c r="B6" s="287"/>
+      <c r="C6" s="297"/>
+      <c r="D6" s="287"/>
+      <c r="E6" s="297"/>
+      <c r="F6" s="287"/>
+      <c r="G6" s="297"/>
+      <c r="H6" s="286"/>
+      <c r="I6" s="299"/>
+      <c r="J6" s="81"/>
+      <c r="K6" s="171" t="s">
         <v>171</v>
       </c>
-      <c r="L6" s="215"/>
-      <c r="M6" s="42" t="s">
+      <c r="L6" s="172"/>
+      <c r="M6" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="N6" s="19"/>
-      <c r="O6" s="14" t="s">
+      <c r="N6" s="18"/>
+      <c r="O6" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="14" t="s">
+      <c r="P6" s="18"/>
+      <c r="Q6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="R6" s="59"/>
+      <c r="R6" s="56"/>
     </row>
     <row r="7" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A7" s="87"/>
-      <c r="B7" s="88"/>
-      <c r="C7" s="88"/>
-      <c r="D7" s="88"/>
-      <c r="E7" s="88"/>
-      <c r="F7" s="88"/>
-      <c r="G7" s="88"/>
-      <c r="H7" s="88"/>
-      <c r="I7" s="88"/>
-      <c r="J7" s="88"/>
-      <c r="K7" s="294" t="s">
+      <c r="A7" s="80"/>
+      <c r="B7" s="81"/>
+      <c r="C7" s="81"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="81"/>
+      <c r="G7" s="81"/>
+      <c r="H7" s="81"/>
+      <c r="I7" s="81"/>
+      <c r="J7" s="81"/>
+      <c r="K7" s="273" t="s">
         <v>172</v>
       </c>
-      <c r="L7" s="295"/>
-      <c r="M7" s="20" t="s">
+      <c r="L7" s="274"/>
+      <c r="M7" s="19" t="s">
         <v>3</v>
       </c>
       <c r="N7" s="10"/>
-      <c r="O7" s="267" t="s">
+      <c r="O7" s="182" t="s">
         <v>108</v>
       </c>
-      <c r="P7" s="212"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="6"/>
+      <c r="P7" s="184"/>
+      <c r="Q7" s="164"/>
+      <c r="R7" s="252"/>
     </row>
     <row r="8" spans="1:18" s="3" customFormat="1" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A8" s="60" t="s">
+      <c r="A8" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="E8" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="F8" s="29" t="s">
+      <c r="F8" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="G8" s="29" t="s">
+      <c r="G8" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="H8" s="27" t="s">
+      <c r="H8" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="I8" s="61" t="s">
+      <c r="I8" s="58" t="s">
         <v>84</v>
       </c>
       <c r="J8" s="4"/>
-      <c r="K8" s="112" t="s">
+      <c r="K8" s="101" t="s">
         <v>142</v>
       </c>
       <c r="L8" s="4"/>
@@ -4671,152 +4680,152 @@
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
-      <c r="R8" s="74"/>
+      <c r="R8" s="70"/>
     </row>
     <row r="9" spans="1:18" s="3" customFormat="1" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A9" s="63" t="s">
+      <c r="A9" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="64" t="s">
+      <c r="B9" s="61" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="64" t="s">
+      <c r="C9" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="D9" s="65" t="s">
+      <c r="D9" s="62" t="s">
         <v>97</v>
       </c>
-      <c r="E9" s="64" t="s">
+      <c r="E9" s="61" t="s">
         <v>98</v>
       </c>
-      <c r="F9" s="64" t="s">
+      <c r="F9" s="61" t="s">
         <v>99</v>
       </c>
-      <c r="G9" s="64" t="s">
+      <c r="G9" s="61" t="s">
         <v>100</v>
       </c>
-      <c r="H9" s="66" t="s">
+      <c r="H9" s="63" t="s">
         <v>101</v>
       </c>
-      <c r="I9" s="67" t="s">
+      <c r="I9" s="64" t="s">
         <v>34</v>
       </c>
       <c r="J9" s="4"/>
-      <c r="K9" s="71" t="s">
+      <c r="K9" s="68" t="s">
         <v>104</v>
       </c>
-      <c r="L9" s="38" t="s">
+      <c r="L9" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="M9" s="39"/>
-      <c r="N9" s="278" t="s">
+      <c r="M9" s="37"/>
+      <c r="N9" s="280" t="s">
         <v>109</v>
       </c>
-      <c r="O9" s="279"/>
-      <c r="P9" s="234" t="s">
+      <c r="O9" s="272"/>
+      <c r="P9" s="185" t="s">
         <v>110</v>
       </c>
-      <c r="Q9" s="235"/>
-      <c r="R9" s="287"/>
+      <c r="Q9" s="186"/>
+      <c r="R9" s="281"/>
     </row>
     <row r="10" spans="1:18" ht="21.75" customHeight="1">
-      <c r="A10" s="68" t="s">
+      <c r="A10" s="65" t="s">
         <v>86</v>
       </c>
-      <c r="B10" s="69"/>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="69"/>
-      <c r="G10" s="69"/>
-      <c r="H10" s="69"/>
-      <c r="I10" s="70"/>
-      <c r="J10" s="88"/>
-      <c r="K10" s="24" t="s">
+      <c r="B10" s="66"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="67"/>
+      <c r="J10" s="81"/>
+      <c r="K10" s="22" t="s">
         <v>105</v>
       </c>
       <c r="L10" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="M10" s="12"/>
+      <c r="M10" s="11"/>
       <c r="N10" s="173" t="s">
         <v>109</v>
       </c>
-      <c r="O10" s="215"/>
-      <c r="P10" s="257" t="s">
+      <c r="O10" s="172"/>
+      <c r="P10" s="166" t="s">
         <v>110</v>
       </c>
-      <c r="Q10" s="210"/>
-      <c r="R10" s="288"/>
+      <c r="Q10" s="181"/>
+      <c r="R10" s="282"/>
     </row>
     <row r="11" spans="1:18" ht="21.75" customHeight="1">
-      <c r="A11" s="94"/>
-      <c r="B11" s="95"/>
-      <c r="C11" s="95"/>
-      <c r="D11" s="95"/>
-      <c r="E11" s="95"/>
-      <c r="F11" s="95"/>
-      <c r="G11" s="95"/>
-      <c r="H11" s="95"/>
-      <c r="I11" s="96"/>
-      <c r="J11" s="88"/>
-      <c r="K11" s="24" t="s">
+      <c r="A11" s="87"/>
+      <c r="B11" s="88"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="88"/>
+      <c r="E11" s="88"/>
+      <c r="F11" s="88"/>
+      <c r="G11" s="88"/>
+      <c r="H11" s="88"/>
+      <c r="I11" s="89"/>
+      <c r="J11" s="81"/>
+      <c r="K11" s="22" t="s">
         <v>106</v>
       </c>
       <c r="L11" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="M11" s="12"/>
+      <c r="M11" s="11"/>
       <c r="N11" s="173" t="s">
         <v>109</v>
       </c>
-      <c r="O11" s="215"/>
+      <c r="O11" s="172"/>
       <c r="P11" s="173" t="s">
         <v>110</v>
       </c>
       <c r="Q11" s="174"/>
-      <c r="R11" s="175"/>
+      <c r="R11" s="269"/>
     </row>
     <row r="12" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A12" s="97"/>
-      <c r="B12" s="98"/>
-      <c r="C12" s="98"/>
-      <c r="D12" s="98"/>
-      <c r="E12" s="98"/>
-      <c r="F12" s="98"/>
-      <c r="G12" s="98"/>
-      <c r="H12" s="98"/>
-      <c r="I12" s="99"/>
-      <c r="J12" s="88"/>
-      <c r="K12" s="73" t="s">
+      <c r="A12" s="90"/>
+      <c r="B12" s="91"/>
+      <c r="C12" s="91"/>
+      <c r="D12" s="91"/>
+      <c r="E12" s="91"/>
+      <c r="F12" s="91"/>
+      <c r="G12" s="91"/>
+      <c r="H12" s="91"/>
+      <c r="I12" s="92"/>
+      <c r="J12" s="81"/>
+      <c r="K12" s="69" t="s">
         <v>107</v>
       </c>
       <c r="L12" s="5" t="s">
         <v>127</v>
       </c>
       <c r="M12" s="10"/>
-      <c r="N12" s="267" t="s">
+      <c r="N12" s="182" t="s">
         <v>109</v>
       </c>
-      <c r="O12" s="212"/>
+      <c r="O12" s="184"/>
       <c r="P12" s="173" t="s">
         <v>110</v>
       </c>
       <c r="Q12" s="174"/>
-      <c r="R12" s="175"/>
+      <c r="R12" s="269"/>
     </row>
     <row r="13" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A13" s="97"/>
-      <c r="B13" s="98"/>
-      <c r="C13" s="98"/>
-      <c r="D13" s="98"/>
-      <c r="E13" s="98"/>
-      <c r="F13" s="98"/>
-      <c r="G13" s="98"/>
-      <c r="H13" s="98"/>
-      <c r="I13" s="99"/>
-      <c r="J13" s="88"/>
-      <c r="K13" s="112" t="s">
+      <c r="A13" s="90"/>
+      <c r="B13" s="91"/>
+      <c r="C13" s="91"/>
+      <c r="D13" s="91"/>
+      <c r="E13" s="91"/>
+      <c r="F13" s="91"/>
+      <c r="G13" s="91"/>
+      <c r="H13" s="91"/>
+      <c r="I13" s="92"/>
+      <c r="J13" s="81"/>
+      <c r="K13" s="101" t="s">
         <v>143</v>
       </c>
       <c r="L13" s="4"/>
@@ -4825,116 +4834,116 @@
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
-      <c r="R13" s="74"/>
+      <c r="R13" s="70"/>
     </row>
     <row r="14" spans="1:18" ht="21.75" customHeight="1">
-      <c r="A14" s="97"/>
-      <c r="B14" s="98"/>
-      <c r="C14" s="98"/>
-      <c r="D14" s="98"/>
-      <c r="E14" s="98"/>
-      <c r="F14" s="98"/>
-      <c r="G14" s="98"/>
-      <c r="H14" s="98"/>
-      <c r="I14" s="99"/>
-      <c r="J14" s="88"/>
-      <c r="K14" s="37" t="s">
+      <c r="A14" s="90"/>
+      <c r="B14" s="91"/>
+      <c r="C14" s="91"/>
+      <c r="D14" s="91"/>
+      <c r="E14" s="91"/>
+      <c r="F14" s="91"/>
+      <c r="G14" s="91"/>
+      <c r="H14" s="91"/>
+      <c r="I14" s="92"/>
+      <c r="J14" s="81"/>
+      <c r="K14" s="35" t="s">
         <v>144</v>
       </c>
-      <c r="L14" s="38"/>
-      <c r="M14" s="38"/>
-      <c r="N14" s="39"/>
-      <c r="O14" s="101" t="s">
+      <c r="L14" s="36"/>
+      <c r="M14" s="36"/>
+      <c r="N14" s="37"/>
+      <c r="O14" s="94" t="s">
         <v>104</v>
       </c>
-      <c r="P14" s="101" t="s">
+      <c r="P14" s="94" t="s">
         <v>105</v>
       </c>
-      <c r="Q14" s="101" t="s">
+      <c r="Q14" s="94" t="s">
         <v>106</v>
       </c>
-      <c r="R14" s="102" t="s">
+      <c r="R14" s="95" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="21.75" customHeight="1">
-      <c r="A15" s="97"/>
-      <c r="B15" s="98"/>
-      <c r="C15" s="98"/>
-      <c r="D15" s="98"/>
-      <c r="E15" s="98"/>
-      <c r="F15" s="98"/>
-      <c r="G15" s="98"/>
-      <c r="H15" s="98"/>
-      <c r="I15" s="99"/>
-      <c r="J15" s="88"/>
-      <c r="K15" s="58" t="s">
+      <c r="A15" s="90"/>
+      <c r="B15" s="91"/>
+      <c r="C15" s="91"/>
+      <c r="D15" s="91"/>
+      <c r="E15" s="91"/>
+      <c r="F15" s="91"/>
+      <c r="G15" s="91"/>
+      <c r="H15" s="91"/>
+      <c r="I15" s="92"/>
+      <c r="J15" s="81"/>
+      <c r="K15" s="55" t="s">
         <v>145</v>
       </c>
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
       <c r="R15" s="9"/>
     </row>
     <row r="16" spans="1:18" ht="21.75" customHeight="1">
-      <c r="A16" s="97"/>
-      <c r="B16" s="98"/>
-      <c r="C16" s="98"/>
-      <c r="D16" s="98"/>
-      <c r="E16" s="98"/>
-      <c r="F16" s="98"/>
-      <c r="G16" s="98"/>
-      <c r="H16" s="98"/>
-      <c r="I16" s="99"/>
-      <c r="J16" s="88"/>
-      <c r="K16" s="58" t="s">
+      <c r="A16" s="90"/>
+      <c r="B16" s="91"/>
+      <c r="C16" s="91"/>
+      <c r="D16" s="91"/>
+      <c r="E16" s="91"/>
+      <c r="F16" s="91"/>
+      <c r="G16" s="91"/>
+      <c r="H16" s="91"/>
+      <c r="I16" s="92"/>
+      <c r="J16" s="81"/>
+      <c r="K16" s="55" t="s">
         <v>146</v>
       </c>
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
       <c r="R16" s="9"/>
     </row>
     <row r="17" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A17" s="97"/>
-      <c r="B17" s="98"/>
-      <c r="C17" s="98"/>
-      <c r="D17" s="98"/>
-      <c r="E17" s="98"/>
-      <c r="F17" s="98"/>
-      <c r="G17" s="98"/>
-      <c r="H17" s="98"/>
-      <c r="I17" s="99"/>
-      <c r="J17" s="88"/>
-      <c r="K17" s="62" t="s">
+      <c r="A17" s="90"/>
+      <c r="B17" s="91"/>
+      <c r="C17" s="91"/>
+      <c r="D17" s="91"/>
+      <c r="E17" s="91"/>
+      <c r="F17" s="91"/>
+      <c r="G17" s="91"/>
+      <c r="H17" s="91"/>
+      <c r="I17" s="92"/>
+      <c r="J17" s="81"/>
+      <c r="K17" s="59" t="s">
         <v>147</v>
       </c>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
       <c r="N17" s="10"/>
-      <c r="O17" s="16"/>
-      <c r="P17" s="16"/>
-      <c r="Q17" s="16"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
       <c r="R17" s="6"/>
     </row>
     <row r="18" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A18" s="93"/>
-      <c r="B18" s="75"/>
-      <c r="C18" s="75"/>
-      <c r="D18" s="75"/>
-      <c r="E18" s="75"/>
-      <c r="F18" s="75"/>
-      <c r="G18" s="75"/>
-      <c r="H18" s="75"/>
-      <c r="I18" s="57"/>
-      <c r="J18" s="88"/>
-      <c r="K18" s="112" t="s">
+      <c r="A18" s="86"/>
+      <c r="B18" s="71"/>
+      <c r="C18" s="71"/>
+      <c r="D18" s="71"/>
+      <c r="E18" s="71"/>
+      <c r="F18" s="71"/>
+      <c r="G18" s="71"/>
+      <c r="H18" s="71"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="81"/>
+      <c r="K18" s="101" t="s">
         <v>111</v>
       </c>
       <c r="L18" s="4"/>
@@ -4943,164 +4952,164 @@
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
-      <c r="R18" s="74"/>
+      <c r="R18" s="70"/>
     </row>
     <row r="19" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A19" s="272" t="s">
+      <c r="A19" s="285" t="s">
         <v>85</v>
       </c>
-      <c r="B19" s="273"/>
-      <c r="C19" s="273"/>
-      <c r="D19" s="274"/>
-      <c r="E19" s="75"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="75"/>
-      <c r="H19" s="75"/>
-      <c r="I19" s="57"/>
-      <c r="J19" s="88"/>
-      <c r="K19" s="37" t="s">
+      <c r="B19" s="286"/>
+      <c r="C19" s="286"/>
+      <c r="D19" s="287"/>
+      <c r="E19" s="71"/>
+      <c r="F19" s="71"/>
+      <c r="G19" s="71"/>
+      <c r="H19" s="71"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="81"/>
+      <c r="K19" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="L19" s="38"/>
-      <c r="M19" s="38"/>
-      <c r="N19" s="39"/>
-      <c r="O19" s="278" t="s">
+      <c r="L19" s="36"/>
+      <c r="M19" s="36"/>
+      <c r="N19" s="37"/>
+      <c r="O19" s="280" t="s">
         <v>118</v>
       </c>
-      <c r="P19" s="279"/>
-      <c r="Q19" s="284" t="s">
+      <c r="P19" s="272"/>
+      <c r="Q19" s="294" t="s">
         <v>119</v>
       </c>
-      <c r="R19" s="285"/>
+      <c r="R19" s="295"/>
     </row>
     <row r="20" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A20" s="87"/>
-      <c r="B20" s="88"/>
-      <c r="C20" s="88"/>
-      <c r="D20" s="88"/>
-      <c r="E20" s="88"/>
-      <c r="F20" s="88"/>
-      <c r="G20" s="88"/>
-      <c r="H20" s="88"/>
-      <c r="I20" s="88"/>
-      <c r="J20" s="88"/>
-      <c r="K20" s="58" t="s">
+      <c r="A20" s="80"/>
+      <c r="B20" s="81"/>
+      <c r="C20" s="81"/>
+      <c r="D20" s="81"/>
+      <c r="E20" s="81"/>
+      <c r="F20" s="81"/>
+      <c r="G20" s="81"/>
+      <c r="H20" s="81"/>
+      <c r="I20" s="81"/>
+      <c r="J20" s="81"/>
+      <c r="K20" s="55" t="s">
         <v>113</v>
       </c>
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
-      <c r="N20" s="12"/>
-      <c r="O20" s="11"/>
-      <c r="P20" s="12"/>
-      <c r="Q20" s="8"/>
-      <c r="R20" s="9"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="173"/>
+      <c r="P20" s="172"/>
+      <c r="Q20" s="173"/>
+      <c r="R20" s="269"/>
     </row>
     <row r="21" spans="1:18" s="3" customFormat="1" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A21" s="218" t="s">
+      <c r="A21" s="216" t="s">
         <v>90</v>
       </c>
-      <c r="B21" s="283"/>
-      <c r="C21" s="286" t="s">
+      <c r="B21" s="275"/>
+      <c r="C21" s="276" t="s">
         <v>89</v>
       </c>
-      <c r="D21" s="283"/>
-      <c r="E21" s="286" t="s">
+      <c r="D21" s="275"/>
+      <c r="E21" s="276" t="s">
         <v>91</v>
       </c>
-      <c r="F21" s="283"/>
-      <c r="G21" s="219" t="s">
+      <c r="F21" s="275"/>
+      <c r="G21" s="217" t="s">
         <v>87</v>
       </c>
-      <c r="H21" s="219"/>
-      <c r="I21" s="220"/>
+      <c r="H21" s="217"/>
+      <c r="I21" s="218"/>
       <c r="J21" s="4"/>
-      <c r="K21" s="58" t="s">
+      <c r="K21" s="55" t="s">
         <v>115</v>
       </c>
       <c r="L21" s="8"/>
       <c r="M21" s="8"/>
-      <c r="N21" s="12"/>
-      <c r="O21" s="11"/>
-      <c r="P21" s="12"/>
-      <c r="Q21" s="8"/>
-      <c r="R21" s="9"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="173"/>
+      <c r="P21" s="172"/>
+      <c r="Q21" s="173"/>
+      <c r="R21" s="269"/>
     </row>
     <row r="22" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A22" s="54"/>
-      <c r="B22" s="55"/>
-      <c r="C22" s="76"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="76"/>
-      <c r="F22" s="55"/>
-      <c r="G22" s="56"/>
-      <c r="H22" s="56"/>
-      <c r="I22" s="57"/>
-      <c r="J22" s="88"/>
-      <c r="K22" s="21" t="s">
+      <c r="A22" s="300"/>
+      <c r="B22" s="301"/>
+      <c r="C22" s="302"/>
+      <c r="D22" s="301"/>
+      <c r="E22" s="302"/>
+      <c r="F22" s="301"/>
+      <c r="G22" s="302"/>
+      <c r="H22" s="303"/>
+      <c r="I22" s="304"/>
+      <c r="J22" s="81"/>
+      <c r="K22" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="L22" s="77"/>
-      <c r="M22" s="78"/>
-      <c r="N22" s="42" t="s">
+      <c r="L22" s="72"/>
+      <c r="M22" s="73"/>
+      <c r="N22" s="40" t="s">
         <v>117</v>
       </c>
-      <c r="O22" s="79"/>
-      <c r="P22" s="78"/>
-      <c r="Q22" s="77"/>
-      <c r="R22" s="48" t="s">
+      <c r="O22" s="203"/>
+      <c r="P22" s="204"/>
+      <c r="Q22" s="72"/>
+      <c r="R22" s="46" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A23" s="87"/>
-      <c r="B23" s="88"/>
-      <c r="C23" s="88"/>
-      <c r="D23" s="88"/>
-      <c r="E23" s="88"/>
-      <c r="F23" s="88"/>
-      <c r="G23" s="88"/>
-      <c r="H23" s="88"/>
-      <c r="I23" s="88"/>
-      <c r="J23" s="88"/>
-      <c r="K23" s="62" t="s">
+      <c r="A23" s="80"/>
+      <c r="B23" s="81"/>
+      <c r="C23" s="81"/>
+      <c r="D23" s="81"/>
+      <c r="E23" s="81"/>
+      <c r="F23" s="81"/>
+      <c r="G23" s="81"/>
+      <c r="H23" s="81"/>
+      <c r="I23" s="81"/>
+      <c r="J23" s="81"/>
+      <c r="K23" s="59" t="s">
         <v>114</v>
       </c>
       <c r="L23" s="5"/>
       <c r="M23" s="10"/>
-      <c r="N23" s="20" t="s">
+      <c r="N23" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="O23" s="23"/>
-      <c r="P23" s="10"/>
-      <c r="Q23" s="5"/>
-      <c r="R23" s="6"/>
+      <c r="O23" s="164"/>
+      <c r="P23" s="165"/>
+      <c r="Q23" s="164"/>
+      <c r="R23" s="252"/>
     </row>
     <row r="24" spans="1:18" s="3" customFormat="1" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A24" s="60" t="s">
+      <c r="A24" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="C24" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="D24" s="29" t="s">
+      <c r="D24" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="E24" s="29" t="s">
+      <c r="E24" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="F24" s="29" t="s">
+      <c r="F24" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="G24" s="29" t="s">
+      <c r="G24" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="H24" s="27" t="s">
+      <c r="H24" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="I24" s="61" t="s">
+      <c r="I24" s="58" t="s">
         <v>84</v>
       </c>
       <c r="J24" s="4"/>
@@ -5111,308 +5120,312 @@
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
-      <c r="R24" s="74"/>
+      <c r="R24" s="70"/>
     </row>
     <row r="25" spans="1:18" s="3" customFormat="1" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A25" s="63" t="s">
+      <c r="A25" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="64" t="s">
+      <c r="B25" s="61" t="s">
         <v>95</v>
       </c>
-      <c r="C25" s="64" t="s">
+      <c r="C25" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="D25" s="65" t="s">
+      <c r="D25" s="62" t="s">
         <v>97</v>
       </c>
-      <c r="E25" s="64" t="s">
+      <c r="E25" s="61" t="s">
         <v>98</v>
       </c>
-      <c r="F25" s="64" t="s">
+      <c r="F25" s="61" t="s">
         <v>99</v>
       </c>
-      <c r="G25" s="64" t="s">
+      <c r="G25" s="61" t="s">
         <v>100</v>
       </c>
-      <c r="H25" s="66" t="s">
+      <c r="H25" s="63" t="s">
         <v>101</v>
       </c>
-      <c r="I25" s="67" t="s">
+      <c r="I25" s="64" t="s">
         <v>34</v>
       </c>
       <c r="J25" s="4"/>
-      <c r="K25" s="275" t="s">
+      <c r="K25" s="288" t="s">
         <v>148</v>
       </c>
-      <c r="L25" s="276"/>
-      <c r="M25" s="276"/>
-      <c r="N25" s="276"/>
-      <c r="O25" s="276"/>
-      <c r="P25" s="276"/>
-      <c r="Q25" s="276"/>
-      <c r="R25" s="277"/>
+      <c r="L25" s="289"/>
+      <c r="M25" s="289"/>
+      <c r="N25" s="289"/>
+      <c r="O25" s="289"/>
+      <c r="P25" s="289"/>
+      <c r="Q25" s="289"/>
+      <c r="R25" s="290"/>
     </row>
     <row r="26" spans="1:18" ht="21.75" customHeight="1">
-      <c r="A26" s="68" t="s">
+      <c r="A26" s="65" t="s">
         <v>86</v>
       </c>
-      <c r="B26" s="69"/>
-      <c r="C26" s="69"/>
-      <c r="D26" s="69"/>
-      <c r="E26" s="69"/>
-      <c r="F26" s="69"/>
-      <c r="G26" s="69"/>
-      <c r="H26" s="69"/>
-      <c r="I26" s="70"/>
-      <c r="J26" s="88"/>
-      <c r="K26" s="80" t="s">
+      <c r="B26" s="66"/>
+      <c r="C26" s="66"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="66"/>
+      <c r="F26" s="66"/>
+      <c r="G26" s="66"/>
+      <c r="H26" s="66"/>
+      <c r="I26" s="67"/>
+      <c r="J26" s="81"/>
+      <c r="K26" s="74" t="s">
         <v>120</v>
       </c>
-      <c r="L26" s="81"/>
-      <c r="M26" s="82"/>
-      <c r="N26" s="187" t="s">
+      <c r="L26" s="75"/>
+      <c r="M26" s="76"/>
+      <c r="N26" s="239" t="s">
         <v>122</v>
       </c>
-      <c r="O26" s="202"/>
-      <c r="P26" s="188"/>
-      <c r="Q26" s="202" t="s">
+      <c r="O26" s="240"/>
+      <c r="P26" s="241"/>
+      <c r="Q26" s="240" t="s">
         <v>123</v>
       </c>
-      <c r="R26" s="280"/>
+      <c r="R26" s="291"/>
     </row>
     <row r="27" spans="1:18" ht="21.75" customHeight="1">
-      <c r="A27" s="94"/>
-      <c r="B27" s="95"/>
-      <c r="C27" s="95"/>
-      <c r="D27" s="95"/>
-      <c r="E27" s="95"/>
-      <c r="F27" s="95"/>
-      <c r="G27" s="95"/>
-      <c r="H27" s="95"/>
-      <c r="I27" s="96"/>
-      <c r="J27" s="88"/>
-      <c r="K27" s="103" t="s">
+      <c r="A27" s="87"/>
+      <c r="B27" s="88"/>
+      <c r="C27" s="88"/>
+      <c r="D27" s="88"/>
+      <c r="E27" s="88"/>
+      <c r="F27" s="88"/>
+      <c r="G27" s="88"/>
+      <c r="H27" s="88"/>
+      <c r="I27" s="89"/>
+      <c r="J27" s="81"/>
+      <c r="K27" s="96" t="s">
         <v>149</v>
       </c>
-      <c r="L27" s="77"/>
-      <c r="M27" s="78"/>
-      <c r="N27" s="104"/>
-      <c r="O27" s="105"/>
-      <c r="P27" s="106"/>
-      <c r="Q27" s="105"/>
-      <c r="R27" s="107"/>
+      <c r="L27" s="72"/>
+      <c r="M27" s="73"/>
+      <c r="N27" s="203"/>
+      <c r="O27" s="306"/>
+      <c r="P27" s="204"/>
+      <c r="Q27" s="203"/>
+      <c r="R27" s="308"/>
     </row>
     <row r="28" spans="1:18" ht="21.75" customHeight="1">
-      <c r="A28" s="97"/>
-      <c r="B28" s="98"/>
-      <c r="C28" s="98"/>
-      <c r="D28" s="98"/>
-      <c r="E28" s="98"/>
-      <c r="F28" s="98"/>
-      <c r="G28" s="98"/>
-      <c r="H28" s="98"/>
-      <c r="I28" s="99"/>
-      <c r="J28" s="88"/>
-      <c r="K28" s="103" t="s">
+      <c r="A28" s="90"/>
+      <c r="B28" s="91"/>
+      <c r="C28" s="91"/>
+      <c r="D28" s="91"/>
+      <c r="E28" s="91"/>
+      <c r="F28" s="91"/>
+      <c r="G28" s="91"/>
+      <c r="H28" s="91"/>
+      <c r="I28" s="92"/>
+      <c r="J28" s="81"/>
+      <c r="K28" s="96" t="s">
         <v>121</v>
       </c>
-      <c r="L28" s="77"/>
-      <c r="M28" s="78"/>
-      <c r="N28" s="104"/>
-      <c r="O28" s="105"/>
-      <c r="P28" s="106"/>
-      <c r="Q28" s="105"/>
-      <c r="R28" s="107"/>
+      <c r="L28" s="72"/>
+      <c r="M28" s="73"/>
+      <c r="N28" s="203"/>
+      <c r="O28" s="306"/>
+      <c r="P28" s="204"/>
+      <c r="Q28" s="203"/>
+      <c r="R28" s="308"/>
     </row>
     <row r="29" spans="1:18" ht="21.75" customHeight="1">
-      <c r="A29" s="97"/>
-      <c r="B29" s="98"/>
-      <c r="C29" s="98"/>
-      <c r="D29" s="98"/>
-      <c r="E29" s="98"/>
-      <c r="F29" s="98"/>
-      <c r="G29" s="98"/>
-      <c r="H29" s="98"/>
-      <c r="I29" s="99"/>
-      <c r="J29" s="88"/>
-      <c r="K29" s="83" t="s">
+      <c r="A29" s="90"/>
+      <c r="B29" s="91"/>
+      <c r="C29" s="91"/>
+      <c r="D29" s="91"/>
+      <c r="E29" s="91"/>
+      <c r="F29" s="91"/>
+      <c r="G29" s="91"/>
+      <c r="H29" s="91"/>
+      <c r="I29" s="92"/>
+      <c r="J29" s="81"/>
+      <c r="K29" s="77" t="s">
         <v>150</v>
       </c>
-      <c r="L29" s="84"/>
-      <c r="M29" s="85"/>
-      <c r="N29" s="86"/>
-      <c r="O29" s="84"/>
-      <c r="P29" s="85"/>
-      <c r="Q29" s="84"/>
-      <c r="R29" s="72"/>
+      <c r="L29" s="78"/>
+      <c r="M29" s="79"/>
+      <c r="N29" s="203"/>
+      <c r="O29" s="306"/>
+      <c r="P29" s="204"/>
+      <c r="Q29" s="203"/>
+      <c r="R29" s="308"/>
     </row>
     <row r="30" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A30" s="97"/>
-      <c r="B30" s="98"/>
-      <c r="C30" s="98"/>
-      <c r="D30" s="98"/>
-      <c r="E30" s="98"/>
-      <c r="F30" s="98"/>
-      <c r="G30" s="98"/>
-      <c r="H30" s="98"/>
-      <c r="I30" s="99"/>
-      <c r="J30" s="88"/>
-      <c r="K30" s="108" t="s">
+      <c r="A30" s="90"/>
+      <c r="B30" s="91"/>
+      <c r="C30" s="91"/>
+      <c r="D30" s="91"/>
+      <c r="E30" s="91"/>
+      <c r="F30" s="91"/>
+      <c r="G30" s="91"/>
+      <c r="H30" s="91"/>
+      <c r="I30" s="92"/>
+      <c r="J30" s="81"/>
+      <c r="K30" s="97" t="s">
         <v>151</v>
       </c>
-      <c r="L30" s="56"/>
-      <c r="M30" s="55"/>
-      <c r="N30" s="76"/>
-      <c r="O30" s="56"/>
-      <c r="P30" s="55"/>
-      <c r="Q30" s="56"/>
-      <c r="R30" s="57"/>
+      <c r="L30" s="53"/>
+      <c r="M30" s="52"/>
+      <c r="N30" s="249"/>
+      <c r="O30" s="307"/>
+      <c r="P30" s="250"/>
+      <c r="Q30" s="249"/>
+      <c r="R30" s="309"/>
     </row>
     <row r="31" spans="1:18" ht="21.75" customHeight="1">
-      <c r="A31" s="97"/>
-      <c r="B31" s="98"/>
-      <c r="C31" s="98"/>
-      <c r="D31" s="98"/>
-      <c r="E31" s="98"/>
-      <c r="F31" s="98"/>
-      <c r="G31" s="98"/>
-      <c r="H31" s="98"/>
-      <c r="I31" s="99"/>
-      <c r="J31" s="88"/>
-      <c r="K31" s="50"/>
-      <c r="L31" s="52"/>
-      <c r="M31" s="52"/>
-      <c r="N31" s="52"/>
-      <c r="O31" s="52"/>
-      <c r="P31" s="52"/>
-      <c r="Q31" s="52"/>
-      <c r="R31" s="53"/>
+      <c r="A31" s="90"/>
+      <c r="B31" s="91"/>
+      <c r="C31" s="91"/>
+      <c r="D31" s="91"/>
+      <c r="E31" s="91"/>
+      <c r="F31" s="91"/>
+      <c r="G31" s="91"/>
+      <c r="H31" s="91"/>
+      <c r="I31" s="92"/>
+      <c r="J31" s="81"/>
+      <c r="K31" s="48"/>
+      <c r="L31" s="49"/>
+      <c r="M31" s="49"/>
+      <c r="N31" s="49"/>
+      <c r="O31" s="49"/>
+      <c r="P31" s="49"/>
+      <c r="Q31" s="49"/>
+      <c r="R31" s="50"/>
     </row>
     <row r="32" spans="1:18" ht="21.75" customHeight="1">
-      <c r="A32" s="97"/>
-      <c r="B32" s="98"/>
-      <c r="C32" s="98"/>
-      <c r="D32" s="98"/>
-      <c r="E32" s="98"/>
-      <c r="F32" s="98"/>
-      <c r="G32" s="98"/>
-      <c r="H32" s="98"/>
-      <c r="I32" s="99"/>
-      <c r="J32" s="88"/>
-      <c r="K32" s="116" t="s">
+      <c r="A32" s="90"/>
+      <c r="B32" s="91"/>
+      <c r="C32" s="91"/>
+      <c r="D32" s="91"/>
+      <c r="E32" s="91"/>
+      <c r="F32" s="91"/>
+      <c r="G32" s="91"/>
+      <c r="H32" s="91"/>
+      <c r="I32" s="92"/>
+      <c r="J32" s="81"/>
+      <c r="K32" s="105" t="s">
         <v>128</v>
       </c>
-      <c r="L32" s="88"/>
-      <c r="M32" s="281"/>
-      <c r="N32" s="281"/>
-      <c r="O32" s="281"/>
-      <c r="P32" s="281"/>
-      <c r="Q32" s="281"/>
-      <c r="R32" s="282"/>
+      <c r="L32" s="81"/>
+      <c r="M32" s="292"/>
+      <c r="N32" s="292"/>
+      <c r="O32" s="292"/>
+      <c r="P32" s="292"/>
+      <c r="Q32" s="292"/>
+      <c r="R32" s="293"/>
     </row>
     <row r="33" spans="1:18" ht="21.75" customHeight="1">
-      <c r="A33" s="97"/>
-      <c r="B33" s="98"/>
-      <c r="C33" s="98"/>
-      <c r="D33" s="98"/>
-      <c r="E33" s="98"/>
-      <c r="F33" s="98"/>
-      <c r="G33" s="98"/>
-      <c r="H33" s="98"/>
-      <c r="I33" s="99"/>
-      <c r="J33" s="88"/>
-      <c r="K33" s="87" t="s">
+      <c r="A33" s="90"/>
+      <c r="B33" s="91"/>
+      <c r="C33" s="91"/>
+      <c r="D33" s="91"/>
+      <c r="E33" s="91"/>
+      <c r="F33" s="91"/>
+      <c r="G33" s="91"/>
+      <c r="H33" s="91"/>
+      <c r="I33" s="92"/>
+      <c r="J33" s="81"/>
+      <c r="K33" s="80" t="s">
         <v>129</v>
       </c>
-      <c r="L33" s="88"/>
-      <c r="M33" s="88"/>
-      <c r="N33" s="88"/>
-      <c r="O33" s="88"/>
-      <c r="P33" s="88"/>
-      <c r="Q33" s="88"/>
-      <c r="R33" s="89"/>
+      <c r="L33" s="81"/>
+      <c r="M33" s="81"/>
+      <c r="N33" s="81"/>
+      <c r="O33" s="81"/>
+      <c r="P33" s="81"/>
+      <c r="Q33" s="81"/>
+      <c r="R33" s="82"/>
     </row>
     <row r="34" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A34" s="93"/>
-      <c r="B34" s="75"/>
-      <c r="C34" s="75"/>
-      <c r="D34" s="75"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="75"/>
-      <c r="G34" s="75"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="57"/>
-      <c r="J34" s="88"/>
-      <c r="K34" s="87" t="s">
+      <c r="A34" s="86"/>
+      <c r="B34" s="71"/>
+      <c r="C34" s="71"/>
+      <c r="D34" s="71"/>
+      <c r="E34" s="71"/>
+      <c r="F34" s="71"/>
+      <c r="G34" s="71"/>
+      <c r="H34" s="71"/>
+      <c r="I34" s="54"/>
+      <c r="J34" s="81"/>
+      <c r="K34" s="80" t="s">
         <v>130</v>
       </c>
-      <c r="L34" s="88"/>
-      <c r="M34" s="88"/>
-      <c r="N34" s="88"/>
-      <c r="O34" s="88"/>
-      <c r="P34" s="88"/>
-      <c r="Q34" s="88"/>
-      <c r="R34" s="89"/>
+      <c r="L34" s="81"/>
+      <c r="M34" s="81"/>
+      <c r="N34" s="81"/>
+      <c r="O34" s="81"/>
+      <c r="P34" s="81"/>
+      <c r="Q34" s="81"/>
+      <c r="R34" s="82"/>
     </row>
     <row r="35" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A35" s="272" t="s">
+      <c r="A35" s="285" t="s">
         <v>85</v>
       </c>
-      <c r="B35" s="273"/>
-      <c r="C35" s="273"/>
-      <c r="D35" s="274"/>
-      <c r="E35" s="75"/>
-      <c r="F35" s="75"/>
-      <c r="G35" s="75"/>
-      <c r="H35" s="75"/>
-      <c r="I35" s="57"/>
-      <c r="J35" s="88"/>
-      <c r="K35" s="54"/>
-      <c r="L35" s="56"/>
-      <c r="M35" s="56"/>
-      <c r="N35" s="56"/>
-      <c r="O35" s="56"/>
-      <c r="P35" s="56"/>
-      <c r="Q35" s="56"/>
-      <c r="R35" s="117" t="s">
+      <c r="B35" s="286"/>
+      <c r="C35" s="286"/>
+      <c r="D35" s="287"/>
+      <c r="E35" s="71"/>
+      <c r="F35" s="71"/>
+      <c r="G35" s="71"/>
+      <c r="H35" s="71"/>
+      <c r="I35" s="54"/>
+      <c r="J35" s="81"/>
+      <c r="K35" s="51"/>
+      <c r="L35" s="53"/>
+      <c r="M35" s="53"/>
+      <c r="N35" s="53"/>
+      <c r="O35" s="53"/>
+      <c r="P35" s="53"/>
+      <c r="Q35" s="53"/>
+      <c r="R35" s="106" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:18" ht="20.399999999999999">
-      <c r="A36" s="113" t="s">
+      <c r="A36" s="102" t="s">
         <v>173</v>
       </c>
-      <c r="B36" s="114"/>
-      <c r="C36" s="114"/>
-      <c r="D36" s="114"/>
-      <c r="E36" s="114"/>
-      <c r="F36" s="114"/>
-      <c r="G36" s="115"/>
-      <c r="Q36" s="270" t="s">
+      <c r="B36" s="103"/>
+      <c r="C36" s="103"/>
+      <c r="D36" s="103"/>
+      <c r="E36" s="103"/>
+      <c r="F36" s="103"/>
+      <c r="G36" s="104"/>
+      <c r="Q36" s="283" t="s">
         <v>154</v>
       </c>
-      <c r="R36" s="271"/>
+      <c r="R36" s="284"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="K4:R4"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="P9:R9"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="P10:R10"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="P11:R11"/>
+  <mergeCells count="58">
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="N27:P27"/>
+    <mergeCell ref="N28:P28"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="N30:P30"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
     <mergeCell ref="Q36:R36"/>
     <mergeCell ref="A35:D35"/>
     <mergeCell ref="K25:R25"/>
@@ -5429,6 +5442,27 @@
     <mergeCell ref="Q19:R19"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="P9:R9"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="P10:R10"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="P11:R11"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="K4:R4"/>
+    <mergeCell ref="A5:B6"/>
+    <mergeCell ref="C5:D6"/>
+    <mergeCell ref="E5:F6"/>
+    <mergeCell ref="G5:I6"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
M3 Cord Production System #973 - Implements Wet Pick up #14
</commit_message>
<xml_diff>
--- a/05.Controls/M3.Cord.Controls/Resources/Excels/FMCS11_S8.xlsx
+++ b/05.Controls/M3.Cord.Controls/Resources/Excels/FMCS11_S8.xlsx
@@ -10,7 +10,7 @@
     <sheet name="FM-CS-11" sheetId="4" r:id="rId1"/>
     <sheet name="FM-CS-11(หน้า2)" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="977461"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -780,7 +780,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="14"/>
       <name val="Cordia New"/>
@@ -941,6 +941,12 @@
       <family val="1"/>
       <charset val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <name val="Wingdings 2"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1852,7 +1858,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="310">
+  <cellXfs count="320">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1876,9 +1882,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2319,16 +2322,90 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2337,115 +2414,64 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2454,43 +2480,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2541,123 +2534,205 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2666,12 +2741,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2681,54 +2750,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2741,34 +2762,49 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3212,1149 +3248,1149 @@
   <sheetData>
     <row r="1" spans="1:47" ht="6" customHeight="1" thickBot="1"/>
     <row r="2" spans="1:47" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A2" s="228" t="s">
+      <c r="A2" s="225" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="228"/>
-      <c r="C2" s="228"/>
-      <c r="D2" s="228"/>
-      <c r="E2" s="228"/>
-      <c r="F2" s="228"/>
-      <c r="G2" s="228"/>
-      <c r="H2" s="228"/>
-      <c r="I2" s="228"/>
-      <c r="J2" s="228"/>
-      <c r="K2" s="228"/>
-      <c r="L2" s="228"/>
-      <c r="M2" s="228"/>
-      <c r="N2" s="228"/>
-      <c r="O2" s="228"/>
-      <c r="P2" s="228"/>
-      <c r="Q2" s="228"/>
-      <c r="R2" s="229"/>
-      <c r="S2" s="216" t="s">
+      <c r="B2" s="225"/>
+      <c r="C2" s="225"/>
+      <c r="D2" s="225"/>
+      <c r="E2" s="225"/>
+      <c r="F2" s="225"/>
+      <c r="G2" s="225"/>
+      <c r="H2" s="225"/>
+      <c r="I2" s="225"/>
+      <c r="J2" s="225"/>
+      <c r="K2" s="225"/>
+      <c r="L2" s="225"/>
+      <c r="M2" s="225"/>
+      <c r="N2" s="225"/>
+      <c r="O2" s="225"/>
+      <c r="P2" s="225"/>
+      <c r="Q2" s="225"/>
+      <c r="R2" s="226"/>
+      <c r="S2" s="213" t="s">
         <v>155</v>
       </c>
-      <c r="T2" s="217"/>
-      <c r="U2" s="218"/>
-      <c r="V2" s="216" t="s">
+      <c r="T2" s="214"/>
+      <c r="U2" s="215"/>
+      <c r="V2" s="213" t="s">
         <v>156</v>
       </c>
-      <c r="W2" s="217"/>
-      <c r="X2" s="218"/>
-      <c r="Z2" s="219"/>
-      <c r="AA2" s="219"/>
-      <c r="AB2" s="219"/>
-      <c r="AC2" s="219"/>
-      <c r="AD2" s="219"/>
-      <c r="AE2" s="219"/>
-      <c r="AF2" s="219"/>
-      <c r="AG2" s="219"/>
-      <c r="AH2" s="219"/>
-      <c r="AI2" s="219"/>
-      <c r="AJ2" s="219"/>
-      <c r="AK2" s="219"/>
-      <c r="AL2" s="219"/>
-      <c r="AM2" s="219"/>
-      <c r="AN2" s="219"/>
-      <c r="AO2" s="219"/>
-      <c r="AP2" s="219"/>
-      <c r="AQ2" s="219"/>
-      <c r="AR2" s="219"/>
-      <c r="AS2" s="219"/>
-      <c r="AT2" s="219"/>
-      <c r="AU2" s="219"/>
+      <c r="W2" s="214"/>
+      <c r="X2" s="215"/>
+      <c r="Z2" s="216"/>
+      <c r="AA2" s="216"/>
+      <c r="AB2" s="216"/>
+      <c r="AC2" s="216"/>
+      <c r="AD2" s="216"/>
+      <c r="AE2" s="216"/>
+      <c r="AF2" s="216"/>
+      <c r="AG2" s="216"/>
+      <c r="AH2" s="216"/>
+      <c r="AI2" s="216"/>
+      <c r="AJ2" s="216"/>
+      <c r="AK2" s="216"/>
+      <c r="AL2" s="216"/>
+      <c r="AM2" s="216"/>
+      <c r="AN2" s="216"/>
+      <c r="AO2" s="216"/>
+      <c r="AP2" s="216"/>
+      <c r="AQ2" s="216"/>
+      <c r="AR2" s="216"/>
+      <c r="AS2" s="216"/>
+      <c r="AT2" s="216"/>
+      <c r="AU2" s="216"/>
     </row>
     <row r="3" spans="1:47" ht="39.75" customHeight="1" thickBot="1">
-      <c r="A3" s="230"/>
-      <c r="B3" s="230"/>
-      <c r="C3" s="230"/>
-      <c r="D3" s="230"/>
-      <c r="E3" s="230"/>
-      <c r="F3" s="230"/>
-      <c r="G3" s="230"/>
-      <c r="H3" s="230"/>
-      <c r="I3" s="230"/>
-      <c r="J3" s="230"/>
-      <c r="K3" s="230"/>
-      <c r="L3" s="230"/>
-      <c r="M3" s="230"/>
-      <c r="N3" s="230"/>
-      <c r="O3" s="230"/>
-      <c r="P3" s="230"/>
-      <c r="Q3" s="230"/>
-      <c r="R3" s="231"/>
-      <c r="S3" s="108"/>
-      <c r="T3" s="109"/>
-      <c r="U3" s="107"/>
-      <c r="V3" s="108"/>
-      <c r="W3" s="110"/>
-      <c r="X3" s="45"/>
+      <c r="A3" s="227"/>
+      <c r="B3" s="227"/>
+      <c r="C3" s="227"/>
+      <c r="D3" s="227"/>
+      <c r="E3" s="227"/>
+      <c r="F3" s="227"/>
+      <c r="G3" s="227"/>
+      <c r="H3" s="227"/>
+      <c r="I3" s="227"/>
+      <c r="J3" s="227"/>
+      <c r="K3" s="227"/>
+      <c r="L3" s="227"/>
+      <c r="M3" s="227"/>
+      <c r="N3" s="227"/>
+      <c r="O3" s="227"/>
+      <c r="P3" s="227"/>
+      <c r="Q3" s="227"/>
+      <c r="R3" s="228"/>
+      <c r="S3" s="107"/>
+      <c r="T3" s="108"/>
+      <c r="U3" s="106"/>
+      <c r="V3" s="107"/>
+      <c r="W3" s="109"/>
+      <c r="X3" s="44"/>
     </row>
     <row r="4" spans="1:47" s="2" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A4" s="220" t="s">
+      <c r="A4" s="217" t="s">
         <v>163</v>
       </c>
-      <c r="B4" s="221"/>
-      <c r="C4" s="222" t="s">
+      <c r="B4" s="218"/>
+      <c r="C4" s="219" t="s">
         <v>164</v>
       </c>
-      <c r="D4" s="223"/>
-      <c r="E4" s="221"/>
-      <c r="F4" s="222" t="s">
+      <c r="D4" s="220"/>
+      <c r="E4" s="218"/>
+      <c r="F4" s="219" t="s">
         <v>165</v>
       </c>
-      <c r="G4" s="223"/>
-      <c r="H4" s="223"/>
-      <c r="I4" s="221"/>
-      <c r="J4" s="223" t="s">
+      <c r="G4" s="220"/>
+      <c r="H4" s="220"/>
+      <c r="I4" s="218"/>
+      <c r="J4" s="220" t="s">
         <v>166</v>
       </c>
-      <c r="K4" s="223"/>
-      <c r="L4" s="223"/>
-      <c r="M4" s="221"/>
-      <c r="N4" s="223" t="s">
+      <c r="K4" s="220"/>
+      <c r="L4" s="220"/>
+      <c r="M4" s="218"/>
+      <c r="N4" s="220" t="s">
         <v>167</v>
       </c>
-      <c r="O4" s="223"/>
-      <c r="P4" s="223"/>
-      <c r="Q4" s="221"/>
-      <c r="R4" s="224" t="s">
+      <c r="O4" s="220"/>
+      <c r="P4" s="220"/>
+      <c r="Q4" s="218"/>
+      <c r="R4" s="221" t="s">
         <v>168</v>
       </c>
-      <c r="S4" s="225"/>
-      <c r="T4" s="224" t="s">
+      <c r="S4" s="222"/>
+      <c r="T4" s="221" t="s">
         <v>169</v>
       </c>
-      <c r="U4" s="226"/>
-      <c r="V4" s="226"/>
-      <c r="W4" s="226"/>
-      <c r="X4" s="227"/>
+      <c r="U4" s="223"/>
+      <c r="V4" s="223"/>
+      <c r="W4" s="223"/>
+      <c r="X4" s="224"/>
     </row>
     <row r="5" spans="1:47" s="3" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A5" s="158"/>
-      <c r="B5" s="159"/>
-      <c r="C5" s="185"/>
-      <c r="D5" s="186"/>
-      <c r="E5" s="159"/>
-      <c r="F5" s="190"/>
-      <c r="G5" s="191"/>
-      <c r="H5" s="191"/>
-      <c r="I5" s="192"/>
-      <c r="J5" s="205" t="s">
+      <c r="A5" s="241"/>
+      <c r="B5" s="242"/>
+      <c r="C5" s="256"/>
+      <c r="D5" s="257"/>
+      <c r="E5" s="242"/>
+      <c r="F5" s="260"/>
+      <c r="G5" s="261"/>
+      <c r="H5" s="261"/>
+      <c r="I5" s="262"/>
+      <c r="J5" s="157" t="s">
         <v>140</v>
       </c>
-      <c r="K5" s="206"/>
-      <c r="L5" s="206"/>
-      <c r="M5" s="207"/>
-      <c r="N5" s="205" t="s">
+      <c r="K5" s="231"/>
+      <c r="L5" s="231"/>
+      <c r="M5" s="232"/>
+      <c r="N5" s="157" t="s">
         <v>140</v>
       </c>
-      <c r="O5" s="206"/>
-      <c r="P5" s="206"/>
-      <c r="Q5" s="207"/>
-      <c r="R5" s="42" t="s">
+      <c r="O5" s="231"/>
+      <c r="P5" s="231"/>
+      <c r="Q5" s="232"/>
+      <c r="R5" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="S5" s="16" t="s">
+      <c r="S5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="T5" s="199" t="s">
+      <c r="T5" s="229" t="s">
         <v>0</v>
       </c>
-      <c r="U5" s="200"/>
-      <c r="V5" s="205" t="s">
+      <c r="U5" s="230"/>
+      <c r="V5" s="157" t="s">
         <v>2</v>
       </c>
-      <c r="W5" s="266"/>
-      <c r="X5" s="267"/>
+      <c r="W5" s="158"/>
+      <c r="X5" s="159"/>
     </row>
     <row r="6" spans="1:47" s="3" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A6" s="160"/>
-      <c r="B6" s="161"/>
-      <c r="C6" s="187"/>
-      <c r="D6" s="188"/>
-      <c r="E6" s="161"/>
-      <c r="F6" s="193"/>
-      <c r="G6" s="194"/>
-      <c r="H6" s="194"/>
-      <c r="I6" s="195"/>
-      <c r="J6" s="175"/>
-      <c r="K6" s="176"/>
-      <c r="L6" s="176"/>
-      <c r="M6" s="177"/>
-      <c r="N6" s="210"/>
-      <c r="O6" s="211"/>
-      <c r="P6" s="211"/>
-      <c r="Q6" s="212"/>
-      <c r="R6" s="208"/>
-      <c r="S6" s="208"/>
-      <c r="T6" s="201" t="s">
+      <c r="A6" s="243"/>
+      <c r="B6" s="244"/>
+      <c r="C6" s="258"/>
+      <c r="D6" s="259"/>
+      <c r="E6" s="244"/>
+      <c r="F6" s="263"/>
+      <c r="G6" s="264"/>
+      <c r="H6" s="264"/>
+      <c r="I6" s="265"/>
+      <c r="J6" s="249"/>
+      <c r="K6" s="250"/>
+      <c r="L6" s="250"/>
+      <c r="M6" s="251"/>
+      <c r="N6" s="235"/>
+      <c r="O6" s="236"/>
+      <c r="P6" s="236"/>
+      <c r="Q6" s="237"/>
+      <c r="R6" s="233"/>
+      <c r="S6" s="233"/>
+      <c r="T6" s="209" t="s">
         <v>1</v>
       </c>
-      <c r="U6" s="202"/>
-      <c r="V6" s="168" t="s">
+      <c r="U6" s="210"/>
+      <c r="V6" s="160" t="s">
         <v>67</v>
       </c>
-      <c r="W6" s="189"/>
-      <c r="X6" s="268"/>
+      <c r="W6" s="161"/>
+      <c r="X6" s="162"/>
     </row>
     <row r="7" spans="1:47" s="3" customFormat="1" ht="21" customHeight="1">
-      <c r="A7" s="162"/>
-      <c r="B7" s="163"/>
-      <c r="C7" s="168"/>
-      <c r="D7" s="189"/>
-      <c r="E7" s="163"/>
-      <c r="F7" s="196"/>
-      <c r="G7" s="197"/>
-      <c r="H7" s="197"/>
-      <c r="I7" s="198"/>
-      <c r="J7" s="178"/>
-      <c r="K7" s="179"/>
-      <c r="L7" s="179"/>
-      <c r="M7" s="180"/>
-      <c r="N7" s="213"/>
-      <c r="O7" s="214"/>
-      <c r="P7" s="214"/>
-      <c r="Q7" s="215"/>
-      <c r="R7" s="209"/>
-      <c r="S7" s="209"/>
-      <c r="T7" s="203" t="s">
+      <c r="A7" s="187"/>
+      <c r="B7" s="188"/>
+      <c r="C7" s="160"/>
+      <c r="D7" s="161"/>
+      <c r="E7" s="188"/>
+      <c r="F7" s="266"/>
+      <c r="G7" s="267"/>
+      <c r="H7" s="267"/>
+      <c r="I7" s="268"/>
+      <c r="J7" s="252"/>
+      <c r="K7" s="253"/>
+      <c r="L7" s="253"/>
+      <c r="M7" s="254"/>
+      <c r="N7" s="238"/>
+      <c r="O7" s="239"/>
+      <c r="P7" s="239"/>
+      <c r="Q7" s="240"/>
+      <c r="R7" s="234"/>
+      <c r="S7" s="234"/>
+      <c r="T7" s="207" t="s">
         <v>3</v>
       </c>
-      <c r="U7" s="204"/>
-      <c r="V7" s="173"/>
-      <c r="W7" s="174"/>
-      <c r="X7" s="269"/>
+      <c r="U7" s="208"/>
+      <c r="V7" s="163"/>
+      <c r="W7" s="164"/>
+      <c r="X7" s="165"/>
     </row>
     <row r="8" spans="1:47" s="3" customFormat="1" ht="19.8">
-      <c r="A8" s="171" t="s">
+      <c r="A8" s="248" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="172"/>
-      <c r="C8" s="173" t="s">
+      <c r="B8" s="206"/>
+      <c r="C8" s="163" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="174"/>
-      <c r="E8" s="172"/>
-      <c r="F8" s="173" t="s">
+      <c r="D8" s="164"/>
+      <c r="E8" s="206"/>
+      <c r="F8" s="163" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="172"/>
-      <c r="H8" s="173" t="s">
+      <c r="G8" s="206"/>
+      <c r="H8" s="163" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="172"/>
-      <c r="J8" s="174" t="s">
+      <c r="I8" s="206"/>
+      <c r="J8" s="164" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="174"/>
-      <c r="L8" s="174"/>
-      <c r="M8" s="172"/>
-      <c r="N8" s="174" t="s">
+      <c r="K8" s="164"/>
+      <c r="L8" s="164"/>
+      <c r="M8" s="206"/>
+      <c r="N8" s="164" t="s">
         <v>19</v>
       </c>
-      <c r="O8" s="174"/>
-      <c r="P8" s="174"/>
-      <c r="Q8" s="172"/>
-      <c r="R8" s="232" t="s">
+      <c r="O8" s="164"/>
+      <c r="P8" s="164"/>
+      <c r="Q8" s="206"/>
+      <c r="R8" s="211" t="s">
         <v>7</v>
       </c>
-      <c r="S8" s="233"/>
-      <c r="T8" s="203" t="s">
+      <c r="S8" s="212"/>
+      <c r="T8" s="207" t="s">
         <v>4</v>
       </c>
-      <c r="U8" s="204"/>
-      <c r="V8" s="173"/>
-      <c r="W8" s="174"/>
-      <c r="X8" s="269"/>
+      <c r="U8" s="208"/>
+      <c r="V8" s="163"/>
+      <c r="W8" s="164"/>
+      <c r="X8" s="165"/>
     </row>
     <row r="9" spans="1:47" s="3" customFormat="1" ht="21" customHeight="1">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="166"/>
-      <c r="D9" s="181"/>
-      <c r="E9" s="167"/>
-      <c r="F9" s="245"/>
-      <c r="G9" s="246"/>
-      <c r="H9" s="181"/>
-      <c r="I9" s="167"/>
-      <c r="J9" s="173" t="s">
+      <c r="C9" s="245"/>
+      <c r="D9" s="201"/>
+      <c r="E9" s="186"/>
+      <c r="F9" s="197"/>
+      <c r="G9" s="198"/>
+      <c r="H9" s="201"/>
+      <c r="I9" s="186"/>
+      <c r="J9" s="163" t="s">
         <v>17</v>
       </c>
-      <c r="K9" s="172"/>
-      <c r="L9" s="174" t="s">
+      <c r="K9" s="206"/>
+      <c r="L9" s="164" t="s">
         <v>18</v>
       </c>
-      <c r="M9" s="172"/>
-      <c r="N9" s="173" t="s">
+      <c r="M9" s="206"/>
+      <c r="N9" s="163" t="s">
         <v>17</v>
       </c>
-      <c r="O9" s="172"/>
-      <c r="P9" s="174" t="s">
+      <c r="O9" s="206"/>
+      <c r="P9" s="164" t="s">
         <v>18</v>
       </c>
-      <c r="Q9" s="172"/>
-      <c r="R9" s="201" t="s">
+      <c r="Q9" s="206"/>
+      <c r="R9" s="209" t="s">
         <v>8</v>
       </c>
-      <c r="S9" s="202"/>
-      <c r="T9" s="203" t="s">
+      <c r="S9" s="210"/>
+      <c r="T9" s="207" t="s">
         <v>5</v>
       </c>
-      <c r="U9" s="204"/>
-      <c r="V9" s="173"/>
-      <c r="W9" s="174"/>
-      <c r="X9" s="269"/>
+      <c r="U9" s="208"/>
+      <c r="V9" s="163"/>
+      <c r="W9" s="164"/>
+      <c r="X9" s="165"/>
     </row>
     <row r="10" spans="1:47" s="3" customFormat="1" ht="29.25" customHeight="1" thickBot="1">
-      <c r="A10" s="156"/>
-      <c r="B10" s="157"/>
-      <c r="C10" s="182"/>
-      <c r="D10" s="183"/>
-      <c r="E10" s="184"/>
-      <c r="F10" s="247"/>
-      <c r="G10" s="248"/>
-      <c r="H10" s="183"/>
-      <c r="I10" s="184"/>
-      <c r="J10" s="164"/>
-      <c r="K10" s="165"/>
-      <c r="L10" s="164"/>
-      <c r="M10" s="165"/>
-      <c r="N10" s="164"/>
-      <c r="O10" s="165"/>
-      <c r="P10" s="164"/>
-      <c r="Q10" s="165"/>
-      <c r="R10" s="249"/>
-      <c r="S10" s="250"/>
-      <c r="T10" s="237" t="s">
+      <c r="A10" s="155"/>
+      <c r="B10" s="156"/>
+      <c r="C10" s="255"/>
+      <c r="D10" s="202"/>
+      <c r="E10" s="203"/>
+      <c r="F10" s="199"/>
+      <c r="G10" s="200"/>
+      <c r="H10" s="202"/>
+      <c r="I10" s="203"/>
+      <c r="J10" s="166"/>
+      <c r="K10" s="189"/>
+      <c r="L10" s="166"/>
+      <c r="M10" s="189"/>
+      <c r="N10" s="166"/>
+      <c r="O10" s="189"/>
+      <c r="P10" s="166"/>
+      <c r="Q10" s="189"/>
+      <c r="R10" s="204"/>
+      <c r="S10" s="205"/>
+      <c r="T10" s="191" t="s">
         <v>20</v>
       </c>
-      <c r="U10" s="238"/>
-      <c r="V10" s="164"/>
-      <c r="W10" s="251"/>
-      <c r="X10" s="252"/>
+      <c r="U10" s="192"/>
+      <c r="V10" s="166"/>
+      <c r="W10" s="167"/>
+      <c r="X10" s="168"/>
     </row>
     <row r="11" spans="1:47" s="3" customFormat="1" ht="9.75" customHeight="1" thickBot="1"/>
     <row r="12" spans="1:47" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A12" s="135" t="s">
+      <c r="A12" s="134" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="137" t="s">
+      <c r="B12" s="136" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="239" t="s">
+      <c r="C12" s="177" t="s">
         <v>72</v>
       </c>
-      <c r="D12" s="240"/>
-      <c r="E12" s="241"/>
-      <c r="F12" s="239" t="s">
+      <c r="D12" s="193"/>
+      <c r="E12" s="178"/>
+      <c r="F12" s="177" t="s">
         <v>71</v>
       </c>
-      <c r="G12" s="241"/>
-      <c r="H12" s="142" t="s">
+      <c r="G12" s="178"/>
+      <c r="H12" s="141" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="142" t="s">
+      <c r="I12" s="141" t="s">
         <v>55</v>
       </c>
-      <c r="J12" s="142" t="s">
+      <c r="J12" s="141" t="s">
         <v>50</v>
       </c>
-      <c r="K12" s="142" t="s">
+      <c r="K12" s="141" t="s">
         <v>57</v>
       </c>
-      <c r="L12" s="137" t="s">
+      <c r="L12" s="136" t="s">
         <v>23</v>
       </c>
-      <c r="M12" s="239" t="s">
+      <c r="M12" s="177" t="s">
         <v>70</v>
       </c>
-      <c r="N12" s="240"/>
-      <c r="O12" s="241"/>
-      <c r="P12" s="239" t="s">
+      <c r="N12" s="193"/>
+      <c r="O12" s="178"/>
+      <c r="P12" s="177" t="s">
         <v>69</v>
       </c>
-      <c r="Q12" s="240"/>
-      <c r="R12" s="240"/>
-      <c r="S12" s="241"/>
-      <c r="T12" s="242" t="s">
+      <c r="Q12" s="193"/>
+      <c r="R12" s="193"/>
+      <c r="S12" s="178"/>
+      <c r="T12" s="194" t="s">
         <v>60</v>
       </c>
-      <c r="U12" s="243"/>
-      <c r="V12" s="244"/>
-      <c r="W12" s="140" t="s">
+      <c r="U12" s="195"/>
+      <c r="V12" s="196"/>
+      <c r="W12" s="139" t="s">
         <v>32</v>
       </c>
-      <c r="X12" s="141" t="s">
+      <c r="X12" s="140" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:47" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A13" s="136"/>
-      <c r="B13" s="138" t="s">
+      <c r="A13" s="135"/>
+      <c r="B13" s="137" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="D13" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="26" t="s">
+      <c r="E13" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="26" t="s">
+      <c r="F13" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="G13" s="26" t="s">
+      <c r="G13" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="28" t="s">
+      <c r="H13" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="I13" s="28" t="s">
+      <c r="I13" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="J13" s="28" t="s">
+      <c r="J13" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="K13" s="28" t="s">
+      <c r="K13" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="L13" s="28" t="s">
+      <c r="L13" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="M13" s="28" t="s">
+      <c r="M13" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="N13" s="28" t="s">
+      <c r="N13" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="O13" s="28" t="s">
+      <c r="O13" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="P13" s="26" t="s">
+      <c r="P13" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="Q13" s="26" t="s">
+      <c r="Q13" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="R13" s="26" t="s">
+      <c r="R13" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="S13" s="28" t="s">
+      <c r="S13" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="T13" s="28" t="s">
+      <c r="T13" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="U13" s="28" t="s">
+      <c r="U13" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="V13" s="28" t="s">
+      <c r="V13" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="W13" s="28" t="s">
+      <c r="W13" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="X13" s="24" t="s">
+      <c r="X13" s="23" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:47" s="3" customFormat="1" ht="24.75" customHeight="1" thickBot="1">
-      <c r="A14" s="126" t="s">
+      <c r="A14" s="125" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="139" t="s">
+      <c r="B14" s="138" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="93" t="s">
+      <c r="C14" s="92" t="s">
         <v>135</v>
       </c>
-      <c r="D14" s="93" t="s">
+      <c r="D14" s="92" t="s">
         <v>136</v>
       </c>
-      <c r="E14" s="93" t="s">
+      <c r="E14" s="92" t="s">
         <v>137</v>
       </c>
-      <c r="F14" s="93" t="s">
+      <c r="F14" s="92" t="s">
         <v>135</v>
       </c>
-      <c r="G14" s="31" t="s">
+      <c r="G14" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="H14" s="29" t="s">
+      <c r="H14" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="I14" s="29" t="s">
+      <c r="I14" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="J14" s="29" t="s">
+      <c r="J14" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="K14" s="29" t="s">
+      <c r="K14" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="L14" s="29" t="s">
+      <c r="L14" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="M14" s="29" t="s">
+      <c r="M14" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="N14" s="29" t="s">
+      <c r="N14" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="O14" s="30" t="s">
+      <c r="O14" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="P14" s="29" t="s">
+      <c r="P14" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="Q14" s="29" t="s">
+      <c r="Q14" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="R14" s="31" t="s">
+      <c r="R14" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="S14" s="31" t="s">
+      <c r="S14" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="T14" s="29" t="s">
+      <c r="T14" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="U14" s="29" t="s">
+      <c r="U14" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="V14" s="29" t="s">
+      <c r="V14" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="W14" s="15"/>
+      <c r="W14" s="14"/>
       <c r="X14" s="6"/>
     </row>
     <row r="15" spans="1:47" s="3" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A15" s="136"/>
-      <c r="B15" s="138"/>
-      <c r="C15" s="146"/>
-      <c r="D15" s="146"/>
-      <c r="E15" s="146"/>
-      <c r="F15" s="146"/>
-      <c r="G15" s="146"/>
-      <c r="H15" s="146"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
-      <c r="O15" s="144"/>
-      <c r="P15" s="28"/>
-      <c r="Q15" s="28"/>
-      <c r="R15" s="143"/>
-      <c r="S15" s="143"/>
-      <c r="T15" s="28"/>
-      <c r="U15" s="28"/>
-      <c r="V15" s="28"/>
-      <c r="W15" s="145"/>
-      <c r="X15" s="70"/>
+      <c r="A15" s="135"/>
+      <c r="B15" s="137"/>
+      <c r="C15" s="145"/>
+      <c r="D15" s="145"/>
+      <c r="E15" s="145"/>
+      <c r="F15" s="145"/>
+      <c r="G15" s="145"/>
+      <c r="H15" s="145"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="27"/>
+      <c r="O15" s="143"/>
+      <c r="P15" s="27"/>
+      <c r="Q15" s="27"/>
+      <c r="R15" s="142"/>
+      <c r="S15" s="142"/>
+      <c r="T15" s="27"/>
+      <c r="U15" s="27"/>
+      <c r="V15" s="27"/>
+      <c r="W15" s="144"/>
+      <c r="X15" s="69"/>
     </row>
     <row r="16" spans="1:47" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A16" s="150"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="154"/>
-      <c r="D16" s="154"/>
-      <c r="E16" s="154"/>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="155"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="14"/>
-      <c r="T16" s="14"/>
-      <c r="U16" s="14"/>
-      <c r="V16" s="14"/>
-      <c r="W16" s="14"/>
-      <c r="X16" s="128"/>
+      <c r="A16" s="149"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="153"/>
+      <c r="D16" s="153"/>
+      <c r="E16" s="153"/>
+      <c r="F16" s="153"/>
+      <c r="G16" s="153"/>
+      <c r="H16" s="154"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="13"/>
+      <c r="S16" s="13"/>
+      <c r="T16" s="13"/>
+      <c r="U16" s="13"/>
+      <c r="V16" s="13"/>
+      <c r="W16" s="13"/>
+      <c r="X16" s="127"/>
     </row>
     <row r="17" spans="1:24" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A17" s="153" t="s">
+      <c r="A17" s="152" t="s">
         <v>134</v>
       </c>
-      <c r="B17" s="151"/>
-      <c r="C17" s="151"/>
-      <c r="D17" s="151"/>
-      <c r="E17" s="151"/>
-      <c r="F17" s="151"/>
-      <c r="G17" s="151"/>
-      <c r="H17" s="151"/>
-      <c r="I17" s="151"/>
-      <c r="J17" s="151"/>
-      <c r="K17" s="151"/>
-      <c r="L17" s="151"/>
-      <c r="M17" s="151"/>
-      <c r="N17" s="151"/>
-      <c r="O17" s="151"/>
-      <c r="P17" s="151"/>
-      <c r="Q17" s="151"/>
-      <c r="R17" s="151"/>
-      <c r="S17" s="151"/>
-      <c r="T17" s="151"/>
-      <c r="U17" s="151"/>
-      <c r="V17" s="151"/>
-      <c r="W17" s="151"/>
-      <c r="X17" s="152"/>
+      <c r="B17" s="150"/>
+      <c r="C17" s="150"/>
+      <c r="D17" s="150"/>
+      <c r="E17" s="150"/>
+      <c r="F17" s="150"/>
+      <c r="G17" s="150"/>
+      <c r="H17" s="150"/>
+      <c r="I17" s="150"/>
+      <c r="J17" s="150"/>
+      <c r="K17" s="150"/>
+      <c r="L17" s="150"/>
+      <c r="M17" s="150"/>
+      <c r="N17" s="150"/>
+      <c r="O17" s="150"/>
+      <c r="P17" s="150"/>
+      <c r="Q17" s="150"/>
+      <c r="R17" s="150"/>
+      <c r="S17" s="150"/>
+      <c r="T17" s="150"/>
+      <c r="U17" s="150"/>
+      <c r="V17" s="150"/>
+      <c r="W17" s="150"/>
+      <c r="X17" s="151"/>
     </row>
     <row r="18" spans="1:24" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A18" s="147"/>
-      <c r="B18" s="148"/>
-      <c r="C18" s="148"/>
-      <c r="D18" s="148"/>
-      <c r="E18" s="148"/>
-      <c r="F18" s="148"/>
-      <c r="G18" s="148"/>
-      <c r="H18" s="148"/>
-      <c r="I18" s="148"/>
-      <c r="J18" s="148"/>
-      <c r="K18" s="148"/>
-      <c r="L18" s="148"/>
-      <c r="M18" s="148"/>
-      <c r="N18" s="148"/>
-      <c r="O18" s="148"/>
-      <c r="P18" s="148"/>
-      <c r="Q18" s="148"/>
-      <c r="R18" s="148"/>
-      <c r="S18" s="148"/>
-      <c r="T18" s="148"/>
-      <c r="U18" s="148"/>
-      <c r="V18" s="148"/>
-      <c r="W18" s="148"/>
-      <c r="X18" s="149"/>
+      <c r="A18" s="146"/>
+      <c r="B18" s="147"/>
+      <c r="C18" s="147"/>
+      <c r="D18" s="147"/>
+      <c r="E18" s="147"/>
+      <c r="F18" s="147"/>
+      <c r="G18" s="147"/>
+      <c r="H18" s="147"/>
+      <c r="I18" s="147"/>
+      <c r="J18" s="147"/>
+      <c r="K18" s="147"/>
+      <c r="L18" s="147"/>
+      <c r="M18" s="147"/>
+      <c r="N18" s="147"/>
+      <c r="O18" s="147"/>
+      <c r="P18" s="147"/>
+      <c r="Q18" s="147"/>
+      <c r="R18" s="147"/>
+      <c r="S18" s="147"/>
+      <c r="T18" s="147"/>
+      <c r="U18" s="147"/>
+      <c r="V18" s="147"/>
+      <c r="W18" s="147"/>
+      <c r="X18" s="148"/>
     </row>
     <row r="19" spans="1:24" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A19" s="83"/>
-      <c r="B19" s="84"/>
-      <c r="C19" s="84"/>
-      <c r="D19" s="84"/>
-      <c r="E19" s="84"/>
-      <c r="F19" s="84"/>
-      <c r="G19" s="84"/>
-      <c r="H19" s="84"/>
-      <c r="I19" s="84"/>
-      <c r="J19" s="84"/>
-      <c r="K19" s="84"/>
-      <c r="L19" s="84"/>
-      <c r="M19" s="84"/>
-      <c r="N19" s="84"/>
-      <c r="O19" s="84"/>
-      <c r="P19" s="84"/>
-      <c r="Q19" s="84"/>
-      <c r="R19" s="84"/>
-      <c r="S19" s="84"/>
-      <c r="T19" s="84"/>
-      <c r="U19" s="84"/>
-      <c r="V19" s="84"/>
-      <c r="W19" s="84"/>
-      <c r="X19" s="85"/>
+      <c r="A19" s="82"/>
+      <c r="B19" s="83"/>
+      <c r="C19" s="83"/>
+      <c r="D19" s="83"/>
+      <c r="E19" s="83"/>
+      <c r="F19" s="83"/>
+      <c r="G19" s="83"/>
+      <c r="H19" s="83"/>
+      <c r="I19" s="83"/>
+      <c r="J19" s="83"/>
+      <c r="K19" s="83"/>
+      <c r="L19" s="83"/>
+      <c r="M19" s="83"/>
+      <c r="N19" s="83"/>
+      <c r="O19" s="83"/>
+      <c r="P19" s="83"/>
+      <c r="Q19" s="83"/>
+      <c r="R19" s="83"/>
+      <c r="S19" s="83"/>
+      <c r="T19" s="83"/>
+      <c r="U19" s="83"/>
+      <c r="V19" s="83"/>
+      <c r="W19" s="83"/>
+      <c r="X19" s="84"/>
     </row>
     <row r="20" spans="1:24" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A20" s="83"/>
-      <c r="B20" s="84"/>
-      <c r="C20" s="84"/>
-      <c r="D20" s="84"/>
-      <c r="E20" s="84"/>
-      <c r="F20" s="84"/>
-      <c r="G20" s="84"/>
-      <c r="H20" s="84"/>
-      <c r="I20" s="84"/>
-      <c r="J20" s="84"/>
-      <c r="K20" s="84"/>
-      <c r="L20" s="84"/>
-      <c r="M20" s="84"/>
-      <c r="N20" s="84"/>
-      <c r="O20" s="84"/>
-      <c r="P20" s="84"/>
-      <c r="Q20" s="84"/>
-      <c r="R20" s="84"/>
-      <c r="S20" s="84"/>
-      <c r="T20" s="84"/>
-      <c r="U20" s="84"/>
-      <c r="V20" s="84"/>
-      <c r="W20" s="84"/>
-      <c r="X20" s="85"/>
+      <c r="A20" s="82"/>
+      <c r="B20" s="83"/>
+      <c r="C20" s="83"/>
+      <c r="D20" s="83"/>
+      <c r="E20" s="83"/>
+      <c r="F20" s="83"/>
+      <c r="G20" s="83"/>
+      <c r="H20" s="83"/>
+      <c r="I20" s="83"/>
+      <c r="J20" s="83"/>
+      <c r="K20" s="83"/>
+      <c r="L20" s="83"/>
+      <c r="M20" s="83"/>
+      <c r="N20" s="83"/>
+      <c r="O20" s="83"/>
+      <c r="P20" s="83"/>
+      <c r="Q20" s="83"/>
+      <c r="R20" s="83"/>
+      <c r="S20" s="83"/>
+      <c r="T20" s="83"/>
+      <c r="U20" s="83"/>
+      <c r="V20" s="83"/>
+      <c r="W20" s="83"/>
+      <c r="X20" s="84"/>
     </row>
     <row r="21" spans="1:24" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A21" s="83"/>
-      <c r="B21" s="84"/>
-      <c r="C21" s="84"/>
-      <c r="D21" s="84"/>
-      <c r="E21" s="84"/>
-      <c r="F21" s="84"/>
-      <c r="G21" s="84"/>
-      <c r="H21" s="84"/>
-      <c r="I21" s="84"/>
-      <c r="J21" s="84"/>
-      <c r="K21" s="84"/>
-      <c r="L21" s="84"/>
-      <c r="M21" s="84"/>
-      <c r="N21" s="84"/>
-      <c r="O21" s="84"/>
-      <c r="P21" s="84"/>
-      <c r="Q21" s="84"/>
-      <c r="R21" s="84"/>
-      <c r="S21" s="84"/>
-      <c r="T21" s="84"/>
-      <c r="U21" s="84"/>
-      <c r="V21" s="84"/>
-      <c r="W21" s="84"/>
-      <c r="X21" s="85"/>
+      <c r="A21" s="82"/>
+      <c r="B21" s="83"/>
+      <c r="C21" s="83"/>
+      <c r="D21" s="83"/>
+      <c r="E21" s="83"/>
+      <c r="F21" s="83"/>
+      <c r="G21" s="83"/>
+      <c r="H21" s="83"/>
+      <c r="I21" s="83"/>
+      <c r="J21" s="83"/>
+      <c r="K21" s="83"/>
+      <c r="L21" s="83"/>
+      <c r="M21" s="83"/>
+      <c r="N21" s="83"/>
+      <c r="O21" s="83"/>
+      <c r="P21" s="83"/>
+      <c r="Q21" s="83"/>
+      <c r="R21" s="83"/>
+      <c r="S21" s="83"/>
+      <c r="T21" s="83"/>
+      <c r="U21" s="83"/>
+      <c r="V21" s="83"/>
+      <c r="W21" s="83"/>
+      <c r="X21" s="84"/>
     </row>
     <row r="22" spans="1:24" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A22" s="83"/>
-      <c r="B22" s="84"/>
-      <c r="C22" s="84"/>
-      <c r="D22" s="84"/>
-      <c r="E22" s="84"/>
-      <c r="F22" s="84"/>
-      <c r="G22" s="84"/>
-      <c r="H22" s="84"/>
-      <c r="I22" s="84"/>
-      <c r="J22" s="84"/>
-      <c r="K22" s="84"/>
-      <c r="L22" s="84"/>
-      <c r="M22" s="84"/>
-      <c r="N22" s="84"/>
-      <c r="O22" s="84"/>
-      <c r="P22" s="84"/>
-      <c r="Q22" s="84"/>
-      <c r="R22" s="84"/>
-      <c r="S22" s="84"/>
-      <c r="T22" s="84"/>
-      <c r="U22" s="84"/>
-      <c r="V22" s="84"/>
-      <c r="W22" s="84"/>
-      <c r="X22" s="85"/>
+      <c r="A22" s="82"/>
+      <c r="B22" s="83"/>
+      <c r="C22" s="83"/>
+      <c r="D22" s="83"/>
+      <c r="E22" s="83"/>
+      <c r="F22" s="83"/>
+      <c r="G22" s="83"/>
+      <c r="H22" s="83"/>
+      <c r="I22" s="83"/>
+      <c r="J22" s="83"/>
+      <c r="K22" s="83"/>
+      <c r="L22" s="83"/>
+      <c r="M22" s="83"/>
+      <c r="N22" s="83"/>
+      <c r="O22" s="83"/>
+      <c r="P22" s="83"/>
+      <c r="Q22" s="83"/>
+      <c r="R22" s="83"/>
+      <c r="S22" s="83"/>
+      <c r="T22" s="83"/>
+      <c r="U22" s="83"/>
+      <c r="V22" s="83"/>
+      <c r="W22" s="83"/>
+      <c r="X22" s="84"/>
     </row>
     <row r="23" spans="1:24" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A23" s="83"/>
-      <c r="B23" s="84"/>
-      <c r="C23" s="84"/>
-      <c r="D23" s="84"/>
-      <c r="E23" s="84"/>
-      <c r="F23" s="84"/>
-      <c r="G23" s="84"/>
-      <c r="H23" s="84"/>
-      <c r="I23" s="84"/>
-      <c r="J23" s="84"/>
-      <c r="K23" s="84"/>
-      <c r="L23" s="84"/>
-      <c r="M23" s="84"/>
-      <c r="N23" s="84"/>
-      <c r="O23" s="84"/>
-      <c r="P23" s="84"/>
-      <c r="Q23" s="84"/>
-      <c r="R23" s="84"/>
-      <c r="S23" s="84"/>
-      <c r="T23" s="84"/>
-      <c r="U23" s="84"/>
-      <c r="V23" s="84"/>
-      <c r="W23" s="84"/>
-      <c r="X23" s="85"/>
+      <c r="A23" s="82"/>
+      <c r="B23" s="83"/>
+      <c r="C23" s="83"/>
+      <c r="D23" s="83"/>
+      <c r="E23" s="83"/>
+      <c r="F23" s="83"/>
+      <c r="G23" s="83"/>
+      <c r="H23" s="83"/>
+      <c r="I23" s="83"/>
+      <c r="J23" s="83"/>
+      <c r="K23" s="83"/>
+      <c r="L23" s="83"/>
+      <c r="M23" s="83"/>
+      <c r="N23" s="83"/>
+      <c r="O23" s="83"/>
+      <c r="P23" s="83"/>
+      <c r="Q23" s="83"/>
+      <c r="R23" s="83"/>
+      <c r="S23" s="83"/>
+      <c r="T23" s="83"/>
+      <c r="U23" s="83"/>
+      <c r="V23" s="83"/>
+      <c r="W23" s="83"/>
+      <c r="X23" s="84"/>
     </row>
     <row r="24" spans="1:24" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A24" s="83"/>
-      <c r="B24" s="84"/>
-      <c r="C24" s="84"/>
-      <c r="D24" s="84"/>
-      <c r="E24" s="84"/>
-      <c r="F24" s="84"/>
-      <c r="G24" s="84"/>
-      <c r="H24" s="84"/>
-      <c r="I24" s="84"/>
-      <c r="J24" s="84"/>
-      <c r="K24" s="84"/>
-      <c r="L24" s="84"/>
-      <c r="M24" s="84"/>
-      <c r="N24" s="84"/>
-      <c r="O24" s="84"/>
-      <c r="P24" s="84"/>
-      <c r="Q24" s="84"/>
-      <c r="R24" s="84"/>
-      <c r="S24" s="84"/>
-      <c r="T24" s="84"/>
-      <c r="U24" s="84"/>
-      <c r="V24" s="84"/>
-      <c r="W24" s="84"/>
-      <c r="X24" s="85"/>
+      <c r="A24" s="82"/>
+      <c r="B24" s="83"/>
+      <c r="C24" s="83"/>
+      <c r="D24" s="83"/>
+      <c r="E24" s="83"/>
+      <c r="F24" s="83"/>
+      <c r="G24" s="83"/>
+      <c r="H24" s="83"/>
+      <c r="I24" s="83"/>
+      <c r="J24" s="83"/>
+      <c r="K24" s="83"/>
+      <c r="L24" s="83"/>
+      <c r="M24" s="83"/>
+      <c r="N24" s="83"/>
+      <c r="O24" s="83"/>
+      <c r="P24" s="83"/>
+      <c r="Q24" s="83"/>
+      <c r="R24" s="83"/>
+      <c r="S24" s="83"/>
+      <c r="T24" s="83"/>
+      <c r="U24" s="83"/>
+      <c r="V24" s="83"/>
+      <c r="W24" s="83"/>
+      <c r="X24" s="84"/>
     </row>
     <row r="25" spans="1:24" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A25" s="83"/>
-      <c r="B25" s="84"/>
-      <c r="C25" s="84"/>
-      <c r="D25" s="84"/>
-      <c r="E25" s="84"/>
-      <c r="F25" s="84"/>
-      <c r="G25" s="84"/>
-      <c r="H25" s="84"/>
-      <c r="I25" s="84"/>
-      <c r="J25" s="84"/>
-      <c r="K25" s="84"/>
-      <c r="L25" s="84"/>
-      <c r="M25" s="84"/>
-      <c r="N25" s="84"/>
-      <c r="O25" s="84"/>
-      <c r="P25" s="84"/>
-      <c r="Q25" s="84"/>
-      <c r="R25" s="84"/>
-      <c r="S25" s="84"/>
-      <c r="T25" s="84"/>
-      <c r="U25" s="84"/>
-      <c r="V25" s="84"/>
-      <c r="W25" s="84"/>
-      <c r="X25" s="85"/>
+      <c r="A25" s="82"/>
+      <c r="B25" s="83"/>
+      <c r="C25" s="83"/>
+      <c r="D25" s="83"/>
+      <c r="E25" s="83"/>
+      <c r="F25" s="83"/>
+      <c r="G25" s="83"/>
+      <c r="H25" s="83"/>
+      <c r="I25" s="83"/>
+      <c r="J25" s="83"/>
+      <c r="K25" s="83"/>
+      <c r="L25" s="83"/>
+      <c r="M25" s="83"/>
+      <c r="N25" s="83"/>
+      <c r="O25" s="83"/>
+      <c r="P25" s="83"/>
+      <c r="Q25" s="83"/>
+      <c r="R25" s="83"/>
+      <c r="S25" s="83"/>
+      <c r="T25" s="83"/>
+      <c r="U25" s="83"/>
+      <c r="V25" s="83"/>
+      <c r="W25" s="83"/>
+      <c r="X25" s="84"/>
     </row>
     <row r="26" spans="1:24" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A26" s="83"/>
-      <c r="B26" s="84"/>
-      <c r="C26" s="84"/>
-      <c r="D26" s="84"/>
-      <c r="E26" s="84"/>
-      <c r="F26" s="84"/>
-      <c r="G26" s="84"/>
-      <c r="H26" s="84"/>
-      <c r="I26" s="84"/>
-      <c r="J26" s="84"/>
-      <c r="K26" s="84"/>
-      <c r="L26" s="84"/>
-      <c r="M26" s="84"/>
-      <c r="N26" s="84"/>
-      <c r="O26" s="84"/>
-      <c r="P26" s="84"/>
-      <c r="Q26" s="84"/>
-      <c r="R26" s="84"/>
-      <c r="S26" s="84"/>
-      <c r="T26" s="84"/>
-      <c r="U26" s="84"/>
-      <c r="V26" s="84"/>
-      <c r="W26" s="84"/>
-      <c r="X26" s="85"/>
+      <c r="A26" s="82"/>
+      <c r="B26" s="83"/>
+      <c r="C26" s="83"/>
+      <c r="D26" s="83"/>
+      <c r="E26" s="83"/>
+      <c r="F26" s="83"/>
+      <c r="G26" s="83"/>
+      <c r="H26" s="83"/>
+      <c r="I26" s="83"/>
+      <c r="J26" s="83"/>
+      <c r="K26" s="83"/>
+      <c r="L26" s="83"/>
+      <c r="M26" s="83"/>
+      <c r="N26" s="83"/>
+      <c r="O26" s="83"/>
+      <c r="P26" s="83"/>
+      <c r="Q26" s="83"/>
+      <c r="R26" s="83"/>
+      <c r="S26" s="83"/>
+      <c r="T26" s="83"/>
+      <c r="U26" s="83"/>
+      <c r="V26" s="83"/>
+      <c r="W26" s="83"/>
+      <c r="X26" s="84"/>
     </row>
     <row r="27" spans="1:24" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A27" s="83"/>
-      <c r="B27" s="84"/>
-      <c r="C27" s="84"/>
-      <c r="D27" s="84"/>
-      <c r="E27" s="84"/>
-      <c r="F27" s="84"/>
-      <c r="G27" s="84"/>
-      <c r="H27" s="84"/>
-      <c r="I27" s="84"/>
-      <c r="J27" s="84"/>
-      <c r="K27" s="84"/>
-      <c r="L27" s="84"/>
-      <c r="M27" s="84"/>
-      <c r="N27" s="84"/>
-      <c r="O27" s="84"/>
-      <c r="P27" s="84"/>
-      <c r="Q27" s="84"/>
-      <c r="R27" s="84"/>
-      <c r="S27" s="84"/>
-      <c r="T27" s="84"/>
-      <c r="U27" s="84"/>
-      <c r="V27" s="84"/>
-      <c r="W27" s="84"/>
-      <c r="X27" s="85"/>
+      <c r="A27" s="82"/>
+      <c r="B27" s="83"/>
+      <c r="C27" s="83"/>
+      <c r="D27" s="83"/>
+      <c r="E27" s="83"/>
+      <c r="F27" s="83"/>
+      <c r="G27" s="83"/>
+      <c r="H27" s="83"/>
+      <c r="I27" s="83"/>
+      <c r="J27" s="83"/>
+      <c r="K27" s="83"/>
+      <c r="L27" s="83"/>
+      <c r="M27" s="83"/>
+      <c r="N27" s="83"/>
+      <c r="O27" s="83"/>
+      <c r="P27" s="83"/>
+      <c r="Q27" s="83"/>
+      <c r="R27" s="83"/>
+      <c r="S27" s="83"/>
+      <c r="T27" s="83"/>
+      <c r="U27" s="83"/>
+      <c r="V27" s="83"/>
+      <c r="W27" s="83"/>
+      <c r="X27" s="84"/>
     </row>
     <row r="28" spans="1:24" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A28" s="83"/>
-      <c r="B28" s="84"/>
-      <c r="C28" s="84"/>
-      <c r="D28" s="84"/>
-      <c r="E28" s="84"/>
-      <c r="F28" s="84"/>
-      <c r="G28" s="84"/>
-      <c r="H28" s="84"/>
-      <c r="I28" s="84"/>
-      <c r="J28" s="84"/>
-      <c r="K28" s="84"/>
-      <c r="L28" s="84"/>
-      <c r="M28" s="84"/>
-      <c r="N28" s="84"/>
-      <c r="O28" s="84"/>
-      <c r="P28" s="84"/>
-      <c r="Q28" s="84"/>
-      <c r="R28" s="84"/>
-      <c r="S28" s="84"/>
-      <c r="T28" s="84"/>
-      <c r="U28" s="84"/>
-      <c r="V28" s="84"/>
-      <c r="W28" s="84"/>
-      <c r="X28" s="85"/>
+      <c r="A28" s="82"/>
+      <c r="B28" s="83"/>
+      <c r="C28" s="83"/>
+      <c r="D28" s="83"/>
+      <c r="E28" s="83"/>
+      <c r="F28" s="83"/>
+      <c r="G28" s="83"/>
+      <c r="H28" s="83"/>
+      <c r="I28" s="83"/>
+      <c r="J28" s="83"/>
+      <c r="K28" s="83"/>
+      <c r="L28" s="83"/>
+      <c r="M28" s="83"/>
+      <c r="N28" s="83"/>
+      <c r="O28" s="83"/>
+      <c r="P28" s="83"/>
+      <c r="Q28" s="83"/>
+      <c r="R28" s="83"/>
+      <c r="S28" s="83"/>
+      <c r="T28" s="83"/>
+      <c r="U28" s="83"/>
+      <c r="V28" s="83"/>
+      <c r="W28" s="83"/>
+      <c r="X28" s="84"/>
     </row>
     <row r="29" spans="1:24" s="3" customFormat="1" ht="20.25" customHeight="1" thickBot="1">
-      <c r="A29" s="21"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="15"/>
-      <c r="N29" s="15"/>
-      <c r="O29" s="15"/>
-      <c r="P29" s="15"/>
-      <c r="Q29" s="15"/>
-      <c r="R29" s="15"/>
-      <c r="S29" s="15"/>
-      <c r="T29" s="15"/>
-      <c r="U29" s="15"/>
-      <c r="V29" s="15"/>
-      <c r="W29" s="15"/>
+      <c r="A29" s="20"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="14"/>
+      <c r="O29" s="14"/>
+      <c r="P29" s="14"/>
+      <c r="Q29" s="14"/>
+      <c r="R29" s="14"/>
+      <c r="S29" s="14"/>
+      <c r="T29" s="14"/>
+      <c r="U29" s="14"/>
+      <c r="V29" s="14"/>
+      <c r="W29" s="14"/>
       <c r="X29" s="6"/>
     </row>
     <row r="30" spans="1:24" s="3" customFormat="1" ht="12" customHeight="1" thickBot="1"/>
     <row r="31" spans="1:24" s="3" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A31" s="35"/>
-      <c r="B31" s="37"/>
-      <c r="C31" s="239" t="s">
+      <c r="A31" s="34"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="177" t="s">
         <v>161</v>
       </c>
-      <c r="D31" s="241"/>
-      <c r="E31" s="239" t="s">
+      <c r="D31" s="178"/>
+      <c r="E31" s="177" t="s">
         <v>162</v>
       </c>
-      <c r="F31" s="241"/>
-      <c r="G31" s="127" t="s">
+      <c r="F31" s="178"/>
+      <c r="G31" s="126" t="s">
         <v>73</v>
       </c>
-      <c r="H31" s="130" t="s">
+      <c r="H31" s="129" t="s">
         <v>74</v>
       </c>
-      <c r="I31" s="42" t="s">
+      <c r="I31" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="J31" s="36"/>
-      <c r="K31" s="38" t="s">
+      <c r="J31" s="35"/>
+      <c r="K31" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="L31" s="32" t="s">
+      <c r="L31" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="M31" s="34"/>
-      <c r="N31" s="23" t="s">
+      <c r="M31" s="33"/>
+      <c r="N31" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="O31" s="259" t="s">
+      <c r="O31" s="179" t="s">
         <v>78</v>
       </c>
-      <c r="P31" s="260"/>
-      <c r="Q31" s="260"/>
-      <c r="R31" s="260"/>
-      <c r="S31" s="260"/>
-      <c r="T31" s="260"/>
-      <c r="U31" s="260"/>
-      <c r="V31" s="260"/>
-      <c r="W31" s="260"/>
-      <c r="X31" s="261"/>
+      <c r="P31" s="180"/>
+      <c r="Q31" s="180"/>
+      <c r="R31" s="180"/>
+      <c r="S31" s="180"/>
+      <c r="T31" s="180"/>
+      <c r="U31" s="180"/>
+      <c r="V31" s="180"/>
+      <c r="W31" s="180"/>
+      <c r="X31" s="181"/>
     </row>
     <row r="32" spans="1:24" s="3" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A32" s="265" t="s">
+      <c r="A32" s="185" t="s">
         <v>158</v>
       </c>
-      <c r="B32" s="167"/>
-      <c r="C32" s="166"/>
-      <c r="D32" s="167"/>
-      <c r="E32" s="166"/>
-      <c r="F32" s="167"/>
-      <c r="G32" s="169"/>
-      <c r="H32" s="33">
+      <c r="B32" s="186"/>
+      <c r="C32" s="245"/>
+      <c r="D32" s="186"/>
+      <c r="E32" s="245"/>
+      <c r="F32" s="186"/>
+      <c r="G32" s="246"/>
+      <c r="H32" s="32">
         <v>1</v>
       </c>
-      <c r="I32" s="43" t="s">
+      <c r="I32" s="42" t="s">
         <v>76</v>
       </c>
       <c r="J32" s="8"/>
-      <c r="K32" s="39" t="s">
+      <c r="K32" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="L32" s="44" t="s">
+      <c r="L32" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="M32" s="17"/>
-      <c r="N32" s="131"/>
-      <c r="O32" s="262" t="s">
+      <c r="M32" s="16"/>
+      <c r="N32" s="130"/>
+      <c r="O32" s="182" t="s">
         <v>139</v>
       </c>
-      <c r="P32" s="263"/>
-      <c r="Q32" s="263"/>
-      <c r="R32" s="236"/>
-      <c r="S32" s="235" t="s">
+      <c r="P32" s="183"/>
+      <c r="Q32" s="183"/>
+      <c r="R32" s="172"/>
+      <c r="S32" s="171" t="s">
         <v>79</v>
       </c>
-      <c r="T32" s="263"/>
-      <c r="U32" s="263"/>
-      <c r="V32" s="263"/>
-      <c r="W32" s="263"/>
-      <c r="X32" s="264"/>
+      <c r="T32" s="183"/>
+      <c r="U32" s="183"/>
+      <c r="V32" s="183"/>
+      <c r="W32" s="183"/>
+      <c r="X32" s="184"/>
     </row>
     <row r="33" spans="1:28" s="3" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A33" s="162"/>
-      <c r="B33" s="163"/>
-      <c r="C33" s="168"/>
-      <c r="D33" s="163"/>
-      <c r="E33" s="168"/>
-      <c r="F33" s="163"/>
-      <c r="G33" s="170"/>
-      <c r="H33" s="132" t="s">
+      <c r="A33" s="187"/>
+      <c r="B33" s="188"/>
+      <c r="C33" s="160"/>
+      <c r="D33" s="188"/>
+      <c r="E33" s="160"/>
+      <c r="F33" s="188"/>
+      <c r="G33" s="247"/>
+      <c r="H33" s="131" t="s">
         <v>74</v>
       </c>
-      <c r="I33" s="41" t="s">
+      <c r="I33" s="40" t="s">
         <v>75</v>
       </c>
       <c r="J33" s="8"/>
-      <c r="K33" s="39" t="s">
+      <c r="K33" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="L33" s="26" t="s">
+      <c r="L33" s="25" t="s">
         <v>58</v>
       </c>
       <c r="M33" s="4"/>
-      <c r="N33" s="133" t="s">
+      <c r="N33" s="132" t="s">
         <v>59</v>
       </c>
-      <c r="O33" s="125">
+      <c r="O33" s="124">
         <v>1</v>
       </c>
-      <c r="P33" s="114"/>
-      <c r="Q33" s="114">
+      <c r="P33" s="113"/>
+      <c r="Q33" s="113">
         <v>4</v>
       </c>
-      <c r="R33" s="115"/>
-      <c r="S33" s="116">
+      <c r="R33" s="114"/>
+      <c r="S33" s="115">
         <v>1</v>
       </c>
-      <c r="T33" s="117"/>
-      <c r="U33" s="118"/>
-      <c r="V33" s="235">
+      <c r="T33" s="116"/>
+      <c r="U33" s="117"/>
+      <c r="V33" s="171">
         <v>4</v>
       </c>
-      <c r="W33" s="236"/>
-      <c r="X33" s="119"/>
+      <c r="W33" s="172"/>
+      <c r="X33" s="118"/>
     </row>
     <row r="34" spans="1:28" s="3" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A34" s="253" t="s">
+      <c r="A34" s="169" t="s">
         <v>159</v>
       </c>
-      <c r="B34" s="254"/>
-      <c r="C34" s="173"/>
-      <c r="D34" s="172"/>
-      <c r="E34" s="173"/>
-      <c r="F34" s="172"/>
-      <c r="G34" s="128"/>
-      <c r="H34" s="134">
+      <c r="B34" s="170"/>
+      <c r="C34" s="163"/>
+      <c r="D34" s="206"/>
+      <c r="E34" s="163"/>
+      <c r="F34" s="206"/>
+      <c r="G34" s="127"/>
+      <c r="H34" s="133">
         <v>2</v>
       </c>
-      <c r="I34" s="41" t="s">
+      <c r="I34" s="40" t="s">
         <v>76</v>
       </c>
       <c r="J34" s="8"/>
-      <c r="K34" s="39" t="s">
+      <c r="K34" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="L34" s="44" t="s">
+      <c r="L34" s="43" t="s">
         <v>77</v>
       </c>
       <c r="M34" s="7"/>
-      <c r="N34" s="131"/>
-      <c r="O34" s="125">
+      <c r="N34" s="130"/>
+      <c r="O34" s="124">
         <v>2</v>
       </c>
-      <c r="P34" s="114"/>
-      <c r="Q34" s="114">
+      <c r="P34" s="113"/>
+      <c r="Q34" s="113">
         <v>5</v>
       </c>
-      <c r="R34" s="115"/>
-      <c r="S34" s="114">
+      <c r="R34" s="114"/>
+      <c r="S34" s="113">
         <v>2</v>
       </c>
-      <c r="T34" s="112"/>
-      <c r="U34" s="113"/>
-      <c r="V34" s="235">
+      <c r="T34" s="111"/>
+      <c r="U34" s="112"/>
+      <c r="V34" s="171">
         <v>5</v>
       </c>
-      <c r="W34" s="236"/>
-      <c r="X34" s="119"/>
+      <c r="W34" s="172"/>
+      <c r="X34" s="118"/>
       <c r="AB34" s="4"/>
     </row>
     <row r="35" spans="1:28" s="3" customFormat="1" ht="28.5" customHeight="1" thickBot="1">
-      <c r="A35" s="255" t="s">
+      <c r="A35" s="173" t="s">
         <v>160</v>
       </c>
-      <c r="B35" s="256"/>
-      <c r="C35" s="164"/>
-      <c r="D35" s="165"/>
-      <c r="E35" s="164"/>
-      <c r="F35" s="165"/>
-      <c r="G35" s="129"/>
-      <c r="H35" s="59"/>
+      <c r="B35" s="174"/>
+      <c r="C35" s="166"/>
+      <c r="D35" s="189"/>
+      <c r="E35" s="166"/>
+      <c r="F35" s="189"/>
+      <c r="G35" s="128"/>
+      <c r="H35" s="58"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
       <c r="M35" s="5"/>
       <c r="N35" s="6"/>
-      <c r="O35" s="126">
+      <c r="O35" s="125">
         <v>3</v>
       </c>
-      <c r="P35" s="120"/>
-      <c r="Q35" s="120">
+      <c r="P35" s="119"/>
+      <c r="Q35" s="119">
         <v>6</v>
       </c>
-      <c r="R35" s="121"/>
-      <c r="S35" s="120">
+      <c r="R35" s="120"/>
+      <c r="S35" s="119">
         <v>3</v>
       </c>
-      <c r="T35" s="122"/>
-      <c r="U35" s="123"/>
-      <c r="V35" s="257">
+      <c r="T35" s="121"/>
+      <c r="U35" s="122"/>
+      <c r="V35" s="175">
         <v>6</v>
       </c>
-      <c r="W35" s="258"/>
-      <c r="X35" s="124"/>
+      <c r="W35" s="176"/>
+      <c r="X35" s="123"/>
     </row>
     <row r="36" spans="1:28" s="3" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A36" s="102" t="s">
+      <c r="A36" s="101" t="s">
         <v>173</v>
       </c>
-      <c r="B36" s="103"/>
-      <c r="C36" s="103"/>
-      <c r="D36" s="103"/>
-      <c r="E36" s="103"/>
-      <c r="F36" s="103"/>
-      <c r="G36" s="104"/>
-      <c r="T36" s="234" t="s">
+      <c r="B36" s="102"/>
+      <c r="C36" s="102"/>
+      <c r="D36" s="102"/>
+      <c r="E36" s="102"/>
+      <c r="F36" s="102"/>
+      <c r="G36" s="103"/>
+      <c r="T36" s="190" t="s">
         <v>153</v>
       </c>
-      <c r="U36" s="234"/>
-      <c r="V36" s="234"/>
-      <c r="W36" s="234"/>
-      <c r="X36" s="111" t="s">
+      <c r="U36" s="190"/>
+      <c r="V36" s="190"/>
+      <c r="W36" s="190"/>
+      <c r="X36" s="110" t="s">
         <v>132</v>
       </c>
     </row>
@@ -4377,23 +4413,49 @@
     <row r="48" spans="1:28" s="3" customFormat="1" ht="17.399999999999999"/>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="V5:X5"/>
-    <mergeCell ref="V6:X6"/>
-    <mergeCell ref="V7:X7"/>
-    <mergeCell ref="V8:X8"/>
-    <mergeCell ref="V9:X9"/>
-    <mergeCell ref="V10:X10"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="V34:W34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="V35:W35"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="O31:X31"/>
-    <mergeCell ref="O32:R32"/>
-    <mergeCell ref="S32:X32"/>
-    <mergeCell ref="A32:B33"/>
-    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A5:B7"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="C32:D33"/>
+    <mergeCell ref="E32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:M8"/>
+    <mergeCell ref="J6:M7"/>
+    <mergeCell ref="C9:E10"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C5:E7"/>
+    <mergeCell ref="F5:I7"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="T7:U7"/>
+    <mergeCell ref="J5:M5"/>
+    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="R6:R7"/>
+    <mergeCell ref="S6:S7"/>
+    <mergeCell ref="N6:Q7"/>
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="Z2:AU2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="N4:Q4"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="T4:X4"/>
+    <mergeCell ref="A2:R3"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="T8:U8"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="T9:U9"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="N8:Q8"/>
     <mergeCell ref="T36:W36"/>
     <mergeCell ref="V33:W33"/>
     <mergeCell ref="T10:U10"/>
@@ -4410,49 +4472,23 @@
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="C35:D35"/>
-    <mergeCell ref="T8:U8"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="T9:U9"/>
-    <mergeCell ref="R8:S8"/>
-    <mergeCell ref="N8:Q8"/>
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="Z2:AU2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="N4:Q4"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="T4:X4"/>
-    <mergeCell ref="A2:R3"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="T7:U7"/>
-    <mergeCell ref="J5:M5"/>
-    <mergeCell ref="N5:Q5"/>
-    <mergeCell ref="R6:R7"/>
-    <mergeCell ref="S6:S7"/>
-    <mergeCell ref="N6:Q7"/>
-    <mergeCell ref="A5:B7"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="C32:D33"/>
-    <mergeCell ref="E32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:M8"/>
-    <mergeCell ref="J6:M7"/>
-    <mergeCell ref="C9:E10"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C5:E7"/>
-    <mergeCell ref="F5:I7"/>
+    <mergeCell ref="V10:X10"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="V34:W34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="V35:W35"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="O31:X31"/>
+    <mergeCell ref="O32:R32"/>
+    <mergeCell ref="S32:X32"/>
+    <mergeCell ref="A32:B33"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="V5:X5"/>
+    <mergeCell ref="V6:X6"/>
+    <mergeCell ref="V7:X7"/>
+    <mergeCell ref="V8:X8"/>
+    <mergeCell ref="V9:X9"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -4470,208 +4506,208 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23:P23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22:P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="19.8"/>
   <cols>
-    <col min="1" max="1" width="12.875" style="47" customWidth="1"/>
-    <col min="2" max="2" width="10.75" style="47" customWidth="1"/>
-    <col min="3" max="3" width="12.875" style="47" customWidth="1"/>
-    <col min="4" max="4" width="12.125" style="47" customWidth="1"/>
-    <col min="5" max="7" width="11" style="47" customWidth="1"/>
-    <col min="8" max="9" width="10.75" style="47" customWidth="1"/>
-    <col min="10" max="10" width="4" style="47" customWidth="1"/>
-    <col min="11" max="13" width="11.125" style="47" customWidth="1"/>
-    <col min="14" max="14" width="11.375" style="47" customWidth="1"/>
-    <col min="15" max="18" width="11.125" style="47" customWidth="1"/>
-    <col min="19" max="16384" width="9.125" style="47"/>
+    <col min="1" max="1" width="12.875" style="46" customWidth="1"/>
+    <col min="2" max="2" width="10.75" style="46" customWidth="1"/>
+    <col min="3" max="3" width="12.875" style="46" customWidth="1"/>
+    <col min="4" max="4" width="12.125" style="46" customWidth="1"/>
+    <col min="5" max="7" width="11" style="46" customWidth="1"/>
+    <col min="8" max="9" width="10.75" style="46" customWidth="1"/>
+    <col min="10" max="10" width="4" style="46" customWidth="1"/>
+    <col min="11" max="13" width="11.125" style="46" customWidth="1"/>
+    <col min="14" max="14" width="11.375" style="46" customWidth="1"/>
+    <col min="15" max="18" width="11.125" style="46" customWidth="1"/>
+    <col min="19" max="16384" width="9.125" style="46"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="8.25" customHeight="1" thickBot="1"/>
     <row r="2" spans="1:18" s="1" customFormat="1" ht="23.4">
-      <c r="A2" s="98" t="s">
+      <c r="A2" s="97" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
-      <c r="K2" s="99" t="s">
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98" t="s">
         <v>92</v>
       </c>
-      <c r="L2" s="99"/>
-      <c r="M2" s="99"/>
-      <c r="N2" s="99"/>
-      <c r="O2" s="99"/>
-      <c r="P2" s="99"/>
-      <c r="Q2" s="99"/>
-      <c r="R2" s="100"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
+      <c r="O2" s="98"/>
+      <c r="P2" s="98"/>
+      <c r="Q2" s="98"/>
+      <c r="R2" s="99"/>
     </row>
     <row r="3" spans="1:18" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A3" s="80"/>
-      <c r="B3" s="81"/>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
-      <c r="O3" s="81"/>
-      <c r="P3" s="81"/>
-      <c r="Q3" s="81"/>
-      <c r="R3" s="82"/>
+      <c r="A3" s="79"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="80"/>
+      <c r="K3" s="80"/>
+      <c r="L3" s="80"/>
+      <c r="M3" s="80"/>
+      <c r="N3" s="80"/>
+      <c r="O3" s="80"/>
+      <c r="P3" s="80"/>
+      <c r="Q3" s="80"/>
+      <c r="R3" s="81"/>
     </row>
     <row r="4" spans="1:18" s="3" customFormat="1" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A4" s="216" t="s">
+      <c r="A4" s="213" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="275"/>
-      <c r="C4" s="276" t="s">
+      <c r="B4" s="288"/>
+      <c r="C4" s="291" t="s">
         <v>89</v>
       </c>
-      <c r="D4" s="275"/>
-      <c r="E4" s="276" t="s">
+      <c r="D4" s="288"/>
+      <c r="E4" s="291" t="s">
         <v>88</v>
       </c>
-      <c r="F4" s="275"/>
-      <c r="G4" s="217" t="s">
+      <c r="F4" s="288"/>
+      <c r="G4" s="214" t="s">
         <v>152</v>
       </c>
-      <c r="H4" s="217"/>
-      <c r="I4" s="218"/>
+      <c r="H4" s="214"/>
+      <c r="I4" s="215"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="277" t="s">
+      <c r="K4" s="298" t="s">
         <v>94</v>
       </c>
-      <c r="L4" s="278"/>
-      <c r="M4" s="278"/>
-      <c r="N4" s="278"/>
-      <c r="O4" s="278"/>
-      <c r="P4" s="278"/>
-      <c r="Q4" s="278"/>
-      <c r="R4" s="279"/>
+      <c r="L4" s="299"/>
+      <c r="M4" s="299"/>
+      <c r="N4" s="299"/>
+      <c r="O4" s="299"/>
+      <c r="P4" s="299"/>
+      <c r="Q4" s="299"/>
+      <c r="R4" s="300"/>
     </row>
     <row r="5" spans="1:18" ht="21.75" customHeight="1">
-      <c r="A5" s="296"/>
-      <c r="B5" s="200"/>
-      <c r="C5" s="199"/>
-      <c r="D5" s="200"/>
-      <c r="E5" s="199"/>
-      <c r="F5" s="200"/>
-      <c r="G5" s="199"/>
-      <c r="H5" s="234"/>
-      <c r="I5" s="298"/>
-      <c r="J5" s="81"/>
-      <c r="K5" s="270" t="s">
+      <c r="A5" s="301"/>
+      <c r="B5" s="230"/>
+      <c r="C5" s="229"/>
+      <c r="D5" s="230"/>
+      <c r="E5" s="229"/>
+      <c r="F5" s="230"/>
+      <c r="G5" s="229"/>
+      <c r="H5" s="190"/>
+      <c r="I5" s="303"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="294" t="s">
         <v>170</v>
       </c>
-      <c r="L5" s="271"/>
-      <c r="M5" s="272"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="280" t="s">
+      <c r="L5" s="295"/>
+      <c r="M5" s="284"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="274" t="s">
         <v>141</v>
       </c>
-      <c r="P5" s="272"/>
-      <c r="Q5" s="280"/>
-      <c r="R5" s="305"/>
+      <c r="P5" s="284"/>
+      <c r="Q5" s="274"/>
+      <c r="R5" s="275"/>
     </row>
     <row r="6" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A6" s="285"/>
-      <c r="B6" s="287"/>
-      <c r="C6" s="297"/>
-      <c r="D6" s="287"/>
-      <c r="E6" s="297"/>
-      <c r="F6" s="287"/>
-      <c r="G6" s="297"/>
-      <c r="H6" s="286"/>
-      <c r="I6" s="299"/>
-      <c r="J6" s="81"/>
-      <c r="K6" s="171" t="s">
+      <c r="A6" s="278"/>
+      <c r="B6" s="280"/>
+      <c r="C6" s="302"/>
+      <c r="D6" s="280"/>
+      <c r="E6" s="302"/>
+      <c r="F6" s="280"/>
+      <c r="G6" s="302"/>
+      <c r="H6" s="279"/>
+      <c r="I6" s="304"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="248" t="s">
         <v>171</v>
       </c>
-      <c r="L6" s="172"/>
-      <c r="M6" s="40" t="s">
+      <c r="L6" s="206"/>
+      <c r="M6" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="N6" s="18"/>
-      <c r="O6" s="13" t="s">
+      <c r="N6" s="17"/>
+      <c r="O6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="13" t="s">
+      <c r="P6" s="17"/>
+      <c r="Q6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="R6" s="56"/>
+      <c r="R6" s="55"/>
     </row>
     <row r="7" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A7" s="80"/>
-      <c r="B7" s="81"/>
-      <c r="C7" s="81"/>
-      <c r="D7" s="81"/>
-      <c r="E7" s="81"/>
-      <c r="F7" s="81"/>
-      <c r="G7" s="81"/>
-      <c r="H7" s="81"/>
-      <c r="I7" s="81"/>
-      <c r="J7" s="81"/>
-      <c r="K7" s="273" t="s">
+      <c r="A7" s="79"/>
+      <c r="B7" s="80"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="80"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="80"/>
+      <c r="G7" s="80"/>
+      <c r="H7" s="80"/>
+      <c r="I7" s="80"/>
+      <c r="J7" s="80"/>
+      <c r="K7" s="296" t="s">
         <v>172</v>
       </c>
-      <c r="L7" s="274"/>
-      <c r="M7" s="19" t="s">
+      <c r="L7" s="297"/>
+      <c r="M7" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="N7" s="10"/>
-      <c r="O7" s="182" t="s">
+      <c r="N7" s="9"/>
+      <c r="O7" s="255" t="s">
         <v>108</v>
       </c>
-      <c r="P7" s="184"/>
-      <c r="Q7" s="164"/>
-      <c r="R7" s="252"/>
+      <c r="P7" s="203"/>
+      <c r="Q7" s="166"/>
+      <c r="R7" s="168"/>
     </row>
     <row r="8" spans="1:18" s="3" customFormat="1" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A8" s="57" t="s">
+      <c r="A8" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="H8" s="25" t="s">
+      <c r="H8" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="I8" s="58" t="s">
+      <c r="I8" s="57" t="s">
         <v>84</v>
       </c>
       <c r="J8" s="4"/>
-      <c r="K8" s="101" t="s">
+      <c r="K8" s="100" t="s">
         <v>142</v>
       </c>
       <c r="L8" s="4"/>
@@ -4680,152 +4716,152 @@
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
-      <c r="R8" s="70"/>
+      <c r="R8" s="69"/>
     </row>
     <row r="9" spans="1:18" s="3" customFormat="1" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A9" s="60" t="s">
+      <c r="A9" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="61" t="s">
+      <c r="B9" s="60" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="61" t="s">
+      <c r="C9" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="D9" s="62" t="s">
+      <c r="D9" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="E9" s="61" t="s">
+      <c r="E9" s="60" t="s">
         <v>98</v>
       </c>
-      <c r="F9" s="61" t="s">
+      <c r="F9" s="60" t="s">
         <v>99</v>
       </c>
-      <c r="G9" s="61" t="s">
+      <c r="G9" s="60" t="s">
         <v>100</v>
       </c>
-      <c r="H9" s="63" t="s">
+      <c r="H9" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="I9" s="64" t="s">
+      <c r="I9" s="63" t="s">
         <v>34</v>
       </c>
       <c r="J9" s="4"/>
-      <c r="K9" s="68" t="s">
+      <c r="K9" s="67" t="s">
         <v>104</v>
       </c>
-      <c r="L9" s="36" t="s">
+      <c r="L9" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="M9" s="37"/>
-      <c r="N9" s="280" t="s">
+      <c r="M9" s="36"/>
+      <c r="N9" s="274" t="s">
         <v>109</v>
       </c>
-      <c r="O9" s="272"/>
-      <c r="P9" s="185" t="s">
+      <c r="O9" s="284"/>
+      <c r="P9" s="256" t="s">
         <v>110</v>
       </c>
-      <c r="Q9" s="186"/>
-      <c r="R9" s="281"/>
+      <c r="Q9" s="257"/>
+      <c r="R9" s="292"/>
     </row>
     <row r="10" spans="1:18" ht="21.75" customHeight="1">
-      <c r="A10" s="65" t="s">
+      <c r="A10" s="64" t="s">
         <v>86</v>
       </c>
-      <c r="B10" s="66"/>
-      <c r="C10" s="66"/>
-      <c r="D10" s="66"/>
-      <c r="E10" s="66"/>
-      <c r="F10" s="66"/>
-      <c r="G10" s="66"/>
-      <c r="H10" s="66"/>
-      <c r="I10" s="67"/>
-      <c r="J10" s="81"/>
-      <c r="K10" s="22" t="s">
+      <c r="B10" s="65"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="66"/>
+      <c r="J10" s="80"/>
+      <c r="K10" s="21" t="s">
         <v>105</v>
       </c>
       <c r="L10" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="M10" s="11"/>
-      <c r="N10" s="173" t="s">
+      <c r="M10" s="10"/>
+      <c r="N10" s="163" t="s">
         <v>109</v>
       </c>
-      <c r="O10" s="172"/>
-      <c r="P10" s="166" t="s">
+      <c r="O10" s="206"/>
+      <c r="P10" s="245" t="s">
         <v>110</v>
       </c>
-      <c r="Q10" s="181"/>
-      <c r="R10" s="282"/>
+      <c r="Q10" s="201"/>
+      <c r="R10" s="293"/>
     </row>
     <row r="11" spans="1:18" ht="21.75" customHeight="1">
-      <c r="A11" s="87"/>
-      <c r="B11" s="88"/>
-      <c r="C11" s="88"/>
-      <c r="D11" s="88"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="88"/>
-      <c r="H11" s="88"/>
-      <c r="I11" s="89"/>
-      <c r="J11" s="81"/>
-      <c r="K11" s="22" t="s">
+      <c r="A11" s="86"/>
+      <c r="B11" s="87"/>
+      <c r="C11" s="87"/>
+      <c r="D11" s="87"/>
+      <c r="E11" s="87"/>
+      <c r="F11" s="87"/>
+      <c r="G11" s="87"/>
+      <c r="H11" s="87"/>
+      <c r="I11" s="88"/>
+      <c r="J11" s="80"/>
+      <c r="K11" s="21" t="s">
         <v>106</v>
       </c>
       <c r="L11" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="M11" s="11"/>
-      <c r="N11" s="173" t="s">
+      <c r="M11" s="10"/>
+      <c r="N11" s="163" t="s">
         <v>109</v>
       </c>
-      <c r="O11" s="172"/>
-      <c r="P11" s="173" t="s">
+      <c r="O11" s="206"/>
+      <c r="P11" s="163" t="s">
         <v>110</v>
       </c>
-      <c r="Q11" s="174"/>
-      <c r="R11" s="269"/>
+      <c r="Q11" s="164"/>
+      <c r="R11" s="165"/>
     </row>
     <row r="12" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A12" s="90"/>
-      <c r="B12" s="91"/>
-      <c r="C12" s="91"/>
-      <c r="D12" s="91"/>
-      <c r="E12" s="91"/>
-      <c r="F12" s="91"/>
-      <c r="G12" s="91"/>
-      <c r="H12" s="91"/>
-      <c r="I12" s="92"/>
-      <c r="J12" s="81"/>
-      <c r="K12" s="69" t="s">
+      <c r="A12" s="89"/>
+      <c r="B12" s="90"/>
+      <c r="C12" s="90"/>
+      <c r="D12" s="90"/>
+      <c r="E12" s="90"/>
+      <c r="F12" s="90"/>
+      <c r="G12" s="90"/>
+      <c r="H12" s="90"/>
+      <c r="I12" s="91"/>
+      <c r="J12" s="80"/>
+      <c r="K12" s="68" t="s">
         <v>107</v>
       </c>
       <c r="L12" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="M12" s="10"/>
-      <c r="N12" s="182" t="s">
+      <c r="M12" s="9"/>
+      <c r="N12" s="255" t="s">
         <v>109</v>
       </c>
-      <c r="O12" s="184"/>
-      <c r="P12" s="173" t="s">
+      <c r="O12" s="203"/>
+      <c r="P12" s="163" t="s">
         <v>110</v>
       </c>
-      <c r="Q12" s="174"/>
-      <c r="R12" s="269"/>
+      <c r="Q12" s="164"/>
+      <c r="R12" s="165"/>
     </row>
     <row r="13" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A13" s="90"/>
-      <c r="B13" s="91"/>
-      <c r="C13" s="91"/>
-      <c r="D13" s="91"/>
-      <c r="E13" s="91"/>
-      <c r="F13" s="91"/>
-      <c r="G13" s="91"/>
-      <c r="H13" s="91"/>
-      <c r="I13" s="92"/>
-      <c r="J13" s="81"/>
-      <c r="K13" s="101" t="s">
+      <c r="A13" s="89"/>
+      <c r="B13" s="90"/>
+      <c r="C13" s="90"/>
+      <c r="D13" s="90"/>
+      <c r="E13" s="90"/>
+      <c r="F13" s="90"/>
+      <c r="G13" s="90"/>
+      <c r="H13" s="90"/>
+      <c r="I13" s="91"/>
+      <c r="J13" s="80"/>
+      <c r="K13" s="100" t="s">
         <v>143</v>
       </c>
       <c r="L13" s="4"/>
@@ -4834,116 +4870,116 @@
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
-      <c r="R13" s="70"/>
+      <c r="R13" s="69"/>
     </row>
     <row r="14" spans="1:18" ht="21.75" customHeight="1">
-      <c r="A14" s="90"/>
-      <c r="B14" s="91"/>
-      <c r="C14" s="91"/>
-      <c r="D14" s="91"/>
-      <c r="E14" s="91"/>
-      <c r="F14" s="91"/>
-      <c r="G14" s="91"/>
-      <c r="H14" s="91"/>
-      <c r="I14" s="92"/>
-      <c r="J14" s="81"/>
-      <c r="K14" s="35" t="s">
+      <c r="A14" s="89"/>
+      <c r="B14" s="90"/>
+      <c r="C14" s="90"/>
+      <c r="D14" s="90"/>
+      <c r="E14" s="90"/>
+      <c r="F14" s="90"/>
+      <c r="G14" s="90"/>
+      <c r="H14" s="90"/>
+      <c r="I14" s="91"/>
+      <c r="J14" s="80"/>
+      <c r="K14" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="L14" s="36"/>
-      <c r="M14" s="36"/>
-      <c r="N14" s="37"/>
-      <c r="O14" s="94" t="s">
+      <c r="L14" s="35"/>
+      <c r="M14" s="35"/>
+      <c r="N14" s="36"/>
+      <c r="O14" s="93" t="s">
         <v>104</v>
       </c>
-      <c r="P14" s="94" t="s">
+      <c r="P14" s="93" t="s">
         <v>105</v>
       </c>
-      <c r="Q14" s="94" t="s">
+      <c r="Q14" s="93" t="s">
         <v>106</v>
       </c>
-      <c r="R14" s="95" t="s">
+      <c r="R14" s="94" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="21.75" customHeight="1">
-      <c r="A15" s="90"/>
-      <c r="B15" s="91"/>
-      <c r="C15" s="91"/>
-      <c r="D15" s="91"/>
-      <c r="E15" s="91"/>
-      <c r="F15" s="91"/>
-      <c r="G15" s="91"/>
-      <c r="H15" s="91"/>
-      <c r="I15" s="92"/>
-      <c r="J15" s="81"/>
-      <c r="K15" s="55" t="s">
+      <c r="A15" s="89"/>
+      <c r="B15" s="90"/>
+      <c r="C15" s="90"/>
+      <c r="D15" s="90"/>
+      <c r="E15" s="90"/>
+      <c r="F15" s="90"/>
+      <c r="G15" s="90"/>
+      <c r="H15" s="90"/>
+      <c r="I15" s="91"/>
+      <c r="J15" s="80"/>
+      <c r="K15" s="54" t="s">
         <v>145</v>
       </c>
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="9"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="305"/>
+      <c r="P15" s="305"/>
+      <c r="Q15" s="305"/>
+      <c r="R15" s="306"/>
     </row>
     <row r="16" spans="1:18" ht="21.75" customHeight="1">
-      <c r="A16" s="90"/>
-      <c r="B16" s="91"/>
-      <c r="C16" s="91"/>
-      <c r="D16" s="91"/>
-      <c r="E16" s="91"/>
-      <c r="F16" s="91"/>
-      <c r="G16" s="91"/>
-      <c r="H16" s="91"/>
-      <c r="I16" s="92"/>
-      <c r="J16" s="81"/>
-      <c r="K16" s="55" t="s">
+      <c r="A16" s="89"/>
+      <c r="B16" s="90"/>
+      <c r="C16" s="90"/>
+      <c r="D16" s="90"/>
+      <c r="E16" s="90"/>
+      <c r="F16" s="90"/>
+      <c r="G16" s="90"/>
+      <c r="H16" s="90"/>
+      <c r="I16" s="91"/>
+      <c r="J16" s="80"/>
+      <c r="K16" s="54" t="s">
         <v>146</v>
       </c>
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
-      <c r="N16" s="11"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="9"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="305"/>
+      <c r="P16" s="305"/>
+      <c r="Q16" s="305"/>
+      <c r="R16" s="306"/>
     </row>
     <row r="17" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A17" s="90"/>
-      <c r="B17" s="91"/>
-      <c r="C17" s="91"/>
-      <c r="D17" s="91"/>
-      <c r="E17" s="91"/>
-      <c r="F17" s="91"/>
-      <c r="G17" s="91"/>
-      <c r="H17" s="91"/>
-      <c r="I17" s="92"/>
-      <c r="J17" s="81"/>
-      <c r="K17" s="59" t="s">
+      <c r="A17" s="89"/>
+      <c r="B17" s="90"/>
+      <c r="C17" s="90"/>
+      <c r="D17" s="90"/>
+      <c r="E17" s="90"/>
+      <c r="F17" s="90"/>
+      <c r="G17" s="90"/>
+      <c r="H17" s="90"/>
+      <c r="I17" s="91"/>
+      <c r="J17" s="80"/>
+      <c r="K17" s="58" t="s">
         <v>147</v>
       </c>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="6"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="307"/>
+      <c r="P17" s="307"/>
+      <c r="Q17" s="307"/>
+      <c r="R17" s="308"/>
     </row>
     <row r="18" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A18" s="86"/>
-      <c r="B18" s="71"/>
-      <c r="C18" s="71"/>
-      <c r="D18" s="71"/>
-      <c r="E18" s="71"/>
-      <c r="F18" s="71"/>
-      <c r="G18" s="71"/>
-      <c r="H18" s="71"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="81"/>
-      <c r="K18" s="101" t="s">
+      <c r="A18" s="85"/>
+      <c r="B18" s="70"/>
+      <c r="C18" s="70"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="70"/>
+      <c r="F18" s="70"/>
+      <c r="G18" s="70"/>
+      <c r="H18" s="70"/>
+      <c r="I18" s="53"/>
+      <c r="J18" s="80"/>
+      <c r="K18" s="100" t="s">
         <v>111</v>
       </c>
       <c r="L18" s="4"/>
@@ -4952,164 +4988,164 @@
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
-      <c r="R18" s="70"/>
+      <c r="R18" s="69"/>
     </row>
     <row r="19" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A19" s="285" t="s">
+      <c r="A19" s="278" t="s">
         <v>85</v>
       </c>
-      <c r="B19" s="286"/>
-      <c r="C19" s="286"/>
-      <c r="D19" s="287"/>
-      <c r="E19" s="71"/>
-      <c r="F19" s="71"/>
-      <c r="G19" s="71"/>
-      <c r="H19" s="71"/>
-      <c r="I19" s="54"/>
-      <c r="J19" s="81"/>
-      <c r="K19" s="35" t="s">
+      <c r="B19" s="279"/>
+      <c r="C19" s="279"/>
+      <c r="D19" s="280"/>
+      <c r="E19" s="70"/>
+      <c r="F19" s="70"/>
+      <c r="G19" s="70"/>
+      <c r="H19" s="70"/>
+      <c r="I19" s="53"/>
+      <c r="J19" s="80"/>
+      <c r="K19" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="L19" s="36"/>
-      <c r="M19" s="36"/>
-      <c r="N19" s="37"/>
-      <c r="O19" s="280" t="s">
+      <c r="L19" s="35"/>
+      <c r="M19" s="35"/>
+      <c r="N19" s="36"/>
+      <c r="O19" s="274" t="s">
         <v>118</v>
       </c>
-      <c r="P19" s="272"/>
-      <c r="Q19" s="294" t="s">
+      <c r="P19" s="284"/>
+      <c r="Q19" s="289" t="s">
         <v>119</v>
       </c>
-      <c r="R19" s="295"/>
+      <c r="R19" s="290"/>
     </row>
     <row r="20" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A20" s="80"/>
-      <c r="B20" s="81"/>
-      <c r="C20" s="81"/>
-      <c r="D20" s="81"/>
-      <c r="E20" s="81"/>
-      <c r="F20" s="81"/>
-      <c r="G20" s="81"/>
-      <c r="H20" s="81"/>
-      <c r="I20" s="81"/>
-      <c r="J20" s="81"/>
-      <c r="K20" s="55" t="s">
+      <c r="A20" s="79"/>
+      <c r="B20" s="80"/>
+      <c r="C20" s="80"/>
+      <c r="D20" s="80"/>
+      <c r="E20" s="80"/>
+      <c r="F20" s="80"/>
+      <c r="G20" s="80"/>
+      <c r="H20" s="80"/>
+      <c r="I20" s="80"/>
+      <c r="J20" s="80"/>
+      <c r="K20" s="54" t="s">
         <v>113</v>
       </c>
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
-      <c r="N20" s="11"/>
-      <c r="O20" s="173"/>
-      <c r="P20" s="172"/>
-      <c r="Q20" s="173"/>
-      <c r="R20" s="269"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="317"/>
+      <c r="P20" s="318"/>
+      <c r="Q20" s="317"/>
+      <c r="R20" s="319"/>
     </row>
     <row r="21" spans="1:18" s="3" customFormat="1" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A21" s="216" t="s">
+      <c r="A21" s="213" t="s">
         <v>90</v>
       </c>
-      <c r="B21" s="275"/>
-      <c r="C21" s="276" t="s">
+      <c r="B21" s="288"/>
+      <c r="C21" s="291" t="s">
         <v>89</v>
       </c>
-      <c r="D21" s="275"/>
-      <c r="E21" s="276" t="s">
+      <c r="D21" s="288"/>
+      <c r="E21" s="291" t="s">
         <v>91</v>
       </c>
-      <c r="F21" s="275"/>
-      <c r="G21" s="217" t="s">
+      <c r="F21" s="288"/>
+      <c r="G21" s="214" t="s">
         <v>87</v>
       </c>
-      <c r="H21" s="217"/>
-      <c r="I21" s="218"/>
+      <c r="H21" s="214"/>
+      <c r="I21" s="215"/>
       <c r="J21" s="4"/>
-      <c r="K21" s="55" t="s">
+      <c r="K21" s="54" t="s">
         <v>115</v>
       </c>
       <c r="L21" s="8"/>
       <c r="M21" s="8"/>
-      <c r="N21" s="11"/>
-      <c r="O21" s="173"/>
-      <c r="P21" s="172"/>
-      <c r="Q21" s="173"/>
-      <c r="R21" s="269"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="317"/>
+      <c r="P21" s="318"/>
+      <c r="Q21" s="317"/>
+      <c r="R21" s="319"/>
     </row>
     <row r="22" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A22" s="300"/>
-      <c r="B22" s="301"/>
-      <c r="C22" s="302"/>
-      <c r="D22" s="301"/>
-      <c r="E22" s="302"/>
-      <c r="F22" s="301"/>
-      <c r="G22" s="302"/>
-      <c r="H22" s="303"/>
-      <c r="I22" s="304"/>
-      <c r="J22" s="81"/>
-      <c r="K22" s="20" t="s">
+      <c r="A22" s="269"/>
+      <c r="B22" s="270"/>
+      <c r="C22" s="271"/>
+      <c r="D22" s="270"/>
+      <c r="E22" s="271"/>
+      <c r="F22" s="270"/>
+      <c r="G22" s="271"/>
+      <c r="H22" s="272"/>
+      <c r="I22" s="273"/>
+      <c r="J22" s="80"/>
+      <c r="K22" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="L22" s="72"/>
-      <c r="M22" s="73"/>
-      <c r="N22" s="40" t="s">
+      <c r="L22" s="71"/>
+      <c r="M22" s="72"/>
+      <c r="N22" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="O22" s="203"/>
-      <c r="P22" s="204"/>
-      <c r="Q22" s="72"/>
-      <c r="R22" s="46" t="s">
+      <c r="O22" s="207"/>
+      <c r="P22" s="208"/>
+      <c r="Q22" s="71"/>
+      <c r="R22" s="45" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A23" s="80"/>
-      <c r="B23" s="81"/>
-      <c r="C23" s="81"/>
-      <c r="D23" s="81"/>
-      <c r="E23" s="81"/>
-      <c r="F23" s="81"/>
-      <c r="G23" s="81"/>
-      <c r="H23" s="81"/>
-      <c r="I23" s="81"/>
-      <c r="J23" s="81"/>
-      <c r="K23" s="59" t="s">
+      <c r="A23" s="79"/>
+      <c r="B23" s="80"/>
+      <c r="C23" s="80"/>
+      <c r="D23" s="80"/>
+      <c r="E23" s="80"/>
+      <c r="F23" s="80"/>
+      <c r="G23" s="80"/>
+      <c r="H23" s="80"/>
+      <c r="I23" s="80"/>
+      <c r="J23" s="80"/>
+      <c r="K23" s="58" t="s">
         <v>114</v>
       </c>
       <c r="L23" s="5"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="19" t="s">
+      <c r="M23" s="9"/>
+      <c r="N23" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="O23" s="164"/>
-      <c r="P23" s="165"/>
-      <c r="Q23" s="164"/>
-      <c r="R23" s="252"/>
+      <c r="O23" s="166"/>
+      <c r="P23" s="189"/>
+      <c r="Q23" s="166"/>
+      <c r="R23" s="168"/>
     </row>
     <row r="24" spans="1:18" s="3" customFormat="1" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A24" s="57" t="s">
+      <c r="A24" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="D24" s="27" t="s">
+      <c r="D24" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="E24" s="27" t="s">
+      <c r="E24" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="F24" s="27" t="s">
+      <c r="F24" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="G24" s="27" t="s">
+      <c r="G24" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="H24" s="25" t="s">
+      <c r="H24" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="I24" s="58" t="s">
+      <c r="I24" s="57" t="s">
         <v>84</v>
       </c>
       <c r="J24" s="4"/>
@@ -5120,312 +5156,306 @@
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
-      <c r="R24" s="70"/>
+      <c r="R24" s="69"/>
     </row>
     <row r="25" spans="1:18" s="3" customFormat="1" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A25" s="60" t="s">
+      <c r="A25" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="61" t="s">
+      <c r="B25" s="60" t="s">
         <v>95</v>
       </c>
-      <c r="C25" s="61" t="s">
+      <c r="C25" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="D25" s="62" t="s">
+      <c r="D25" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="E25" s="61" t="s">
+      <c r="E25" s="60" t="s">
         <v>98</v>
       </c>
-      <c r="F25" s="61" t="s">
+      <c r="F25" s="60" t="s">
         <v>99</v>
       </c>
-      <c r="G25" s="61" t="s">
+      <c r="G25" s="60" t="s">
         <v>100</v>
       </c>
-      <c r="H25" s="63" t="s">
+      <c r="H25" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="I25" s="64" t="s">
+      <c r="I25" s="63" t="s">
         <v>34</v>
       </c>
       <c r="J25" s="4"/>
-      <c r="K25" s="288" t="s">
+      <c r="K25" s="281" t="s">
         <v>148</v>
       </c>
-      <c r="L25" s="289"/>
-      <c r="M25" s="289"/>
-      <c r="N25" s="289"/>
-      <c r="O25" s="289"/>
-      <c r="P25" s="289"/>
-      <c r="Q25" s="289"/>
-      <c r="R25" s="290"/>
+      <c r="L25" s="282"/>
+      <c r="M25" s="282"/>
+      <c r="N25" s="282"/>
+      <c r="O25" s="282"/>
+      <c r="P25" s="282"/>
+      <c r="Q25" s="282"/>
+      <c r="R25" s="283"/>
     </row>
     <row r="26" spans="1:18" ht="21.75" customHeight="1">
-      <c r="A26" s="65" t="s">
+      <c r="A26" s="64" t="s">
         <v>86</v>
       </c>
-      <c r="B26" s="66"/>
-      <c r="C26" s="66"/>
-      <c r="D26" s="66"/>
-      <c r="E26" s="66"/>
-      <c r="F26" s="66"/>
-      <c r="G26" s="66"/>
-      <c r="H26" s="66"/>
-      <c r="I26" s="67"/>
-      <c r="J26" s="81"/>
-      <c r="K26" s="74" t="s">
+      <c r="B26" s="65"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="65"/>
+      <c r="E26" s="65"/>
+      <c r="F26" s="65"/>
+      <c r="G26" s="65"/>
+      <c r="H26" s="65"/>
+      <c r="I26" s="66"/>
+      <c r="J26" s="80"/>
+      <c r="K26" s="73" t="s">
         <v>120</v>
       </c>
-      <c r="L26" s="75"/>
-      <c r="M26" s="76"/>
-      <c r="N26" s="239" t="s">
+      <c r="L26" s="74"/>
+      <c r="M26" s="75"/>
+      <c r="N26" s="177" t="s">
         <v>122</v>
       </c>
-      <c r="O26" s="240"/>
-      <c r="P26" s="241"/>
-      <c r="Q26" s="240" t="s">
+      <c r="O26" s="193"/>
+      <c r="P26" s="178"/>
+      <c r="Q26" s="193" t="s">
         <v>123</v>
       </c>
-      <c r="R26" s="291"/>
+      <c r="R26" s="285"/>
     </row>
     <row r="27" spans="1:18" ht="21.75" customHeight="1">
-      <c r="A27" s="87"/>
-      <c r="B27" s="88"/>
-      <c r="C27" s="88"/>
-      <c r="D27" s="88"/>
-      <c r="E27" s="88"/>
-      <c r="F27" s="88"/>
-      <c r="G27" s="88"/>
-      <c r="H27" s="88"/>
-      <c r="I27" s="89"/>
-      <c r="J27" s="81"/>
-      <c r="K27" s="96" t="s">
+      <c r="A27" s="86"/>
+      <c r="B27" s="87"/>
+      <c r="C27" s="87"/>
+      <c r="D27" s="87"/>
+      <c r="E27" s="87"/>
+      <c r="F27" s="87"/>
+      <c r="G27" s="87"/>
+      <c r="H27" s="87"/>
+      <c r="I27" s="88"/>
+      <c r="J27" s="80"/>
+      <c r="K27" s="95" t="s">
         <v>149</v>
       </c>
-      <c r="L27" s="72"/>
-      <c r="M27" s="73"/>
-      <c r="N27" s="203"/>
-      <c r="O27" s="306"/>
-      <c r="P27" s="204"/>
-      <c r="Q27" s="203"/>
-      <c r="R27" s="308"/>
+      <c r="L27" s="71"/>
+      <c r="M27" s="72"/>
+      <c r="N27" s="309"/>
+      <c r="O27" s="310"/>
+      <c r="P27" s="311"/>
+      <c r="Q27" s="309"/>
+      <c r="R27" s="312"/>
     </row>
     <row r="28" spans="1:18" ht="21.75" customHeight="1">
-      <c r="A28" s="90"/>
-      <c r="B28" s="91"/>
-      <c r="C28" s="91"/>
-      <c r="D28" s="91"/>
-      <c r="E28" s="91"/>
-      <c r="F28" s="91"/>
-      <c r="G28" s="91"/>
-      <c r="H28" s="91"/>
-      <c r="I28" s="92"/>
-      <c r="J28" s="81"/>
-      <c r="K28" s="96" t="s">
+      <c r="A28" s="89"/>
+      <c r="B28" s="90"/>
+      <c r="C28" s="90"/>
+      <c r="D28" s="90"/>
+      <c r="E28" s="90"/>
+      <c r="F28" s="90"/>
+      <c r="G28" s="90"/>
+      <c r="H28" s="90"/>
+      <c r="I28" s="91"/>
+      <c r="J28" s="80"/>
+      <c r="K28" s="95" t="s">
         <v>121</v>
       </c>
-      <c r="L28" s="72"/>
-      <c r="M28" s="73"/>
-      <c r="N28" s="203"/>
-      <c r="O28" s="306"/>
-      <c r="P28" s="204"/>
-      <c r="Q28" s="203"/>
-      <c r="R28" s="308"/>
+      <c r="L28" s="71"/>
+      <c r="M28" s="72"/>
+      <c r="N28" s="309"/>
+      <c r="O28" s="310"/>
+      <c r="P28" s="311"/>
+      <c r="Q28" s="309"/>
+      <c r="R28" s="312"/>
     </row>
     <row r="29" spans="1:18" ht="21.75" customHeight="1">
-      <c r="A29" s="90"/>
-      <c r="B29" s="91"/>
-      <c r="C29" s="91"/>
-      <c r="D29" s="91"/>
-      <c r="E29" s="91"/>
-      <c r="F29" s="91"/>
-      <c r="G29" s="91"/>
-      <c r="H29" s="91"/>
-      <c r="I29" s="92"/>
-      <c r="J29" s="81"/>
-      <c r="K29" s="77" t="s">
+      <c r="A29" s="89"/>
+      <c r="B29" s="90"/>
+      <c r="C29" s="90"/>
+      <c r="D29" s="90"/>
+      <c r="E29" s="90"/>
+      <c r="F29" s="90"/>
+      <c r="G29" s="90"/>
+      <c r="H29" s="90"/>
+      <c r="I29" s="91"/>
+      <c r="J29" s="80"/>
+      <c r="K29" s="76" t="s">
         <v>150</v>
       </c>
-      <c r="L29" s="78"/>
-      <c r="M29" s="79"/>
-      <c r="N29" s="203"/>
-      <c r="O29" s="306"/>
-      <c r="P29" s="204"/>
-      <c r="Q29" s="203"/>
-      <c r="R29" s="308"/>
+      <c r="L29" s="77"/>
+      <c r="M29" s="78"/>
+      <c r="N29" s="309"/>
+      <c r="O29" s="310"/>
+      <c r="P29" s="311"/>
+      <c r="Q29" s="309"/>
+      <c r="R29" s="312"/>
     </row>
     <row r="30" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A30" s="90"/>
-      <c r="B30" s="91"/>
-      <c r="C30" s="91"/>
-      <c r="D30" s="91"/>
-      <c r="E30" s="91"/>
-      <c r="F30" s="91"/>
-      <c r="G30" s="91"/>
-      <c r="H30" s="91"/>
-      <c r="I30" s="92"/>
-      <c r="J30" s="81"/>
-      <c r="K30" s="97" t="s">
+      <c r="A30" s="89"/>
+      <c r="B30" s="90"/>
+      <c r="C30" s="90"/>
+      <c r="D30" s="90"/>
+      <c r="E30" s="90"/>
+      <c r="F30" s="90"/>
+      <c r="G30" s="90"/>
+      <c r="H30" s="90"/>
+      <c r="I30" s="91"/>
+      <c r="J30" s="80"/>
+      <c r="K30" s="96" t="s">
         <v>151</v>
       </c>
-      <c r="L30" s="53"/>
-      <c r="M30" s="52"/>
-      <c r="N30" s="249"/>
-      <c r="O30" s="307"/>
-      <c r="P30" s="250"/>
-      <c r="Q30" s="249"/>
-      <c r="R30" s="309"/>
+      <c r="L30" s="52"/>
+      <c r="M30" s="51"/>
+      <c r="N30" s="313"/>
+      <c r="O30" s="314"/>
+      <c r="P30" s="315"/>
+      <c r="Q30" s="313"/>
+      <c r="R30" s="316"/>
     </row>
     <row r="31" spans="1:18" ht="21.75" customHeight="1">
-      <c r="A31" s="90"/>
-      <c r="B31" s="91"/>
-      <c r="C31" s="91"/>
-      <c r="D31" s="91"/>
-      <c r="E31" s="91"/>
-      <c r="F31" s="91"/>
-      <c r="G31" s="91"/>
-      <c r="H31" s="91"/>
-      <c r="I31" s="92"/>
-      <c r="J31" s="81"/>
-      <c r="K31" s="48"/>
-      <c r="L31" s="49"/>
-      <c r="M31" s="49"/>
-      <c r="N31" s="49"/>
-      <c r="O31" s="49"/>
-      <c r="P31" s="49"/>
-      <c r="Q31" s="49"/>
-      <c r="R31" s="50"/>
+      <c r="A31" s="89"/>
+      <c r="B31" s="90"/>
+      <c r="C31" s="90"/>
+      <c r="D31" s="90"/>
+      <c r="E31" s="90"/>
+      <c r="F31" s="90"/>
+      <c r="G31" s="90"/>
+      <c r="H31" s="90"/>
+      <c r="I31" s="91"/>
+      <c r="J31" s="80"/>
+      <c r="K31" s="47"/>
+      <c r="L31" s="48"/>
+      <c r="M31" s="48"/>
+      <c r="N31" s="48"/>
+      <c r="O31" s="48"/>
+      <c r="P31" s="48"/>
+      <c r="Q31" s="48"/>
+      <c r="R31" s="49"/>
     </row>
     <row r="32" spans="1:18" ht="21.75" customHeight="1">
-      <c r="A32" s="90"/>
-      <c r="B32" s="91"/>
-      <c r="C32" s="91"/>
-      <c r="D32" s="91"/>
-      <c r="E32" s="91"/>
-      <c r="F32" s="91"/>
-      <c r="G32" s="91"/>
-      <c r="H32" s="91"/>
-      <c r="I32" s="92"/>
-      <c r="J32" s="81"/>
-      <c r="K32" s="105" t="s">
+      <c r="A32" s="89"/>
+      <c r="B32" s="90"/>
+      <c r="C32" s="90"/>
+      <c r="D32" s="90"/>
+      <c r="E32" s="90"/>
+      <c r="F32" s="90"/>
+      <c r="G32" s="90"/>
+      <c r="H32" s="90"/>
+      <c r="I32" s="91"/>
+      <c r="J32" s="80"/>
+      <c r="K32" s="104" t="s">
         <v>128</v>
       </c>
-      <c r="L32" s="81"/>
-      <c r="M32" s="292"/>
-      <c r="N32" s="292"/>
-      <c r="O32" s="292"/>
-      <c r="P32" s="292"/>
-      <c r="Q32" s="292"/>
-      <c r="R32" s="293"/>
+      <c r="L32" s="80"/>
+      <c r="M32" s="286"/>
+      <c r="N32" s="286"/>
+      <c r="O32" s="286"/>
+      <c r="P32" s="286"/>
+      <c r="Q32" s="286"/>
+      <c r="R32" s="287"/>
     </row>
     <row r="33" spans="1:18" ht="21.75" customHeight="1">
-      <c r="A33" s="90"/>
-      <c r="B33" s="91"/>
-      <c r="C33" s="91"/>
-      <c r="D33" s="91"/>
-      <c r="E33" s="91"/>
-      <c r="F33" s="91"/>
-      <c r="G33" s="91"/>
-      <c r="H33" s="91"/>
-      <c r="I33" s="92"/>
-      <c r="J33" s="81"/>
-      <c r="K33" s="80" t="s">
+      <c r="A33" s="89"/>
+      <c r="B33" s="90"/>
+      <c r="C33" s="90"/>
+      <c r="D33" s="90"/>
+      <c r="E33" s="90"/>
+      <c r="F33" s="90"/>
+      <c r="G33" s="90"/>
+      <c r="H33" s="90"/>
+      <c r="I33" s="91"/>
+      <c r="J33" s="80"/>
+      <c r="K33" s="79" t="s">
         <v>129</v>
       </c>
-      <c r="L33" s="81"/>
-      <c r="M33" s="81"/>
-      <c r="N33" s="81"/>
-      <c r="O33" s="81"/>
-      <c r="P33" s="81"/>
-      <c r="Q33" s="81"/>
-      <c r="R33" s="82"/>
+      <c r="L33" s="80"/>
+      <c r="M33" s="80"/>
+      <c r="N33" s="80"/>
+      <c r="O33" s="80"/>
+      <c r="P33" s="80"/>
+      <c r="Q33" s="80"/>
+      <c r="R33" s="81"/>
     </row>
     <row r="34" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A34" s="86"/>
-      <c r="B34" s="71"/>
-      <c r="C34" s="71"/>
-      <c r="D34" s="71"/>
-      <c r="E34" s="71"/>
-      <c r="F34" s="71"/>
-      <c r="G34" s="71"/>
-      <c r="H34" s="71"/>
-      <c r="I34" s="54"/>
-      <c r="J34" s="81"/>
-      <c r="K34" s="80" t="s">
+      <c r="A34" s="85"/>
+      <c r="B34" s="70"/>
+      <c r="C34" s="70"/>
+      <c r="D34" s="70"/>
+      <c r="E34" s="70"/>
+      <c r="F34" s="70"/>
+      <c r="G34" s="70"/>
+      <c r="H34" s="70"/>
+      <c r="I34" s="53"/>
+      <c r="J34" s="80"/>
+      <c r="K34" s="79" t="s">
         <v>130</v>
       </c>
-      <c r="L34" s="81"/>
-      <c r="M34" s="81"/>
-      <c r="N34" s="81"/>
-      <c r="O34" s="81"/>
-      <c r="P34" s="81"/>
-      <c r="Q34" s="81"/>
-      <c r="R34" s="82"/>
+      <c r="L34" s="80"/>
+      <c r="M34" s="80"/>
+      <c r="N34" s="80"/>
+      <c r="O34" s="80"/>
+      <c r="P34" s="80"/>
+      <c r="Q34" s="80"/>
+      <c r="R34" s="81"/>
     </row>
     <row r="35" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A35" s="285" t="s">
+      <c r="A35" s="278" t="s">
         <v>85</v>
       </c>
-      <c r="B35" s="286"/>
-      <c r="C35" s="286"/>
-      <c r="D35" s="287"/>
-      <c r="E35" s="71"/>
-      <c r="F35" s="71"/>
-      <c r="G35" s="71"/>
-      <c r="H35" s="71"/>
-      <c r="I35" s="54"/>
-      <c r="J35" s="81"/>
-      <c r="K35" s="51"/>
-      <c r="L35" s="53"/>
-      <c r="M35" s="53"/>
-      <c r="N35" s="53"/>
-      <c r="O35" s="53"/>
-      <c r="P35" s="53"/>
-      <c r="Q35" s="53"/>
-      <c r="R35" s="106" t="s">
+      <c r="B35" s="279"/>
+      <c r="C35" s="279"/>
+      <c r="D35" s="280"/>
+      <c r="E35" s="70"/>
+      <c r="F35" s="70"/>
+      <c r="G35" s="70"/>
+      <c r="H35" s="70"/>
+      <c r="I35" s="53"/>
+      <c r="J35" s="80"/>
+      <c r="K35" s="50"/>
+      <c r="L35" s="52"/>
+      <c r="M35" s="52"/>
+      <c r="N35" s="52"/>
+      <c r="O35" s="52"/>
+      <c r="P35" s="52"/>
+      <c r="Q35" s="52"/>
+      <c r="R35" s="105" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:18" ht="20.399999999999999">
-      <c r="A36" s="102" t="s">
+      <c r="A36" s="101" t="s">
         <v>173</v>
       </c>
-      <c r="B36" s="103"/>
-      <c r="C36" s="103"/>
-      <c r="D36" s="103"/>
-      <c r="E36" s="103"/>
-      <c r="F36" s="103"/>
-      <c r="G36" s="104"/>
-      <c r="Q36" s="283" t="s">
+      <c r="B36" s="102"/>
+      <c r="C36" s="102"/>
+      <c r="D36" s="102"/>
+      <c r="E36" s="102"/>
+      <c r="F36" s="102"/>
+      <c r="G36" s="103"/>
+      <c r="Q36" s="276" t="s">
         <v>154</v>
       </c>
-      <c r="R36" s="284"/>
+      <c r="R36" s="277"/>
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="N27:P27"/>
-    <mergeCell ref="N28:P28"/>
-    <mergeCell ref="N29:P29"/>
-    <mergeCell ref="N30:P30"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="Q30:R30"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="Q20:R20"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="A5:B6"/>
+    <mergeCell ref="C5:D6"/>
+    <mergeCell ref="E5:F6"/>
+    <mergeCell ref="G5:I6"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="K4:R4"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="P11:R11"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
     <mergeCell ref="Q36:R36"/>
     <mergeCell ref="A35:D35"/>
     <mergeCell ref="K25:R25"/>
@@ -5442,27 +5472,33 @@
     <mergeCell ref="Q19:R19"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="E21:F21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
     <mergeCell ref="G21:I21"/>
     <mergeCell ref="N12:O12"/>
     <mergeCell ref="N9:O9"/>
     <mergeCell ref="P9:R9"/>
     <mergeCell ref="N10:O10"/>
     <mergeCell ref="P10:R10"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="P11:R11"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="K4:R4"/>
-    <mergeCell ref="A5:B6"/>
-    <mergeCell ref="C5:D6"/>
-    <mergeCell ref="E5:F6"/>
-    <mergeCell ref="G5:I6"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="N30:P30"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="N27:P27"/>
+    <mergeCell ref="N28:P28"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
M3 Cord Production System #1009 - S8 Production Condition Update Structure #4 (export)
</commit_message>
<xml_diff>
--- a/05.Controls/M3.Cord.Controls/Resources/Excels/FMCS11_S8.xlsx
+++ b/05.Controls/M3.Cord.Controls/Resources/Excels/FMCS11_S8.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="72" windowWidth="11712" windowHeight="6456" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="72" windowWidth="11712" windowHeight="6456"/>
   </bookViews>
   <sheets>
     <sheet name="FM-CS-11" sheetId="4" r:id="rId1"/>
@@ -936,16 +936,15 @@
       <charset val="2"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="14"/>
       <name val="Wingdings 2"/>
       <family val="1"/>
       <charset val="2"/>
     </font>
     <font>
-      <sz val="14"/>
-      <name val="Wingdings 2"/>
+      <sz val="22"/>
+      <name val="AngsanaUPC"/>
       <family val="1"/>
-      <charset val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -2322,358 +2321,394 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2681,15 +2716,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2699,7 +2725,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2711,16 +2737,37 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2729,82 +2776,34 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3220,8 +3219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AU48"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6:S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="23.4"/>
@@ -3248,78 +3247,78 @@
   <sheetData>
     <row r="1" spans="1:47" ht="6" customHeight="1" thickBot="1"/>
     <row r="2" spans="1:47" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A2" s="225" t="s">
+      <c r="A2" s="229" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="225"/>
-      <c r="C2" s="225"/>
-      <c r="D2" s="225"/>
-      <c r="E2" s="225"/>
-      <c r="F2" s="225"/>
-      <c r="G2" s="225"/>
-      <c r="H2" s="225"/>
-      <c r="I2" s="225"/>
-      <c r="J2" s="225"/>
-      <c r="K2" s="225"/>
-      <c r="L2" s="225"/>
-      <c r="M2" s="225"/>
-      <c r="N2" s="225"/>
-      <c r="O2" s="225"/>
-      <c r="P2" s="225"/>
-      <c r="Q2" s="225"/>
-      <c r="R2" s="226"/>
-      <c r="S2" s="213" t="s">
+      <c r="B2" s="229"/>
+      <c r="C2" s="229"/>
+      <c r="D2" s="229"/>
+      <c r="E2" s="229"/>
+      <c r="F2" s="229"/>
+      <c r="G2" s="229"/>
+      <c r="H2" s="229"/>
+      <c r="I2" s="229"/>
+      <c r="J2" s="229"/>
+      <c r="K2" s="229"/>
+      <c r="L2" s="229"/>
+      <c r="M2" s="229"/>
+      <c r="N2" s="229"/>
+      <c r="O2" s="229"/>
+      <c r="P2" s="229"/>
+      <c r="Q2" s="229"/>
+      <c r="R2" s="230"/>
+      <c r="S2" s="217" t="s">
         <v>155</v>
       </c>
-      <c r="T2" s="214"/>
-      <c r="U2" s="215"/>
-      <c r="V2" s="213" t="s">
+      <c r="T2" s="218"/>
+      <c r="U2" s="219"/>
+      <c r="V2" s="217" t="s">
         <v>156</v>
       </c>
-      <c r="W2" s="214"/>
-      <c r="X2" s="215"/>
-      <c r="Z2" s="216"/>
-      <c r="AA2" s="216"/>
-      <c r="AB2" s="216"/>
-      <c r="AC2" s="216"/>
-      <c r="AD2" s="216"/>
-      <c r="AE2" s="216"/>
-      <c r="AF2" s="216"/>
-      <c r="AG2" s="216"/>
-      <c r="AH2" s="216"/>
-      <c r="AI2" s="216"/>
-      <c r="AJ2" s="216"/>
-      <c r="AK2" s="216"/>
-      <c r="AL2" s="216"/>
-      <c r="AM2" s="216"/>
-      <c r="AN2" s="216"/>
-      <c r="AO2" s="216"/>
-      <c r="AP2" s="216"/>
-      <c r="AQ2" s="216"/>
-      <c r="AR2" s="216"/>
-      <c r="AS2" s="216"/>
-      <c r="AT2" s="216"/>
-      <c r="AU2" s="216"/>
+      <c r="W2" s="218"/>
+      <c r="X2" s="219"/>
+      <c r="Z2" s="220"/>
+      <c r="AA2" s="220"/>
+      <c r="AB2" s="220"/>
+      <c r="AC2" s="220"/>
+      <c r="AD2" s="220"/>
+      <c r="AE2" s="220"/>
+      <c r="AF2" s="220"/>
+      <c r="AG2" s="220"/>
+      <c r="AH2" s="220"/>
+      <c r="AI2" s="220"/>
+      <c r="AJ2" s="220"/>
+      <c r="AK2" s="220"/>
+      <c r="AL2" s="220"/>
+      <c r="AM2" s="220"/>
+      <c r="AN2" s="220"/>
+      <c r="AO2" s="220"/>
+      <c r="AP2" s="220"/>
+      <c r="AQ2" s="220"/>
+      <c r="AR2" s="220"/>
+      <c r="AS2" s="220"/>
+      <c r="AT2" s="220"/>
+      <c r="AU2" s="220"/>
     </row>
     <row r="3" spans="1:47" ht="39.75" customHeight="1" thickBot="1">
-      <c r="A3" s="227"/>
-      <c r="B3" s="227"/>
-      <c r="C3" s="227"/>
-      <c r="D3" s="227"/>
-      <c r="E3" s="227"/>
-      <c r="F3" s="227"/>
-      <c r="G3" s="227"/>
-      <c r="H3" s="227"/>
-      <c r="I3" s="227"/>
-      <c r="J3" s="227"/>
-      <c r="K3" s="227"/>
-      <c r="L3" s="227"/>
-      <c r="M3" s="227"/>
-      <c r="N3" s="227"/>
-      <c r="O3" s="227"/>
-      <c r="P3" s="227"/>
-      <c r="Q3" s="227"/>
-      <c r="R3" s="228"/>
+      <c r="A3" s="231"/>
+      <c r="B3" s="231"/>
+      <c r="C3" s="231"/>
+      <c r="D3" s="231"/>
+      <c r="E3" s="231"/>
+      <c r="F3" s="231"/>
+      <c r="G3" s="231"/>
+      <c r="H3" s="231"/>
+      <c r="I3" s="231"/>
+      <c r="J3" s="231"/>
+      <c r="K3" s="231"/>
+      <c r="L3" s="231"/>
+      <c r="M3" s="231"/>
+      <c r="N3" s="231"/>
+      <c r="O3" s="231"/>
+      <c r="P3" s="231"/>
+      <c r="Q3" s="231"/>
+      <c r="R3" s="232"/>
       <c r="S3" s="107"/>
       <c r="T3" s="108"/>
       <c r="U3" s="106"/>
@@ -3328,182 +3327,182 @@
       <c r="X3" s="44"/>
     </row>
     <row r="4" spans="1:47" s="2" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A4" s="217" t="s">
+      <c r="A4" s="221" t="s">
         <v>163</v>
       </c>
-      <c r="B4" s="218"/>
-      <c r="C4" s="219" t="s">
+      <c r="B4" s="222"/>
+      <c r="C4" s="223" t="s">
         <v>164</v>
       </c>
-      <c r="D4" s="220"/>
-      <c r="E4" s="218"/>
-      <c r="F4" s="219" t="s">
+      <c r="D4" s="224"/>
+      <c r="E4" s="222"/>
+      <c r="F4" s="223" t="s">
         <v>165</v>
       </c>
-      <c r="G4" s="220"/>
-      <c r="H4" s="220"/>
-      <c r="I4" s="218"/>
-      <c r="J4" s="220" t="s">
+      <c r="G4" s="224"/>
+      <c r="H4" s="224"/>
+      <c r="I4" s="222"/>
+      <c r="J4" s="224" t="s">
         <v>166</v>
       </c>
-      <c r="K4" s="220"/>
-      <c r="L4" s="220"/>
-      <c r="M4" s="218"/>
-      <c r="N4" s="220" t="s">
+      <c r="K4" s="224"/>
+      <c r="L4" s="224"/>
+      <c r="M4" s="222"/>
+      <c r="N4" s="224" t="s">
         <v>167</v>
       </c>
-      <c r="O4" s="220"/>
-      <c r="P4" s="220"/>
-      <c r="Q4" s="218"/>
-      <c r="R4" s="221" t="s">
+      <c r="O4" s="224"/>
+      <c r="P4" s="224"/>
+      <c r="Q4" s="222"/>
+      <c r="R4" s="225" t="s">
         <v>168</v>
       </c>
-      <c r="S4" s="222"/>
-      <c r="T4" s="221" t="s">
+      <c r="S4" s="226"/>
+      <c r="T4" s="225" t="s">
         <v>169</v>
       </c>
-      <c r="U4" s="223"/>
-      <c r="V4" s="223"/>
-      <c r="W4" s="223"/>
-      <c r="X4" s="224"/>
+      <c r="U4" s="227"/>
+      <c r="V4" s="227"/>
+      <c r="W4" s="227"/>
+      <c r="X4" s="228"/>
     </row>
     <row r="5" spans="1:47" s="3" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A5" s="241"/>
-      <c r="B5" s="242"/>
-      <c r="C5" s="256"/>
-      <c r="D5" s="257"/>
-      <c r="E5" s="242"/>
-      <c r="F5" s="260"/>
-      <c r="G5" s="261"/>
-      <c r="H5" s="261"/>
-      <c r="I5" s="262"/>
-      <c r="J5" s="157" t="s">
+      <c r="A5" s="161"/>
+      <c r="B5" s="162"/>
+      <c r="C5" s="188"/>
+      <c r="D5" s="189"/>
+      <c r="E5" s="162"/>
+      <c r="F5" s="193"/>
+      <c r="G5" s="194"/>
+      <c r="H5" s="194"/>
+      <c r="I5" s="195"/>
+      <c r="J5" s="208" t="s">
         <v>140</v>
       </c>
-      <c r="K5" s="231"/>
-      <c r="L5" s="231"/>
-      <c r="M5" s="232"/>
-      <c r="N5" s="157" t="s">
+      <c r="K5" s="209"/>
+      <c r="L5" s="209"/>
+      <c r="M5" s="210"/>
+      <c r="N5" s="208" t="s">
         <v>140</v>
       </c>
-      <c r="O5" s="231"/>
-      <c r="P5" s="231"/>
-      <c r="Q5" s="232"/>
+      <c r="O5" s="209"/>
+      <c r="P5" s="209"/>
+      <c r="Q5" s="210"/>
       <c r="R5" s="41" t="s">
         <v>9</v>
       </c>
       <c r="S5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="T5" s="229" t="s">
+      <c r="T5" s="202" t="s">
         <v>0</v>
       </c>
-      <c r="U5" s="230"/>
-      <c r="V5" s="157" t="s">
+      <c r="U5" s="203"/>
+      <c r="V5" s="208" t="s">
         <v>2</v>
       </c>
-      <c r="W5" s="158"/>
-      <c r="X5" s="159"/>
+      <c r="W5" s="267"/>
+      <c r="X5" s="268"/>
     </row>
     <row r="6" spans="1:47" s="3" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A6" s="243"/>
-      <c r="B6" s="244"/>
-      <c r="C6" s="258"/>
-      <c r="D6" s="259"/>
-      <c r="E6" s="244"/>
-      <c r="F6" s="263"/>
-      <c r="G6" s="264"/>
-      <c r="H6" s="264"/>
-      <c r="I6" s="265"/>
-      <c r="J6" s="249"/>
-      <c r="K6" s="250"/>
-      <c r="L6" s="250"/>
-      <c r="M6" s="251"/>
-      <c r="N6" s="235"/>
-      <c r="O6" s="236"/>
-      <c r="P6" s="236"/>
-      <c r="Q6" s="237"/>
-      <c r="R6" s="233"/>
-      <c r="S6" s="233"/>
-      <c r="T6" s="209" t="s">
+      <c r="A6" s="163"/>
+      <c r="B6" s="164"/>
+      <c r="C6" s="190"/>
+      <c r="D6" s="191"/>
+      <c r="E6" s="164"/>
+      <c r="F6" s="196"/>
+      <c r="G6" s="197"/>
+      <c r="H6" s="197"/>
+      <c r="I6" s="198"/>
+      <c r="J6" s="178"/>
+      <c r="K6" s="179"/>
+      <c r="L6" s="179"/>
+      <c r="M6" s="180"/>
+      <c r="N6" s="211"/>
+      <c r="O6" s="212"/>
+      <c r="P6" s="212"/>
+      <c r="Q6" s="213"/>
+      <c r="R6" s="318"/>
+      <c r="S6" s="318"/>
+      <c r="T6" s="204" t="s">
         <v>1</v>
       </c>
-      <c r="U6" s="210"/>
-      <c r="V6" s="160" t="s">
+      <c r="U6" s="205"/>
+      <c r="V6" s="171" t="s">
         <v>67</v>
       </c>
-      <c r="W6" s="161"/>
-      <c r="X6" s="162"/>
+      <c r="W6" s="192"/>
+      <c r="X6" s="269"/>
     </row>
     <row r="7" spans="1:47" s="3" customFormat="1" ht="21" customHeight="1">
-      <c r="A7" s="187"/>
-      <c r="B7" s="188"/>
-      <c r="C7" s="160"/>
-      <c r="D7" s="161"/>
-      <c r="E7" s="188"/>
-      <c r="F7" s="266"/>
-      <c r="G7" s="267"/>
-      <c r="H7" s="267"/>
-      <c r="I7" s="268"/>
-      <c r="J7" s="252"/>
-      <c r="K7" s="253"/>
-      <c r="L7" s="253"/>
-      <c r="M7" s="254"/>
-      <c r="N7" s="238"/>
-      <c r="O7" s="239"/>
-      <c r="P7" s="239"/>
-      <c r="Q7" s="240"/>
-      <c r="R7" s="234"/>
-      <c r="S7" s="234"/>
-      <c r="T7" s="207" t="s">
+      <c r="A7" s="165"/>
+      <c r="B7" s="166"/>
+      <c r="C7" s="171"/>
+      <c r="D7" s="192"/>
+      <c r="E7" s="166"/>
+      <c r="F7" s="199"/>
+      <c r="G7" s="200"/>
+      <c r="H7" s="200"/>
+      <c r="I7" s="201"/>
+      <c r="J7" s="181"/>
+      <c r="K7" s="182"/>
+      <c r="L7" s="182"/>
+      <c r="M7" s="183"/>
+      <c r="N7" s="214"/>
+      <c r="O7" s="215"/>
+      <c r="P7" s="215"/>
+      <c r="Q7" s="216"/>
+      <c r="R7" s="319"/>
+      <c r="S7" s="319"/>
+      <c r="T7" s="206" t="s">
         <v>3</v>
       </c>
-      <c r="U7" s="208"/>
-      <c r="V7" s="163"/>
-      <c r="W7" s="164"/>
-      <c r="X7" s="165"/>
+      <c r="U7" s="207"/>
+      <c r="V7" s="176"/>
+      <c r="W7" s="177"/>
+      <c r="X7" s="270"/>
     </row>
     <row r="8" spans="1:47" s="3" customFormat="1" ht="19.8">
-      <c r="A8" s="248" t="s">
+      <c r="A8" s="174" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="206"/>
-      <c r="C8" s="163" t="s">
+      <c r="B8" s="175"/>
+      <c r="C8" s="176" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="164"/>
-      <c r="E8" s="206"/>
-      <c r="F8" s="163" t="s">
+      <c r="D8" s="177"/>
+      <c r="E8" s="175"/>
+      <c r="F8" s="176" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="206"/>
-      <c r="H8" s="163" t="s">
+      <c r="G8" s="175"/>
+      <c r="H8" s="176" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="206"/>
-      <c r="J8" s="164" t="s">
+      <c r="I8" s="175"/>
+      <c r="J8" s="177" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="164"/>
-      <c r="L8" s="164"/>
-      <c r="M8" s="206"/>
-      <c r="N8" s="164" t="s">
+      <c r="K8" s="177"/>
+      <c r="L8" s="177"/>
+      <c r="M8" s="175"/>
+      <c r="N8" s="177" t="s">
         <v>19</v>
       </c>
-      <c r="O8" s="164"/>
-      <c r="P8" s="164"/>
-      <c r="Q8" s="206"/>
-      <c r="R8" s="211" t="s">
+      <c r="O8" s="177"/>
+      <c r="P8" s="177"/>
+      <c r="Q8" s="175"/>
+      <c r="R8" s="233" t="s">
         <v>7</v>
       </c>
-      <c r="S8" s="212"/>
-      <c r="T8" s="207" t="s">
+      <c r="S8" s="234"/>
+      <c r="T8" s="206" t="s">
         <v>4</v>
       </c>
-      <c r="U8" s="208"/>
-      <c r="V8" s="163"/>
-      <c r="W8" s="164"/>
-      <c r="X8" s="165"/>
+      <c r="U8" s="207"/>
+      <c r="V8" s="176"/>
+      <c r="W8" s="177"/>
+      <c r="X8" s="270"/>
     </row>
     <row r="9" spans="1:47" s="3" customFormat="1" ht="21" customHeight="1">
       <c r="A9" s="21" t="s">
@@ -3512,68 +3511,68 @@
       <c r="B9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="245"/>
-      <c r="D9" s="201"/>
-      <c r="E9" s="186"/>
-      <c r="F9" s="197"/>
-      <c r="G9" s="198"/>
-      <c r="H9" s="201"/>
-      <c r="I9" s="186"/>
-      <c r="J9" s="163" t="s">
+      <c r="C9" s="169"/>
+      <c r="D9" s="184"/>
+      <c r="E9" s="170"/>
+      <c r="F9" s="246"/>
+      <c r="G9" s="247"/>
+      <c r="H9" s="184"/>
+      <c r="I9" s="170"/>
+      <c r="J9" s="176" t="s">
         <v>17</v>
       </c>
-      <c r="K9" s="206"/>
-      <c r="L9" s="164" t="s">
+      <c r="K9" s="175"/>
+      <c r="L9" s="177" t="s">
         <v>18</v>
       </c>
-      <c r="M9" s="206"/>
-      <c r="N9" s="163" t="s">
+      <c r="M9" s="175"/>
+      <c r="N9" s="176" t="s">
         <v>17</v>
       </c>
-      <c r="O9" s="206"/>
-      <c r="P9" s="164" t="s">
+      <c r="O9" s="175"/>
+      <c r="P9" s="177" t="s">
         <v>18</v>
       </c>
-      <c r="Q9" s="206"/>
-      <c r="R9" s="209" t="s">
+      <c r="Q9" s="175"/>
+      <c r="R9" s="204" t="s">
         <v>8</v>
       </c>
-      <c r="S9" s="210"/>
-      <c r="T9" s="207" t="s">
+      <c r="S9" s="205"/>
+      <c r="T9" s="206" t="s">
         <v>5</v>
       </c>
-      <c r="U9" s="208"/>
-      <c r="V9" s="163"/>
-      <c r="W9" s="164"/>
-      <c r="X9" s="165"/>
+      <c r="U9" s="207"/>
+      <c r="V9" s="176"/>
+      <c r="W9" s="177"/>
+      <c r="X9" s="270"/>
     </row>
     <row r="10" spans="1:47" s="3" customFormat="1" ht="29.25" customHeight="1" thickBot="1">
       <c r="A10" s="155"/>
       <c r="B10" s="156"/>
-      <c r="C10" s="255"/>
-      <c r="D10" s="202"/>
-      <c r="E10" s="203"/>
-      <c r="F10" s="199"/>
-      <c r="G10" s="200"/>
-      <c r="H10" s="202"/>
-      <c r="I10" s="203"/>
-      <c r="J10" s="166"/>
-      <c r="K10" s="189"/>
-      <c r="L10" s="166"/>
-      <c r="M10" s="189"/>
-      <c r="N10" s="166"/>
-      <c r="O10" s="189"/>
-      <c r="P10" s="166"/>
-      <c r="Q10" s="189"/>
-      <c r="R10" s="204"/>
-      <c r="S10" s="205"/>
-      <c r="T10" s="191" t="s">
+      <c r="C10" s="185"/>
+      <c r="D10" s="186"/>
+      <c r="E10" s="187"/>
+      <c r="F10" s="248"/>
+      <c r="G10" s="249"/>
+      <c r="H10" s="186"/>
+      <c r="I10" s="187"/>
+      <c r="J10" s="167"/>
+      <c r="K10" s="168"/>
+      <c r="L10" s="167"/>
+      <c r="M10" s="168"/>
+      <c r="N10" s="167"/>
+      <c r="O10" s="168"/>
+      <c r="P10" s="167"/>
+      <c r="Q10" s="168"/>
+      <c r="R10" s="250"/>
+      <c r="S10" s="251"/>
+      <c r="T10" s="238" t="s">
         <v>20</v>
       </c>
-      <c r="U10" s="192"/>
-      <c r="V10" s="166"/>
-      <c r="W10" s="167"/>
-      <c r="X10" s="168"/>
+      <c r="U10" s="239"/>
+      <c r="V10" s="167"/>
+      <c r="W10" s="252"/>
+      <c r="X10" s="253"/>
     </row>
     <row r="11" spans="1:47" s="3" customFormat="1" ht="9.75" customHeight="1" thickBot="1"/>
     <row r="12" spans="1:47" s="3" customFormat="1" ht="20.25" customHeight="1">
@@ -3583,15 +3582,15 @@
       <c r="B12" s="136" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="177" t="s">
+      <c r="C12" s="240" t="s">
         <v>72</v>
       </c>
-      <c r="D12" s="193"/>
-      <c r="E12" s="178"/>
-      <c r="F12" s="177" t="s">
+      <c r="D12" s="241"/>
+      <c r="E12" s="242"/>
+      <c r="F12" s="240" t="s">
         <v>71</v>
       </c>
-      <c r="G12" s="178"/>
+      <c r="G12" s="242"/>
       <c r="H12" s="141" t="s">
         <v>22</v>
       </c>
@@ -3607,22 +3606,22 @@
       <c r="L12" s="136" t="s">
         <v>23</v>
       </c>
-      <c r="M12" s="177" t="s">
+      <c r="M12" s="240" t="s">
         <v>70</v>
       </c>
-      <c r="N12" s="193"/>
-      <c r="O12" s="178"/>
-      <c r="P12" s="177" t="s">
+      <c r="N12" s="241"/>
+      <c r="O12" s="242"/>
+      <c r="P12" s="240" t="s">
         <v>69</v>
       </c>
-      <c r="Q12" s="193"/>
-      <c r="R12" s="193"/>
-      <c r="S12" s="178"/>
-      <c r="T12" s="194" t="s">
+      <c r="Q12" s="241"/>
+      <c r="R12" s="241"/>
+      <c r="S12" s="242"/>
+      <c r="T12" s="243" t="s">
         <v>60</v>
       </c>
-      <c r="U12" s="195"/>
-      <c r="V12" s="196"/>
+      <c r="U12" s="244"/>
+      <c r="V12" s="245"/>
       <c r="W12" s="139" t="s">
         <v>32</v>
       </c>
@@ -4168,14 +4167,14 @@
     <row r="31" spans="1:24" s="3" customFormat="1" ht="28.5" customHeight="1">
       <c r="A31" s="34"/>
       <c r="B31" s="36"/>
-      <c r="C31" s="177" t="s">
+      <c r="C31" s="240" t="s">
         <v>161</v>
       </c>
-      <c r="D31" s="178"/>
-      <c r="E31" s="177" t="s">
+      <c r="D31" s="242"/>
+      <c r="E31" s="240" t="s">
         <v>162</v>
       </c>
-      <c r="F31" s="178"/>
+      <c r="F31" s="242"/>
       <c r="G31" s="126" t="s">
         <v>73</v>
       </c>
@@ -4196,29 +4195,29 @@
       <c r="N31" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="O31" s="179" t="s">
+      <c r="O31" s="260" t="s">
         <v>78</v>
       </c>
-      <c r="P31" s="180"/>
-      <c r="Q31" s="180"/>
-      <c r="R31" s="180"/>
-      <c r="S31" s="180"/>
-      <c r="T31" s="180"/>
-      <c r="U31" s="180"/>
-      <c r="V31" s="180"/>
-      <c r="W31" s="180"/>
-      <c r="X31" s="181"/>
+      <c r="P31" s="261"/>
+      <c r="Q31" s="261"/>
+      <c r="R31" s="261"/>
+      <c r="S31" s="261"/>
+      <c r="T31" s="261"/>
+      <c r="U31" s="261"/>
+      <c r="V31" s="261"/>
+      <c r="W31" s="261"/>
+      <c r="X31" s="262"/>
     </row>
     <row r="32" spans="1:24" s="3" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A32" s="185" t="s">
+      <c r="A32" s="266" t="s">
         <v>158</v>
       </c>
-      <c r="B32" s="186"/>
-      <c r="C32" s="245"/>
-      <c r="D32" s="186"/>
-      <c r="E32" s="245"/>
-      <c r="F32" s="186"/>
-      <c r="G32" s="246"/>
+      <c r="B32" s="170"/>
+      <c r="C32" s="169"/>
+      <c r="D32" s="170"/>
+      <c r="E32" s="169"/>
+      <c r="F32" s="170"/>
+      <c r="G32" s="172"/>
       <c r="H32" s="32">
         <v>1</v>
       </c>
@@ -4234,29 +4233,29 @@
       </c>
       <c r="M32" s="16"/>
       <c r="N32" s="130"/>
-      <c r="O32" s="182" t="s">
+      <c r="O32" s="263" t="s">
         <v>139</v>
       </c>
-      <c r="P32" s="183"/>
-      <c r="Q32" s="183"/>
-      <c r="R32" s="172"/>
-      <c r="S32" s="171" t="s">
+      <c r="P32" s="264"/>
+      <c r="Q32" s="264"/>
+      <c r="R32" s="237"/>
+      <c r="S32" s="236" t="s">
         <v>79</v>
       </c>
-      <c r="T32" s="183"/>
-      <c r="U32" s="183"/>
-      <c r="V32" s="183"/>
-      <c r="W32" s="183"/>
-      <c r="X32" s="184"/>
+      <c r="T32" s="264"/>
+      <c r="U32" s="264"/>
+      <c r="V32" s="264"/>
+      <c r="W32" s="264"/>
+      <c r="X32" s="265"/>
     </row>
     <row r="33" spans="1:28" s="3" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A33" s="187"/>
-      <c r="B33" s="188"/>
-      <c r="C33" s="160"/>
-      <c r="D33" s="188"/>
-      <c r="E33" s="160"/>
-      <c r="F33" s="188"/>
-      <c r="G33" s="247"/>
+      <c r="A33" s="165"/>
+      <c r="B33" s="166"/>
+      <c r="C33" s="171"/>
+      <c r="D33" s="166"/>
+      <c r="E33" s="171"/>
+      <c r="F33" s="166"/>
+      <c r="G33" s="173"/>
       <c r="H33" s="131" t="s">
         <v>74</v>
       </c>
@@ -4287,21 +4286,21 @@
       </c>
       <c r="T33" s="116"/>
       <c r="U33" s="117"/>
-      <c r="V33" s="171">
+      <c r="V33" s="236">
         <v>4</v>
       </c>
-      <c r="W33" s="172"/>
+      <c r="W33" s="237"/>
       <c r="X33" s="118"/>
     </row>
     <row r="34" spans="1:28" s="3" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A34" s="169" t="s">
+      <c r="A34" s="254" t="s">
         <v>159</v>
       </c>
-      <c r="B34" s="170"/>
-      <c r="C34" s="163"/>
-      <c r="D34" s="206"/>
-      <c r="E34" s="163"/>
-      <c r="F34" s="206"/>
+      <c r="B34" s="255"/>
+      <c r="C34" s="176"/>
+      <c r="D34" s="175"/>
+      <c r="E34" s="176"/>
+      <c r="F34" s="175"/>
       <c r="G34" s="127"/>
       <c r="H34" s="133">
         <v>2</v>
@@ -4331,22 +4330,22 @@
       </c>
       <c r="T34" s="111"/>
       <c r="U34" s="112"/>
-      <c r="V34" s="171">
+      <c r="V34" s="236">
         <v>5</v>
       </c>
-      <c r="W34" s="172"/>
+      <c r="W34" s="237"/>
       <c r="X34" s="118"/>
       <c r="AB34" s="4"/>
     </row>
     <row r="35" spans="1:28" s="3" customFormat="1" ht="28.5" customHeight="1" thickBot="1">
-      <c r="A35" s="173" t="s">
+      <c r="A35" s="256" t="s">
         <v>160</v>
       </c>
-      <c r="B35" s="174"/>
-      <c r="C35" s="166"/>
-      <c r="D35" s="189"/>
-      <c r="E35" s="166"/>
-      <c r="F35" s="189"/>
+      <c r="B35" s="257"/>
+      <c r="C35" s="167"/>
+      <c r="D35" s="168"/>
+      <c r="E35" s="167"/>
+      <c r="F35" s="168"/>
       <c r="G35" s="128"/>
       <c r="H35" s="58"/>
       <c r="I35" s="5"/>
@@ -4368,10 +4367,10 @@
       </c>
       <c r="T35" s="121"/>
       <c r="U35" s="122"/>
-      <c r="V35" s="175">
+      <c r="V35" s="258">
         <v>6</v>
       </c>
-      <c r="W35" s="176"/>
+      <c r="W35" s="259"/>
       <c r="X35" s="123"/>
     </row>
     <row r="36" spans="1:28" s="3" customFormat="1" ht="21.75" customHeight="1">
@@ -4384,12 +4383,12 @@
       <c r="E36" s="102"/>
       <c r="F36" s="102"/>
       <c r="G36" s="103"/>
-      <c r="T36" s="190" t="s">
+      <c r="T36" s="235" t="s">
         <v>153</v>
       </c>
-      <c r="U36" s="190"/>
-      <c r="V36" s="190"/>
-      <c r="W36" s="190"/>
+      <c r="U36" s="235"/>
+      <c r="V36" s="235"/>
+      <c r="W36" s="235"/>
       <c r="X36" s="110" t="s">
         <v>132</v>
       </c>
@@ -4413,49 +4412,23 @@
     <row r="48" spans="1:28" s="3" customFormat="1" ht="17.399999999999999"/>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="A5:B7"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="C32:D33"/>
-    <mergeCell ref="E32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:M8"/>
-    <mergeCell ref="J6:M7"/>
-    <mergeCell ref="C9:E10"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C5:E7"/>
-    <mergeCell ref="F5:I7"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="T7:U7"/>
-    <mergeCell ref="J5:M5"/>
-    <mergeCell ref="N5:Q5"/>
-    <mergeCell ref="R6:R7"/>
-    <mergeCell ref="S6:S7"/>
-    <mergeCell ref="N6:Q7"/>
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="Z2:AU2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="N4:Q4"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="T4:X4"/>
-    <mergeCell ref="A2:R3"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="T8:U8"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="T9:U9"/>
-    <mergeCell ref="R8:S8"/>
-    <mergeCell ref="N8:Q8"/>
+    <mergeCell ref="V5:X5"/>
+    <mergeCell ref="V6:X6"/>
+    <mergeCell ref="V7:X7"/>
+    <mergeCell ref="V8:X8"/>
+    <mergeCell ref="V9:X9"/>
+    <mergeCell ref="V10:X10"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="V34:W34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="V35:W35"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="O31:X31"/>
+    <mergeCell ref="O32:R32"/>
+    <mergeCell ref="S32:X32"/>
+    <mergeCell ref="A32:B33"/>
+    <mergeCell ref="E35:F35"/>
     <mergeCell ref="T36:W36"/>
     <mergeCell ref="V33:W33"/>
     <mergeCell ref="T10:U10"/>
@@ -4472,23 +4445,49 @@
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="C35:D35"/>
-    <mergeCell ref="V10:X10"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="V34:W34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="V35:W35"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="O31:X31"/>
-    <mergeCell ref="O32:R32"/>
-    <mergeCell ref="S32:X32"/>
-    <mergeCell ref="A32:B33"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="V5:X5"/>
-    <mergeCell ref="V6:X6"/>
-    <mergeCell ref="V7:X7"/>
-    <mergeCell ref="V8:X8"/>
-    <mergeCell ref="V9:X9"/>
+    <mergeCell ref="T8:U8"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="T9:U9"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="N8:Q8"/>
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="Z2:AU2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="N4:Q4"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="T4:X4"/>
+    <mergeCell ref="A2:R3"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="T7:U7"/>
+    <mergeCell ref="J5:M5"/>
+    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="R6:R7"/>
+    <mergeCell ref="S6:S7"/>
+    <mergeCell ref="N6:Q7"/>
+    <mergeCell ref="A5:B7"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="C32:D33"/>
+    <mergeCell ref="E32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:M8"/>
+    <mergeCell ref="J6:M7"/>
+    <mergeCell ref="C9:E10"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C5:E7"/>
+    <mergeCell ref="F5:I7"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -4506,7 +4505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="O22" sqref="O22:P22"/>
     </sheetView>
   </sheetViews>
@@ -4571,74 +4570,74 @@
       <c r="R3" s="81"/>
     </row>
     <row r="4" spans="1:18" s="3" customFormat="1" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A4" s="213" t="s">
+      <c r="A4" s="217" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="288"/>
-      <c r="C4" s="291" t="s">
+      <c r="B4" s="278"/>
+      <c r="C4" s="279" t="s">
         <v>89</v>
       </c>
-      <c r="D4" s="288"/>
-      <c r="E4" s="291" t="s">
+      <c r="D4" s="278"/>
+      <c r="E4" s="279" t="s">
         <v>88</v>
       </c>
-      <c r="F4" s="288"/>
-      <c r="G4" s="214" t="s">
+      <c r="F4" s="278"/>
+      <c r="G4" s="218" t="s">
         <v>152</v>
       </c>
-      <c r="H4" s="214"/>
-      <c r="I4" s="215"/>
+      <c r="H4" s="218"/>
+      <c r="I4" s="219"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="298" t="s">
+      <c r="K4" s="280" t="s">
         <v>94</v>
       </c>
-      <c r="L4" s="299"/>
-      <c r="M4" s="299"/>
-      <c r="N4" s="299"/>
-      <c r="O4" s="299"/>
-      <c r="P4" s="299"/>
-      <c r="Q4" s="299"/>
-      <c r="R4" s="300"/>
+      <c r="L4" s="281"/>
+      <c r="M4" s="281"/>
+      <c r="N4" s="281"/>
+      <c r="O4" s="281"/>
+      <c r="P4" s="281"/>
+      <c r="Q4" s="281"/>
+      <c r="R4" s="282"/>
     </row>
     <row r="5" spans="1:18" ht="21.75" customHeight="1">
-      <c r="A5" s="301"/>
-      <c r="B5" s="230"/>
-      <c r="C5" s="229"/>
-      <c r="D5" s="230"/>
-      <c r="E5" s="229"/>
-      <c r="F5" s="230"/>
-      <c r="G5" s="229"/>
-      <c r="H5" s="190"/>
-      <c r="I5" s="303"/>
+      <c r="A5" s="271"/>
+      <c r="B5" s="203"/>
+      <c r="C5" s="202"/>
+      <c r="D5" s="203"/>
+      <c r="E5" s="202"/>
+      <c r="F5" s="203"/>
+      <c r="G5" s="202"/>
+      <c r="H5" s="235"/>
+      <c r="I5" s="275"/>
       <c r="J5" s="80"/>
-      <c r="K5" s="294" t="s">
+      <c r="K5" s="283" t="s">
         <v>170</v>
       </c>
-      <c r="L5" s="295"/>
-      <c r="M5" s="284"/>
+      <c r="L5" s="284"/>
+      <c r="M5" s="285"/>
       <c r="N5" s="10"/>
-      <c r="O5" s="274" t="s">
+      <c r="O5" s="293" t="s">
         <v>141</v>
       </c>
-      <c r="P5" s="284"/>
-      <c r="Q5" s="274"/>
-      <c r="R5" s="275"/>
+      <c r="P5" s="285"/>
+      <c r="Q5" s="293"/>
+      <c r="R5" s="304"/>
     </row>
     <row r="6" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A6" s="278"/>
-      <c r="B6" s="280"/>
-      <c r="C6" s="302"/>
-      <c r="D6" s="280"/>
-      <c r="E6" s="302"/>
-      <c r="F6" s="280"/>
-      <c r="G6" s="302"/>
-      <c r="H6" s="279"/>
-      <c r="I6" s="304"/>
+      <c r="A6" s="272"/>
+      <c r="B6" s="273"/>
+      <c r="C6" s="274"/>
+      <c r="D6" s="273"/>
+      <c r="E6" s="274"/>
+      <c r="F6" s="273"/>
+      <c r="G6" s="274"/>
+      <c r="H6" s="276"/>
+      <c r="I6" s="277"/>
       <c r="J6" s="80"/>
-      <c r="K6" s="248" t="s">
+      <c r="K6" s="174" t="s">
         <v>171</v>
       </c>
-      <c r="L6" s="206"/>
+      <c r="L6" s="175"/>
       <c r="M6" s="39" t="s">
         <v>3</v>
       </c>
@@ -4663,20 +4662,20 @@
       <c r="H7" s="80"/>
       <c r="I7" s="80"/>
       <c r="J7" s="80"/>
-      <c r="K7" s="296" t="s">
+      <c r="K7" s="286" t="s">
         <v>172</v>
       </c>
-      <c r="L7" s="297"/>
+      <c r="L7" s="287"/>
       <c r="M7" s="18" t="s">
         <v>3</v>
       </c>
       <c r="N7" s="9"/>
-      <c r="O7" s="255" t="s">
+      <c r="O7" s="185" t="s">
         <v>108</v>
       </c>
-      <c r="P7" s="203"/>
-      <c r="Q7" s="166"/>
-      <c r="R7" s="168"/>
+      <c r="P7" s="187"/>
+      <c r="Q7" s="167"/>
+      <c r="R7" s="253"/>
     </row>
     <row r="8" spans="1:18" s="3" customFormat="1" ht="21.75" customHeight="1" thickBot="1">
       <c r="A8" s="56" t="s">
@@ -4754,15 +4753,15 @@
         <v>124</v>
       </c>
       <c r="M9" s="36"/>
-      <c r="N9" s="274" t="s">
+      <c r="N9" s="293" t="s">
         <v>109</v>
       </c>
-      <c r="O9" s="284"/>
-      <c r="P9" s="256" t="s">
+      <c r="O9" s="285"/>
+      <c r="P9" s="188" t="s">
         <v>110</v>
       </c>
-      <c r="Q9" s="257"/>
-      <c r="R9" s="292"/>
+      <c r="Q9" s="189"/>
+      <c r="R9" s="308"/>
     </row>
     <row r="10" spans="1:18" ht="21.75" customHeight="1">
       <c r="A10" s="64" t="s">
@@ -4784,15 +4783,15 @@
         <v>125</v>
       </c>
       <c r="M10" s="10"/>
-      <c r="N10" s="163" t="s">
+      <c r="N10" s="176" t="s">
         <v>109</v>
       </c>
-      <c r="O10" s="206"/>
-      <c r="P10" s="245" t="s">
+      <c r="O10" s="175"/>
+      <c r="P10" s="169" t="s">
         <v>110</v>
       </c>
-      <c r="Q10" s="201"/>
-      <c r="R10" s="293"/>
+      <c r="Q10" s="184"/>
+      <c r="R10" s="309"/>
     </row>
     <row r="11" spans="1:18" ht="21.75" customHeight="1">
       <c r="A11" s="86"/>
@@ -4812,15 +4811,15 @@
         <v>126</v>
       </c>
       <c r="M11" s="10"/>
-      <c r="N11" s="163" t="s">
+      <c r="N11" s="176" t="s">
         <v>109</v>
       </c>
-      <c r="O11" s="206"/>
-      <c r="P11" s="163" t="s">
+      <c r="O11" s="175"/>
+      <c r="P11" s="176" t="s">
         <v>110</v>
       </c>
-      <c r="Q11" s="164"/>
-      <c r="R11" s="165"/>
+      <c r="Q11" s="177"/>
+      <c r="R11" s="270"/>
     </row>
     <row r="12" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
       <c r="A12" s="89"/>
@@ -4840,15 +4839,15 @@
         <v>127</v>
       </c>
       <c r="M12" s="9"/>
-      <c r="N12" s="255" t="s">
+      <c r="N12" s="185" t="s">
         <v>109</v>
       </c>
-      <c r="O12" s="203"/>
-      <c r="P12" s="163" t="s">
+      <c r="O12" s="187"/>
+      <c r="P12" s="176" t="s">
         <v>110</v>
       </c>
-      <c r="Q12" s="164"/>
-      <c r="R12" s="165"/>
+      <c r="Q12" s="177"/>
+      <c r="R12" s="270"/>
     </row>
     <row r="13" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
       <c r="A13" s="89"/>
@@ -4919,10 +4918,10 @@
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
       <c r="N15" s="10"/>
-      <c r="O15" s="305"/>
-      <c r="P15" s="305"/>
-      <c r="Q15" s="305"/>
-      <c r="R15" s="306"/>
+      <c r="O15" s="157"/>
+      <c r="P15" s="157"/>
+      <c r="Q15" s="157"/>
+      <c r="R15" s="158"/>
     </row>
     <row r="16" spans="1:18" ht="21.75" customHeight="1">
       <c r="A16" s="89"/>
@@ -4941,10 +4940,10 @@
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
       <c r="N16" s="10"/>
-      <c r="O16" s="305"/>
-      <c r="P16" s="305"/>
-      <c r="Q16" s="305"/>
-      <c r="R16" s="306"/>
+      <c r="O16" s="157"/>
+      <c r="P16" s="157"/>
+      <c r="Q16" s="157"/>
+      <c r="R16" s="158"/>
     </row>
     <row r="17" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
       <c r="A17" s="89"/>
@@ -4963,10 +4962,10 @@
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
       <c r="N17" s="9"/>
-      <c r="O17" s="307"/>
-      <c r="P17" s="307"/>
-      <c r="Q17" s="307"/>
-      <c r="R17" s="308"/>
+      <c r="O17" s="159"/>
+      <c r="P17" s="159"/>
+      <c r="Q17" s="159"/>
+      <c r="R17" s="160"/>
     </row>
     <row r="18" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
       <c r="A18" s="85"/>
@@ -4991,12 +4990,12 @@
       <c r="R18" s="69"/>
     </row>
     <row r="19" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A19" s="278" t="s">
+      <c r="A19" s="272" t="s">
         <v>85</v>
       </c>
-      <c r="B19" s="279"/>
-      <c r="C19" s="279"/>
-      <c r="D19" s="280"/>
+      <c r="B19" s="276"/>
+      <c r="C19" s="276"/>
+      <c r="D19" s="273"/>
       <c r="E19" s="70"/>
       <c r="F19" s="70"/>
       <c r="G19" s="70"/>
@@ -5009,14 +5008,14 @@
       <c r="L19" s="35"/>
       <c r="M19" s="35"/>
       <c r="N19" s="36"/>
-      <c r="O19" s="274" t="s">
+      <c r="O19" s="293" t="s">
         <v>118</v>
       </c>
-      <c r="P19" s="284"/>
-      <c r="Q19" s="289" t="s">
+      <c r="P19" s="285"/>
+      <c r="Q19" s="297" t="s">
         <v>119</v>
       </c>
-      <c r="R19" s="290"/>
+      <c r="R19" s="298"/>
     </row>
     <row r="20" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
       <c r="A20" s="79"/>
@@ -5035,29 +5034,29 @@
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
       <c r="N20" s="10"/>
-      <c r="O20" s="317"/>
-      <c r="P20" s="318"/>
-      <c r="Q20" s="317"/>
-      <c r="R20" s="319"/>
+      <c r="O20" s="305"/>
+      <c r="P20" s="306"/>
+      <c r="Q20" s="305"/>
+      <c r="R20" s="307"/>
     </row>
     <row r="21" spans="1:18" s="3" customFormat="1" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A21" s="213" t="s">
+      <c r="A21" s="217" t="s">
         <v>90</v>
       </c>
-      <c r="B21" s="288"/>
-      <c r="C21" s="291" t="s">
+      <c r="B21" s="278"/>
+      <c r="C21" s="279" t="s">
         <v>89</v>
       </c>
-      <c r="D21" s="288"/>
-      <c r="E21" s="291" t="s">
+      <c r="D21" s="278"/>
+      <c r="E21" s="279" t="s">
         <v>91</v>
       </c>
-      <c r="F21" s="288"/>
-      <c r="G21" s="214" t="s">
+      <c r="F21" s="278"/>
+      <c r="G21" s="218" t="s">
         <v>87</v>
       </c>
-      <c r="H21" s="214"/>
-      <c r="I21" s="215"/>
+      <c r="H21" s="218"/>
+      <c r="I21" s="219"/>
       <c r="J21" s="4"/>
       <c r="K21" s="54" t="s">
         <v>115</v>
@@ -5065,21 +5064,21 @@
       <c r="L21" s="8"/>
       <c r="M21" s="8"/>
       <c r="N21" s="10"/>
-      <c r="O21" s="317"/>
-      <c r="P21" s="318"/>
-      <c r="Q21" s="317"/>
-      <c r="R21" s="319"/>
+      <c r="O21" s="305"/>
+      <c r="P21" s="306"/>
+      <c r="Q21" s="305"/>
+      <c r="R21" s="307"/>
     </row>
     <row r="22" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A22" s="269"/>
-      <c r="B22" s="270"/>
-      <c r="C22" s="271"/>
-      <c r="D22" s="270"/>
-      <c r="E22" s="271"/>
-      <c r="F22" s="270"/>
-      <c r="G22" s="271"/>
-      <c r="H22" s="272"/>
-      <c r="I22" s="273"/>
+      <c r="A22" s="299"/>
+      <c r="B22" s="300"/>
+      <c r="C22" s="301"/>
+      <c r="D22" s="300"/>
+      <c r="E22" s="301"/>
+      <c r="F22" s="300"/>
+      <c r="G22" s="301"/>
+      <c r="H22" s="302"/>
+      <c r="I22" s="303"/>
       <c r="J22" s="80"/>
       <c r="K22" s="19" t="s">
         <v>116</v>
@@ -5089,8 +5088,8 @@
       <c r="N22" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="O22" s="207"/>
-      <c r="P22" s="208"/>
+      <c r="O22" s="206"/>
+      <c r="P22" s="207"/>
       <c r="Q22" s="71"/>
       <c r="R22" s="45" t="s">
         <v>131</v>
@@ -5115,10 +5114,10 @@
       <c r="N23" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="O23" s="166"/>
-      <c r="P23" s="189"/>
-      <c r="Q23" s="166"/>
-      <c r="R23" s="168"/>
+      <c r="O23" s="167"/>
+      <c r="P23" s="168"/>
+      <c r="Q23" s="167"/>
+      <c r="R23" s="253"/>
     </row>
     <row r="24" spans="1:18" s="3" customFormat="1" ht="21.75" customHeight="1" thickBot="1">
       <c r="A24" s="56" t="s">
@@ -5187,16 +5186,16 @@
         <v>34</v>
       </c>
       <c r="J25" s="4"/>
-      <c r="K25" s="281" t="s">
+      <c r="K25" s="290" t="s">
         <v>148</v>
       </c>
-      <c r="L25" s="282"/>
-      <c r="M25" s="282"/>
-      <c r="N25" s="282"/>
-      <c r="O25" s="282"/>
-      <c r="P25" s="282"/>
-      <c r="Q25" s="282"/>
-      <c r="R25" s="283"/>
+      <c r="L25" s="291"/>
+      <c r="M25" s="291"/>
+      <c r="N25" s="291"/>
+      <c r="O25" s="291"/>
+      <c r="P25" s="291"/>
+      <c r="Q25" s="291"/>
+      <c r="R25" s="292"/>
     </row>
     <row r="26" spans="1:18" ht="21.75" customHeight="1">
       <c r="A26" s="64" t="s">
@@ -5216,15 +5215,15 @@
       </c>
       <c r="L26" s="74"/>
       <c r="M26" s="75"/>
-      <c r="N26" s="177" t="s">
+      <c r="N26" s="240" t="s">
         <v>122</v>
       </c>
-      <c r="O26" s="193"/>
-      <c r="P26" s="178"/>
-      <c r="Q26" s="193" t="s">
+      <c r="O26" s="241"/>
+      <c r="P26" s="242"/>
+      <c r="Q26" s="241" t="s">
         <v>123</v>
       </c>
-      <c r="R26" s="285"/>
+      <c r="R26" s="294"/>
     </row>
     <row r="27" spans="1:18" ht="21.75" customHeight="1">
       <c r="A27" s="86"/>
@@ -5242,11 +5241,11 @@
       </c>
       <c r="L27" s="71"/>
       <c r="M27" s="72"/>
-      <c r="N27" s="309"/>
-      <c r="O27" s="310"/>
-      <c r="P27" s="311"/>
-      <c r="Q27" s="309"/>
-      <c r="R27" s="312"/>
+      <c r="N27" s="310"/>
+      <c r="O27" s="311"/>
+      <c r="P27" s="312"/>
+      <c r="Q27" s="310"/>
+      <c r="R27" s="316"/>
     </row>
     <row r="28" spans="1:18" ht="21.75" customHeight="1">
       <c r="A28" s="89"/>
@@ -5264,11 +5263,11 @@
       </c>
       <c r="L28" s="71"/>
       <c r="M28" s="72"/>
-      <c r="N28" s="309"/>
-      <c r="O28" s="310"/>
-      <c r="P28" s="311"/>
-      <c r="Q28" s="309"/>
-      <c r="R28" s="312"/>
+      <c r="N28" s="310"/>
+      <c r="O28" s="311"/>
+      <c r="P28" s="312"/>
+      <c r="Q28" s="310"/>
+      <c r="R28" s="316"/>
     </row>
     <row r="29" spans="1:18" ht="21.75" customHeight="1">
       <c r="A29" s="89"/>
@@ -5286,11 +5285,11 @@
       </c>
       <c r="L29" s="77"/>
       <c r="M29" s="78"/>
-      <c r="N29" s="309"/>
-      <c r="O29" s="310"/>
-      <c r="P29" s="311"/>
-      <c r="Q29" s="309"/>
-      <c r="R29" s="312"/>
+      <c r="N29" s="310"/>
+      <c r="O29" s="311"/>
+      <c r="P29" s="312"/>
+      <c r="Q29" s="310"/>
+      <c r="R29" s="316"/>
     </row>
     <row r="30" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
       <c r="A30" s="89"/>
@@ -5312,7 +5311,7 @@
       <c r="O30" s="314"/>
       <c r="P30" s="315"/>
       <c r="Q30" s="313"/>
-      <c r="R30" s="316"/>
+      <c r="R30" s="317"/>
     </row>
     <row r="31" spans="1:18" ht="21.75" customHeight="1">
       <c r="A31" s="89"/>
@@ -5349,12 +5348,12 @@
         <v>128</v>
       </c>
       <c r="L32" s="80"/>
-      <c r="M32" s="286"/>
-      <c r="N32" s="286"/>
-      <c r="O32" s="286"/>
-      <c r="P32" s="286"/>
-      <c r="Q32" s="286"/>
-      <c r="R32" s="287"/>
+      <c r="M32" s="295"/>
+      <c r="N32" s="295"/>
+      <c r="O32" s="295"/>
+      <c r="P32" s="295"/>
+      <c r="Q32" s="295"/>
+      <c r="R32" s="296"/>
     </row>
     <row r="33" spans="1:18" ht="21.75" customHeight="1">
       <c r="A33" s="89"/>
@@ -5401,12 +5400,12 @@
       <c r="R34" s="81"/>
     </row>
     <row r="35" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A35" s="278" t="s">
+      <c r="A35" s="272" t="s">
         <v>85</v>
       </c>
-      <c r="B35" s="279"/>
-      <c r="C35" s="279"/>
-      <c r="D35" s="280"/>
+      <c r="B35" s="276"/>
+      <c r="C35" s="276"/>
+      <c r="D35" s="273"/>
       <c r="E35" s="70"/>
       <c r="F35" s="70"/>
       <c r="G35" s="70"/>
@@ -5434,28 +5433,40 @@
       <c r="E36" s="102"/>
       <c r="F36" s="102"/>
       <c r="G36" s="103"/>
-      <c r="Q36" s="276" t="s">
+      <c r="Q36" s="288" t="s">
         <v>154</v>
       </c>
-      <c r="R36" s="277"/>
+      <c r="R36" s="289"/>
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="A5:B6"/>
-    <mergeCell ref="C5:D6"/>
-    <mergeCell ref="E5:F6"/>
-    <mergeCell ref="G5:I6"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="K4:R4"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="P11:R11"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="N27:P27"/>
+    <mergeCell ref="N28:P28"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="N30:P30"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="P9:R9"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="P10:R10"/>
     <mergeCell ref="Q36:R36"/>
     <mergeCell ref="A35:D35"/>
     <mergeCell ref="K25:R25"/>
@@ -5472,33 +5483,21 @@
     <mergeCell ref="Q19:R19"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="E21:F21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="Q20:R20"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="P9:R9"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="P10:R10"/>
-    <mergeCell ref="N29:P29"/>
-    <mergeCell ref="N30:P30"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="Q30:R30"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="N27:P27"/>
-    <mergeCell ref="N28:P28"/>
+    <mergeCell ref="K4:R4"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="P11:R11"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="A5:B6"/>
+    <mergeCell ref="C5:D6"/>
+    <mergeCell ref="E5:F6"/>
+    <mergeCell ref="G5:I6"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:I4"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>